<commit_message>
Couple of layout changes
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -12,7 +12,7 @@
     <sheet name="tblUnits" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$48</definedName>
     <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$44</definedName>
     <definedName name="tblIngredientTypes" localSheetId="1">tblIngredientTypes!$A$1:$C$6</definedName>
     <definedName name="tblUnits" localSheetId="2">tblUnits!$A$1:$C$4</definedName>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
   <si>
     <t>carrots</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>sweet potatoes</t>
+  </si>
+  <si>
+    <t>grated parmesan</t>
   </si>
 </sst>
 </file>
@@ -1089,10 +1092,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,7 +1156,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1175,7 +1179,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1198,7 +1202,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1221,7 +1225,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1244,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1313,7 +1317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1336,7 +1340,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1359,7 +1363,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1382,7 +1386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1405,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1428,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1497,7 +1501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1543,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1566,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1612,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1635,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1681,7 +1685,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1704,7 +1708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1750,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1773,7 +1777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1796,7 +1800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1980,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2164,7 +2168,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>62</v>
       </c>
@@ -2184,8 +2188,37 @@
         <v>0</v>
       </c>
     </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G46"/>
+  <autoFilter ref="A1:G48">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Grocery"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:G46">
     <sortCondition ref="A2:A46"/>
   </sortState>

</xml_diff>

<commit_message>
Utensil expansion left to second stage to make it clearer that it is working on the previous expansion.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -8,14 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
-    <sheet name="tblIngredientTypes" sheetId="2" r:id="rId2"/>
-    <sheet name="tblUnits" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$48</definedName>
     <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$44</definedName>
-    <definedName name="tblIngredientTypes" localSheetId="1">tblIngredientTypes!$A$1:$C$6</definedName>
-    <definedName name="tblUnits" localSheetId="2">tblUnits!$A$1:$C$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,29 +34,11 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="tblIngredientTypes" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\User\Documents\Shit\tblIngredientTypes.csv" semicolon="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-  <connection id="3" name="tblUnits" type="6" refreshedVersion="4" background="1" saveData="1">
-    <textPr codePage="850" sourceFile="C:\Users\User\Documents\Shit\tblUnits.csv" semicolon="1">
-      <textFields count="3">
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
   <si>
     <t>carrots</t>
   </si>
@@ -207,18 +185,6 @@
   </si>
   <si>
     <t>Water</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>ml</t>
-  </si>
-  <si>
-    <t>tsp</t>
-  </si>
-  <si>
-    <t>tbsp</t>
   </si>
   <si>
     <t>Calories</t>
@@ -795,14 +761,6 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tblIngredients" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tblIngredientTypes" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="tblUnits" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,11 +1050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,25 +1069,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1156,7 +1113,7 @@
         <v>3.7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1179,7 +1136,7 @@
         <v>2.7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1202,7 +1159,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1182,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1248,7 +1205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1273,7 +1230,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
         <v>45</v>
@@ -1317,7 +1274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1297,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1320,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1386,7 +1343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1432,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1501,7 +1458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1524,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1547,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1570,7 +1527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1616,7 +1573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1639,7 +1596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -1685,7 +1642,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1708,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>40</v>
       </c>
@@ -1731,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>3</v>
       </c>
@@ -1754,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -1777,7 +1734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1800,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -1846,7 +1803,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>4</v>
       </c>
@@ -1869,7 +1826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
@@ -1963,7 +1920,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B38" t="s">
         <v>45</v>
@@ -1984,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2030,7 +1987,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -2076,7 +2033,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2168,9 +2125,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
         <v>47</v>
@@ -2190,7 +2147,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
@@ -2212,133 +2169,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G48">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Grocery"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G48"/>
   <sortState ref="A2:G46">
     <sortCondition ref="A2:A46"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Processing in ingredients list.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>carrots</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>grated parmesan</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
 </sst>
 </file>
@@ -1050,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,6 +2171,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G48"/>
   <sortState ref="A2:G46">

</xml_diff>

<commit_message>
Draft of second menu
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,7 +10,7 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$65</definedName>
     <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$44</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
   <si>
     <t>carrots</t>
   </si>
@@ -91,12 +91,6 @@
     <t>peanuts</t>
   </si>
   <si>
-    <t>red chillis</t>
-  </si>
-  <si>
-    <t>green chillis</t>
-  </si>
-  <si>
     <t>chicken</t>
   </si>
   <si>
@@ -224,6 +218,66 @@
   </si>
   <si>
     <t>tomatoes</t>
+  </si>
+  <si>
+    <t>red pepper</t>
+  </si>
+  <si>
+    <t>green pepper</t>
+  </si>
+  <si>
+    <t>aubergine</t>
+  </si>
+  <si>
+    <t>courgette</t>
+  </si>
+  <si>
+    <t>sunflower seeds</t>
+  </si>
+  <si>
+    <t>cottage cheese</t>
+  </si>
+  <si>
+    <t>sour cream</t>
+  </si>
+  <si>
+    <t>bacon</t>
+  </si>
+  <si>
+    <t>chorizo sausage</t>
+  </si>
+  <si>
+    <t>red lentils</t>
+  </si>
+  <si>
+    <t>mushrooms</t>
+  </si>
+  <si>
+    <t>soy sauce</t>
+  </si>
+  <si>
+    <t>sherry</t>
+  </si>
+  <si>
+    <t>pearl barley</t>
+  </si>
+  <si>
+    <t>canned kidney beans</t>
+  </si>
+  <si>
+    <t>green chilli</t>
+  </si>
+  <si>
+    <t>red chilli</t>
+  </si>
+  <si>
+    <t>cumin seeds</t>
+  </si>
+  <si>
+    <t>miso</t>
+  </si>
+  <si>
+    <t>asafoetida</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1110,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,33 +1129,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>50</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>75</v>
@@ -1121,10 +1175,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C3">
         <v>136</v>
@@ -1144,10 +1198,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>90</v>
@@ -1167,10 +1221,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>77</v>
@@ -1190,10 +1244,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1213,10 +1267,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7">
         <v>26</v>
@@ -1236,10 +1290,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1262,7 +1316,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>16</v>
@@ -1285,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C10">
         <v>35</v>
@@ -1308,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C11">
         <v>7</v>
@@ -1331,7 +1385,7 @@
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>412</v>
@@ -1351,10 +1405,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>183</v>
@@ -1377,7 +1431,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1400,7 +1454,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1420,10 +1474,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16">
         <v>176</v>
@@ -1443,10 +1497,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17">
         <v>669</v>
@@ -1466,10 +1520,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>147</v>
@@ -1489,10 +1543,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1512,10 +1566,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1535,10 +1589,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -1558,10 +1612,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1581,10 +1635,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1604,10 +1658,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
         <v>41</v>
-      </c>
-      <c r="B24" t="s">
-        <v>43</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1630,7 +1684,7 @@
         <v>14</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>348</v>
@@ -1650,10 +1704,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C26">
         <v>0</v>
@@ -1673,10 +1727,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1699,7 +1753,7 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C28">
         <v>410</v>
@@ -1722,7 +1776,7 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C29">
         <v>46</v>
@@ -1745,7 +1799,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1765,10 +1819,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1788,10 +1842,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32">
         <v>62</v>
@@ -1814,7 +1868,7 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>899</v>
@@ -1837,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C34">
         <v>36</v>
@@ -1857,10 +1911,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>132</v>
@@ -1883,7 +1937,7 @@
         <v>16</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>564</v>
@@ -1903,10 +1957,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>265</v>
@@ -1926,10 +1980,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -1949,10 +2003,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C39">
         <v>26</v>
@@ -1975,7 +2029,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C40">
         <v>330</v>
@@ -1995,10 +2049,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41">
         <v>205</v>
@@ -2018,10 +2072,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42">
         <v>104</v>
@@ -2044,7 +2098,7 @@
         <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2067,7 +2121,7 @@
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44">
         <v>826</v>
@@ -2090,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45">
         <v>68</v>
@@ -2110,10 +2164,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46">
         <v>138</v>
@@ -2133,10 +2187,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2153,10 +2207,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2176,10 +2230,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2199,29 +2253,443 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>59</v>
+      </c>
+      <c r="B50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51" t="s">
+        <v>45</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>61</v>
       </c>
-      <c r="B50" t="s">
-        <v>47</v>
-      </c>
-      <c r="C50">
-        <v>0</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
-      <c r="F50">
-        <v>0</v>
-      </c>
-      <c r="G50">
+      <c r="B52" t="s">
+        <v>45</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>62</v>
+      </c>
+      <c r="B53" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>63</v>
+      </c>
+      <c r="B54" t="s">
+        <v>45</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B55" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>65</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>66</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>67</v>
+      </c>
+      <c r="B58" t="s">
+        <v>44</v>
+      </c>
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>70</v>
+      </c>
+      <c r="B61" t="s">
+        <v>45</v>
+      </c>
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" t="s">
+        <v>41</v>
+      </c>
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>72</v>
+      </c>
+      <c r="B63" t="s">
+        <v>41</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>73</v>
+      </c>
+      <c r="B64" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66" t="s">
+        <v>41</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" t="s">
+        <v>41</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G48"/>
+  <autoFilter ref="A1:G65"/>
   <sortState ref="A2:G46">
     <sortCondition ref="A2:A46"/>
   </sortState>

</xml_diff>

<commit_message>
Menu B, not sure about the Indian Tomatoes
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,7 +10,7 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$68</definedName>
     <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$44</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
   <si>
     <t>carrots</t>
   </si>
@@ -278,6 +278,24 @@
   </si>
   <si>
     <t>asafoetida</t>
+  </si>
+  <si>
+    <t>wine vinegar</t>
+  </si>
+  <si>
+    <t>salt</t>
+  </si>
+  <si>
+    <t>pepper</t>
+  </si>
+  <si>
+    <t>basil</t>
+  </si>
+  <si>
+    <t>oregano</t>
+  </si>
+  <si>
+    <t>sugar</t>
   </si>
 </sst>
 </file>
@@ -1110,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G68"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74:G74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,206 +1170,206 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>13.6</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
       </c>
       <c r="C3">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>31.7</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>2.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C4">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5">
-        <v>2.2000000000000002</v>
+        <v>4.7</v>
       </c>
       <c r="E5">
-        <v>18</v>
+        <v>13.6</v>
       </c>
       <c r="F5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="G5">
-        <v>1.4</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>136</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>3.9</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>31.7</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C7">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="D7">
-        <v>1.7</v>
+        <v>0.3</v>
       </c>
       <c r="E7">
-        <v>4.0999999999999996</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F7">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="G7">
-        <v>2.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C9">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>45</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D10">
-        <v>0.6</v>
+        <v>1.7</v>
       </c>
       <c r="E10">
-        <v>7.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F10">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="G10">
         <v>2.4</v>
@@ -1359,45 +1377,45 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C12">
-        <v>412</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>34.4</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -1405,114 +1423,114 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13">
-        <v>183</v>
+        <v>16</v>
       </c>
       <c r="D13">
-        <v>29.2</v>
+        <v>0.8</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13">
-        <v>7.3</v>
+        <v>0.4</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16">
-        <v>176</v>
+        <v>412</v>
       </c>
       <c r="D16">
-        <v>6</v>
+        <v>25.5</v>
       </c>
       <c r="E16">
-        <v>35.6</v>
+        <v>0.1</v>
       </c>
       <c r="F16">
-        <v>0.3</v>
+        <v>34.4</v>
       </c>
       <c r="G16">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17">
-        <v>669</v>
+        <v>183</v>
       </c>
       <c r="D17">
-        <v>6</v>
+        <v>29.2</v>
       </c>
       <c r="E17">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>68.8</v>
+        <v>7.3</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1520,22 +1538,22 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
       <c r="F18">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1543,10 +1561,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1566,10 +1584,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1589,22 +1607,22 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -1612,10 +1630,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>37</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1635,45 +1653,45 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G24">
         <v>0</v>
@@ -1681,45 +1699,45 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1727,7 +1745,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
         <v>41</v>
@@ -1750,22 +1768,22 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C28">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G28">
         <v>0</v>
@@ -1773,22 +1791,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C29">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1796,22 +1814,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1819,10 +1837,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>0</v>
@@ -1842,42 +1860,42 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C32">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
       </c>
       <c r="C33">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -1888,114 +1906,114 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C34">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E34">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F34">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G34">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
         <v>43</v>
       </c>
       <c r="C35">
-        <v>132</v>
+        <v>348</v>
       </c>
       <c r="D35">
-        <v>5.2</v>
+        <v>13</v>
       </c>
       <c r="E35">
-        <v>24.4</v>
+        <v>70</v>
       </c>
       <c r="F35">
-        <v>1.5</v>
+        <v>1.8</v>
       </c>
       <c r="G35">
-        <v>1.3</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C36">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>25.6</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F36">
-        <v>46.1</v>
+        <v>0</v>
       </c>
       <c r="G36">
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>37.1</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2003,22 +2021,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>76</v>
+        <v>5</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C39">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="D39">
-        <v>1.8</v>
+        <v>3.3</v>
       </c>
       <c r="E39">
-        <v>4.2</v>
+        <v>5</v>
       </c>
       <c r="F39">
-        <v>0.3</v>
+        <v>1.6</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -2026,45 +2044,45 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E40">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F40">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G40">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2072,30 +2090,30 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
@@ -2118,122 +2136,125 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
         <v>43</v>
       </c>
       <c r="C44">
-        <v>826</v>
+        <v>62</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E44">
-        <v>12.1</v>
+        <v>13</v>
       </c>
       <c r="F44">
-        <v>86.7</v>
+        <v>0.5</v>
       </c>
       <c r="G44">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C45">
-        <v>68</v>
+        <v>899</v>
       </c>
       <c r="D45">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>12.9</v>
+        <v>99.9</v>
       </c>
       <c r="F45">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C46">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="D46">
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
       <c r="E46">
-        <v>30.9</v>
+        <v>7.9</v>
       </c>
       <c r="F46">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="G46">
-        <v>0.1</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="G47">
+        <v>1.3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>16</v>
       </c>
       <c r="B48" t="s">
         <v>43</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2253,33 +2274,33 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2299,22 +2320,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B52" t="s">
         <v>45</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G52">
         <v>0</v>
@@ -2322,10 +2343,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2345,7 +2366,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>45</v>
@@ -2368,33 +2389,33 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>64</v>
+        <v>10</v>
       </c>
       <c r="B55" t="s">
         <v>43</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2437,22 +2458,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="B58" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2460,10 +2481,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2483,33 +2504,33 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
         <v>43</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2529,33 +2550,33 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>71</v>
+        <v>11</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D62">
         <v>0</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2575,10 +2596,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2590,41 +2611,38 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>74</v>
+        <v>6</v>
       </c>
       <c r="B65" t="s">
         <v>43</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2644,10 +2662,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2667,31 +2685,168 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="B68" t="s">
+        <v>43</v>
+      </c>
+      <c r="C68">
+        <v>138</v>
+      </c>
+      <c r="D68">
+        <v>2.6</v>
+      </c>
+      <c r="E68">
+        <v>30.9</v>
+      </c>
+      <c r="F68">
+        <v>1.3</v>
+      </c>
+      <c r="G68">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>80</v>
+      </c>
+      <c r="B69" t="s">
         <v>41</v>
       </c>
-      <c r="C68">
-        <v>0</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B70" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>82</v>
+      </c>
+      <c r="B71" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>83</v>
+      </c>
+      <c r="B72" t="s">
+        <v>41</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>84</v>
+      </c>
+      <c r="B73" t="s">
+        <v>41</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G65"/>
-  <sortState ref="A2:G46">
-    <sortCondition ref="A2:A46"/>
+  <sortState ref="A2:G68">
+    <sortCondition ref="A2:A68"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Better layout for the table of contents.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="87">
   <si>
     <t>carrots</t>
   </si>
@@ -296,6 +296,9 @@
   </si>
   <si>
     <t>sugar</t>
+  </si>
+  <si>
+    <t>pizza</t>
   </si>
 </sst>
 </file>
@@ -1128,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74:G74"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,21 +2829,44 @@
         <v>85</v>
       </c>
       <c r="B74" t="s">
+        <v>41</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>86</v>
+      </c>
+      <c r="B75" t="s">
         <v>43</v>
       </c>
-      <c r="C74">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted the chick pea risotto.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="93">
   <si>
     <t>carrots</t>
   </si>
@@ -1149,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81:G81"/>
+      <selection activeCell="B82" sqref="B82:G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,6 +3026,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>72</v>
+      </c>
+      <c r="B82" t="s">
+        <v>43</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G77">
     <sortCondition ref="A2:A77"/>

</xml_diff>

<commit_message>
Updates to egg curry.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
   <si>
     <t>carrots</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>parmesan</t>
+  </si>
+  <si>
+    <t>curry powder</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G83"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3075,6 +3078,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" t="s">
+        <v>41</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G77">
     <sortCondition ref="A2:A77"/>

</xml_diff>

<commit_message>
Third menu of the new era.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="120">
   <si>
     <t>carrots</t>
   </si>
@@ -323,6 +323,81 @@
   </si>
   <si>
     <t>curry powder</t>
+  </si>
+  <si>
+    <t>oven ready chips</t>
+  </si>
+  <si>
+    <t>cinnamon stick</t>
+  </si>
+  <si>
+    <t>pasta sauce</t>
+  </si>
+  <si>
+    <t>minced meat</t>
+  </si>
+  <si>
+    <t>cashew nuts</t>
+  </si>
+  <si>
+    <t>lemon</t>
+  </si>
+  <si>
+    <t>mustard seeds</t>
+  </si>
+  <si>
+    <t>capers</t>
+  </si>
+  <si>
+    <t>burgers</t>
+  </si>
+  <si>
+    <t>butter</t>
+  </si>
+  <si>
+    <t>pitted olives</t>
+  </si>
+  <si>
+    <t>anchovy fillets</t>
+  </si>
+  <si>
+    <t>canned tuna fish</t>
+  </si>
+  <si>
+    <t>pesto</t>
+  </si>
+  <si>
+    <t>horseraddish sauce</t>
+  </si>
+  <si>
+    <t>mayonaise</t>
+  </si>
+  <si>
+    <t>canned borlotti beans</t>
+  </si>
+  <si>
+    <t>parsnips</t>
+  </si>
+  <si>
+    <t>swedes</t>
+  </si>
+  <si>
+    <t>cloves</t>
+  </si>
+  <si>
+    <t>flaked almonds</t>
+  </si>
+  <si>
+    <t>sausages</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>cider</t>
+  </si>
+  <si>
+    <t>pizza bases</t>
   </si>
 </sst>
 </file>
@@ -1155,10 +1230,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C109" sqref="C109:G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1404,33 +1480,33 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1450,30 +1526,30 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
@@ -1496,91 +1572,91 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
         <v>43</v>
       </c>
       <c r="C15">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E16">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F16">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G16">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E17">
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="F17">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="G17">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C18">
-        <v>412</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="E18">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>34.4</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1588,33 +1664,33 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C19">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="D19">
-        <v>29.2</v>
+        <v>0.6</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F19">
-        <v>7.3</v>
+        <v>0.3</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1634,45 +1710,45 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1680,22 +1756,22 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -1703,10 +1779,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1726,45 +1802,45 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C25">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>35.6</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>68.8</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1772,10 +1848,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>9</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1795,10 +1871,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1818,22 +1894,22 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C29">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E29">
         <v>0</v>
       </c>
       <c r="F29">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -1841,45 +1917,45 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1887,10 +1963,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>0</v>
@@ -1910,22 +1986,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B33" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F33">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -1933,10 +2009,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>94</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1956,10 +2032,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -1979,22 +2055,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2002,7 +2078,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
         <v>41</v>
@@ -2025,33 +2101,33 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C38">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="B39" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2071,10 +2147,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>92</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2094,22 +2170,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41">
-        <v>410</v>
+        <v>20</v>
       </c>
       <c r="D41">
-        <v>19.100000000000001</v>
+        <v>2.9</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F41">
-        <v>37.1</v>
+        <v>0.6</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2117,22 +2193,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C42">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2140,10 +2216,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2163,7 +2239,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="B44" t="s">
         <v>41</v>
@@ -2186,10 +2262,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="B45" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2209,65 +2285,65 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C47">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C48">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -2278,45 +2354,45 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C49">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G49">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>84</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>37.1</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2324,56 +2400,56 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51">
-        <v>132</v>
+        <v>46</v>
       </c>
       <c r="D51">
-        <v>5.2</v>
+        <v>3.3</v>
       </c>
       <c r="E51">
-        <v>24.4</v>
+        <v>5</v>
       </c>
       <c r="F51">
-        <v>1.5</v>
+        <v>1.6</v>
       </c>
       <c r="G51">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C52">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>25.6</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>46.1</v>
+        <v>0</v>
       </c>
       <c r="G52">
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2393,7 +2469,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="B54" t="s">
         <v>41</v>
@@ -2416,33 +2492,33 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C55">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>86</v>
+        <v>33</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2462,10 +2538,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>101</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2485,22 +2561,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C58">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -2508,42 +2584,42 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="B59" t="s">
         <v>43</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2554,56 +2630,56 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C62">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2623,7 +2699,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="B64" t="s">
         <v>42</v>
@@ -2646,22 +2722,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>23</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C65">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2669,56 +2745,56 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B67" t="s">
         <v>43</v>
       </c>
       <c r="C67">
-        <v>104</v>
+        <v>564</v>
       </c>
       <c r="D67">
-        <v>3.6</v>
+        <v>25.6</v>
       </c>
       <c r="E67">
-        <v>22.2</v>
+        <v>12.5</v>
       </c>
       <c r="F67">
-        <v>7</v>
+        <v>46.1</v>
       </c>
       <c r="G67">
-        <v>1.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2738,53 +2814,53 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C69">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D69">
         <v>0</v>
       </c>
       <c r="E69">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G69">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>22</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
         <v>43</v>
@@ -2807,10 +2883,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2822,50 +2898,53 @@
         <v>0</v>
       </c>
       <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="B73" t="s">
         <v>43</v>
       </c>
       <c r="C73">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G73">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
         <v>45</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2873,10 +2952,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B75" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2896,30 +2975,30 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C76">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G76">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B77" t="s">
         <v>41</v>
@@ -2942,33 +3021,33 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="B79" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2988,7 +3067,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="B80" t="s">
         <v>43</v>
@@ -3011,10 +3090,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3034,22 +3113,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3057,10 +3136,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3080,30 +3159,671 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>94</v>
+        <v>31</v>
       </c>
       <c r="B84" t="s">
+        <v>43</v>
+      </c>
+      <c r="C84">
+        <v>104</v>
+      </c>
+      <c r="D84">
+        <v>3.6</v>
+      </c>
+      <c r="E84">
+        <v>22.2</v>
+      </c>
+      <c r="F84">
+        <v>7</v>
+      </c>
+      <c r="G84">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>8</v>
+      </c>
+      <c r="B85" t="s">
         <v>41</v>
       </c>
-      <c r="C84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>0</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84">
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>11</v>
+      </c>
+      <c r="B86" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86">
+        <v>826</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>12.1</v>
+      </c>
+      <c r="F86">
+        <v>86.7</v>
+      </c>
+      <c r="G86">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>41</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>64</v>
+      </c>
+      <c r="B88" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>56</v>
+      </c>
+      <c r="B89" t="s">
+        <v>45</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
+        <v>43</v>
+      </c>
+      <c r="C90">
+        <v>68</v>
+      </c>
+      <c r="D90">
+        <v>4.5</v>
+      </c>
+      <c r="E90">
+        <v>12.9</v>
+      </c>
+      <c r="F90">
+        <v>0.2</v>
+      </c>
+      <c r="G90">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>59</v>
+      </c>
+      <c r="B91" t="s">
+        <v>45</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>58</v>
+      </c>
+      <c r="B93" t="s">
+        <v>46</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B94" t="s">
+        <v>43</v>
+      </c>
+      <c r="C94">
+        <v>138</v>
+      </c>
+      <c r="D94">
+        <v>2.6</v>
+      </c>
+      <c r="E94">
+        <v>30.9</v>
+      </c>
+      <c r="F94">
+        <v>1.3</v>
+      </c>
+      <c r="G94">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>80</v>
+      </c>
+      <c r="B95" t="s">
+        <v>41</v>
+      </c>
+      <c r="C95">
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>105</v>
+      </c>
+      <c r="B96" t="s">
+        <v>43</v>
+      </c>
+      <c r="C96">
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>106</v>
+      </c>
+      <c r="B97" t="s">
+        <v>43</v>
+      </c>
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>107</v>
+      </c>
+      <c r="B98" t="s">
+        <v>43</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>108</v>
+      </c>
+      <c r="B99" t="s">
+        <v>43</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>109</v>
+      </c>
+      <c r="B100" t="s">
+        <v>43</v>
+      </c>
+      <c r="C100">
+        <v>12</v>
+      </c>
+      <c r="D100">
+        <v>2.8</v>
+      </c>
+      <c r="E100">
+        <v>1.4</v>
+      </c>
+      <c r="F100">
+        <v>11.8</v>
+      </c>
+      <c r="G100">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>64</v>
+      </c>
+      <c r="B101" t="s">
+        <v>41</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>110</v>
+      </c>
+      <c r="B102" t="s">
+        <v>43</v>
+      </c>
+      <c r="C102">
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>111</v>
+      </c>
+      <c r="B103" t="s">
+        <v>43</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>112</v>
+      </c>
+      <c r="B104" t="s">
+        <v>45</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" t="s">
+        <v>45</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>96</v>
+      </c>
+      <c r="B106" t="s">
+        <v>41</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+      <c r="F106">
+        <v>0</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>114</v>
+      </c>
+      <c r="B107" t="s">
+        <v>41</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>115</v>
+      </c>
+      <c r="B108" t="s">
+        <v>43</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109" t="s">
+        <v>44</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>117</v>
+      </c>
+      <c r="B110" t="s">
+        <v>45</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
+        <v>0</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" t="s">
+        <v>43</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111">
+        <v>0</v>
+      </c>
+      <c r="F111">
+        <v>0</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>119</v>
+      </c>
+      <c r="B112" t="s">
+        <v>43</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>0</v>
+      </c>
+      <c r="F112">
+        <v>0</v>
+      </c>
+      <c r="G112">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G77">
-    <sortCondition ref="A2:A77"/>
+  <sortState ref="A2:G96">
+    <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Easier to use ground cinnamon
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="121">
   <si>
     <t>carrots</t>
   </si>
@@ -398,6 +398,9 @@
   </si>
   <si>
     <t>pizza bases</t>
+  </si>
+  <si>
+    <t>ground cinnamon</t>
   </si>
 </sst>
 </file>
@@ -1230,11 +1233,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G112"/>
+  <dimension ref="A1:G113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C109" sqref="C109:G112"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,10 +1276,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1296,7 +1299,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B3" t="s">
         <v>45</v>
@@ -1319,10 +1322,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1342,171 +1345,171 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>13.6</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6">
-        <v>136</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>3.9</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>31.7</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>2.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>13.6</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C8">
-        <v>90</v>
+        <v>136</v>
       </c>
       <c r="D8">
-        <v>0.3</v>
+        <v>3.9</v>
       </c>
       <c r="E8">
-        <v>19.899999999999999</v>
+        <v>31.7</v>
       </c>
       <c r="F8">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="G8">
-        <v>1.2</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C9">
-        <v>77</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>104</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -1526,33 +1529,33 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>103</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>104</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1572,30 +1575,30 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>74</v>
+        <v>111</v>
       </c>
       <c r="B16" t="s">
         <v>43</v>
@@ -1618,30 +1621,30 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -1664,91 +1667,91 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E19">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F19">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G19">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>412</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>34.4</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1756,33 +1759,33 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C23">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="D23">
-        <v>29.2</v>
+        <v>0.6</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F23">
-        <v>7.3</v>
+        <v>0.3</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1802,45 +1805,45 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1848,22 +1851,22 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1871,10 +1874,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1894,10 +1897,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29">
         <v>0</v>
@@ -1917,45 +1920,45 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>118</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
       <c r="C30">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>35.6</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G30">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B31" t="s">
         <v>43</v>
       </c>
       <c r="C31">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>68.8</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1963,7 +1966,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
@@ -1986,7 +1989,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
         <v>41</v>
@@ -2009,10 +2012,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2032,10 +2035,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2055,22 +2058,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C36">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E36">
         <v>0</v>
       </c>
       <c r="F36">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -2078,45 +2081,45 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2124,10 +2127,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2147,10 +2150,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2170,22 +2173,22 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C41">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -2193,10 +2196,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2216,22 +2219,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2239,10 +2242,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>115</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2262,7 +2265,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
@@ -2285,33 +2288,33 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C46">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>57</v>
       </c>
       <c r="B47" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2331,7 +2334,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
         <v>45</v>
@@ -2354,22 +2357,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2377,22 +2380,22 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C50">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E50">
         <v>0</v>
       </c>
       <c r="F50">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G50">
         <v>0</v>
@@ -2400,22 +2403,22 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C51">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G51">
         <v>0</v>
@@ -2423,10 +2426,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2446,7 +2449,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B53" t="s">
         <v>41</v>
@@ -2469,7 +2472,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B54" t="s">
         <v>41</v>
@@ -2492,56 +2495,56 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>109</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B56" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2561,10 +2564,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2584,42 +2587,42 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C59">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G59">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>4</v>
+        <v>110</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C60">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D60">
         <v>0</v>
       </c>
       <c r="E60">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2630,45 +2633,45 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C61">
-        <v>36</v>
+        <v>410</v>
       </c>
       <c r="D61">
-        <v>1.2</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E61">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>0.2</v>
+        <v>37.1</v>
       </c>
       <c r="G61">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2676,10 +2679,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2699,10 +2702,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="B64" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2722,10 +2725,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>97</v>
+        <v>12</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2745,56 +2748,56 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C66">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G66">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C67">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>25.6</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>46.1</v>
+        <v>0</v>
       </c>
       <c r="G67">
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="B68" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2814,10 +2817,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2837,42 +2840,42 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B70" t="s">
         <v>43</v>
       </c>
       <c r="C70">
-        <v>265</v>
+        <v>62</v>
       </c>
       <c r="D70">
-        <v>9.1999999999999993</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E70">
-        <v>57.9</v>
+        <v>13</v>
       </c>
       <c r="F70">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="G70">
-        <v>2.2000000000000002</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2883,33 +2886,33 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2929,22 +2932,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B74" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C74">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G74">
         <v>0</v>
@@ -2952,10 +2955,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2975,7 +2978,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
       <c r="B76" t="s">
         <v>45</v>
@@ -2998,10 +3001,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3021,53 +3024,53 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="B78" t="s">
         <v>43</v>
       </c>
       <c r="C78">
-        <v>330</v>
+        <v>132</v>
       </c>
       <c r="D78">
-        <v>8.9</v>
+        <v>5.2</v>
       </c>
       <c r="E78">
-        <v>75.599999999999994</v>
+        <v>24.4</v>
       </c>
       <c r="F78">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="G78">
-        <v>3.1</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B80" t="s">
         <v>43</v>
@@ -3090,10 +3093,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3113,22 +3116,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>23</v>
+        <v>108</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C82">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3136,56 +3139,56 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B83" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>105</v>
       </c>
       <c r="B84" t="s">
         <v>43</v>
       </c>
       <c r="C84">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G84">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>8</v>
+        <v>86</v>
       </c>
       <c r="B85" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3205,33 +3208,33 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>119</v>
       </c>
       <c r="B86" t="s">
         <v>43</v>
       </c>
       <c r="C86">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3251,7 +3254,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B88" t="s">
         <v>43</v>
@@ -3274,50 +3277,53 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="B89" t="s">
         <v>45</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F89">
+        <v>0.3</v>
+      </c>
+      <c r="G89">
         <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="B90" t="s">
         <v>43</v>
       </c>
       <c r="C90">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B91" t="s">
         <v>45</v>
@@ -3340,7 +3346,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B92" t="s">
         <v>41</v>
@@ -3363,10 +3369,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="B93" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3386,30 +3392,30 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B94" t="s">
         <v>43</v>
       </c>
       <c r="C94">
-        <v>138</v>
+        <v>330</v>
       </c>
       <c r="D94">
-        <v>2.6</v>
+        <v>8.9</v>
       </c>
       <c r="E94">
-        <v>30.9</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F94">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="G94">
-        <v>0.1</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B95" t="s">
         <v>41</v>
@@ -3432,7 +3438,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="B96" t="s">
         <v>43</v>
@@ -3455,10 +3461,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3478,22 +3484,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>107</v>
+        <v>23</v>
       </c>
       <c r="B98" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3501,10 +3507,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3524,30 +3530,30 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>109</v>
+        <v>31</v>
       </c>
       <c r="B100" t="s">
         <v>43</v>
       </c>
       <c r="C100">
-        <v>12</v>
+        <v>104</v>
       </c>
       <c r="D100">
-        <v>2.8</v>
+        <v>3.6</v>
       </c>
       <c r="E100">
-        <v>1.4</v>
+        <v>22.2</v>
       </c>
       <c r="F100">
-        <v>11.8</v>
+        <v>7</v>
       </c>
       <c r="G100">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -3570,33 +3576,33 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="B102" t="s">
         <v>43</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G102">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3616,10 +3622,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="B104" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3639,10 +3645,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="B105" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3662,10 +3668,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3685,10 +3691,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>114</v>
+        <v>56</v>
       </c>
       <c r="B107" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3700,41 +3706,38 @@
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
-      </c>
-      <c r="G107">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="B108" t="s">
         <v>43</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G108">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>116</v>
+        <v>59</v>
       </c>
       <c r="B109" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3754,10 +3757,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>117</v>
+        <v>89</v>
       </c>
       <c r="B110" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3777,10 +3780,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>118</v>
+        <v>58</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -3800,30 +3803,53 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>119</v>
+        <v>28</v>
       </c>
       <c r="B112" t="s">
         <v>43</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>30.9</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="G112">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>80</v>
+      </c>
+      <c r="B113" t="s">
+        <v>41</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G96">
-    <sortCondition ref="A2:A96"/>
+  <sortState ref="A2:G113">
+    <sortCondition ref="A2:A113"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
New menu for next week.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,8 +10,8 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$68</definedName>
-    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$73</definedName>
+    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$49</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="131">
   <si>
     <t>carrots</t>
   </si>
@@ -401,6 +401,36 @@
   </si>
   <si>
     <t>ground cinnamon</t>
+  </si>
+  <si>
+    <t>potatoes</t>
+  </si>
+  <si>
+    <t>bay leaf</t>
+  </si>
+  <si>
+    <t>olive oil</t>
+  </si>
+  <si>
+    <t>olives</t>
+  </si>
+  <si>
+    <t>canned evapourated milk</t>
+  </si>
+  <si>
+    <t>cinnamon</t>
+  </si>
+  <si>
+    <t>pineapple chunks</t>
+  </si>
+  <si>
+    <t>canned sweetcorn</t>
+  </si>
+  <si>
+    <t>canned baked beans</t>
+  </si>
+  <si>
+    <t>fish fingers</t>
   </si>
 </sst>
 </file>
@@ -1233,16 +1263,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G113"/>
+  <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48:G48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -1460,79 +1490,79 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="F10">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G10">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C11">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="D11">
-        <v>2.2000000000000002</v>
+        <v>0.3</v>
       </c>
       <c r="E11">
-        <v>18</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>1.3</v>
       </c>
       <c r="G11">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1552,10 +1582,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1575,53 +1605,53 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>104</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="E15">
-        <v>4.0999999999999996</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
@@ -1644,7 +1674,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -1667,7 +1697,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -1690,30 +1720,30 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F20">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1736,7 +1766,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -1759,91 +1789,91 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G23">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>107</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C25">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E25">
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="F25">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G25">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C26">
-        <v>412</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="E26">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F26">
-        <v>34.4</v>
+        <v>0</v>
       </c>
       <c r="G26">
         <v>0</v>
@@ -1851,33 +1881,33 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C27">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="D27">
-        <v>29.2</v>
+        <v>0.6</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F27">
-        <v>7.3</v>
+        <v>0.3</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1897,45 +1927,45 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1943,22 +1973,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -1966,7 +1996,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="B32" t="s">
         <v>41</v>
@@ -1989,10 +2019,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -2012,10 +2042,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>118</v>
       </c>
       <c r="B34" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2035,10 +2065,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2058,10 +2088,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B36" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2081,45 +2111,45 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>114</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E37">
-        <v>35.6</v>
+        <v>0</v>
       </c>
       <c r="F37">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C38">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>68.8</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -2127,10 +2157,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2150,10 +2180,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2173,45 +2203,45 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2219,22 +2249,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C43">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E43">
         <v>0</v>
       </c>
       <c r="F43">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>0</v>
@@ -2242,10 +2272,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>115</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2265,7 +2295,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
@@ -2288,10 +2318,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2311,22 +2341,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>57</v>
+        <v>21</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2334,10 +2364,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2357,22 +2387,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C49">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2380,10 +2410,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2403,7 +2433,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
@@ -2426,7 +2456,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>57</v>
       </c>
       <c r="B52" t="s">
         <v>43</v>
@@ -2449,10 +2479,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2472,22 +2502,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2495,56 +2525,56 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>37</v>
       </c>
       <c r="B55" t="s">
         <v>43</v>
       </c>
       <c r="C55">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="G55">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C56">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G56">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2564,10 +2594,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2587,7 +2617,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B59" t="s">
         <v>41</v>
@@ -2610,68 +2640,68 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B60" t="s">
         <v>43</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C61">
-        <v>410</v>
+        <v>348</v>
       </c>
       <c r="D61">
-        <v>19.100000000000001</v>
+        <v>13</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F61">
-        <v>37.1</v>
+        <v>1.8</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C62">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G62">
         <v>0</v>
@@ -2679,10 +2709,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B63" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2702,7 +2732,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>78</v>
+        <v>38</v>
       </c>
       <c r="B64" t="s">
         <v>41</v>
@@ -2725,10 +2755,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="B65" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2748,22 +2778,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>37.1</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2771,22 +2801,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="B67" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -2794,10 +2824,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B68" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2817,10 +2847,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2840,42 +2870,42 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C70">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F70">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G70">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C71">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="E71">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -2886,30 +2916,30 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="B72" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C72">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="B73" t="s">
         <v>41</v>
@@ -2932,7 +2962,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B74" t="s">
         <v>43</v>
@@ -2955,42 +2985,42 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="B75" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>112</v>
+        <v>4</v>
       </c>
       <c r="B76" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3001,7 +3031,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>124</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
@@ -3024,56 +3054,56 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C78">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E78">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G78">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C79">
-        <v>564</v>
+        <v>36</v>
       </c>
       <c r="D79">
-        <v>25.6</v>
+        <v>1.2</v>
       </c>
       <c r="E79">
-        <v>12.5</v>
+        <v>7.9</v>
       </c>
       <c r="F79">
-        <v>46.1</v>
+        <v>0.2</v>
       </c>
       <c r="G79">
-        <v>6.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3093,10 +3123,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -3116,10 +3146,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -3139,30 +3169,30 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>22</v>
+        <v>112</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C83">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G83">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B84" t="s">
         <v>43</v>
@@ -3185,56 +3215,56 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="B85" t="s">
         <v>43</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>119</v>
+        <v>16</v>
       </c>
       <c r="B86" t="s">
         <v>43</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B87" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3254,10 +3284,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3277,22 +3307,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>76</v>
+        <v>108</v>
       </c>
       <c r="B89" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C89">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G89">
         <v>0</v>
@@ -3300,33 +3330,33 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>69</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
         <v>43</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="B91" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -3346,10 +3376,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>81</v>
+        <v>105</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3369,10 +3399,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B93" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3392,33 +3422,33 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="B94" t="s">
         <v>43</v>
       </c>
       <c r="C94">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G94">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3438,10 +3468,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>72</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3461,10 +3491,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B97" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3484,22 +3514,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B98" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C98">
-        <v>205</v>
+        <v>26</v>
       </c>
       <c r="D98">
-        <v>2.9</v>
+        <v>1.8</v>
       </c>
       <c r="E98">
-        <v>3.8</v>
+        <v>4.2</v>
       </c>
       <c r="F98">
-        <v>19.899999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3507,10 +3537,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B99" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3530,30 +3560,30 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="B100" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C100">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G100">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>8</v>
+        <v>81</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -3576,56 +3606,56 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>116</v>
       </c>
       <c r="B102" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C102">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F102">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G102">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>85</v>
+        <v>10</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G103">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3645,10 +3675,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="B105" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3668,10 +3698,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>113</v>
+        <v>66</v>
       </c>
       <c r="B106" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3691,73 +3721,76 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F107">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="G107">
         <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="B108" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C108">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G108">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B109" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G109">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>89</v>
+        <v>8</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -3780,70 +3813,274 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="B111" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G111">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C112">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G112">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>64</v>
+      </c>
+      <c r="B113" t="s">
+        <v>43</v>
+      </c>
+      <c r="C113">
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+      <c r="F113">
+        <v>0</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>64</v>
+      </c>
+      <c r="B114" t="s">
+        <v>41</v>
+      </c>
+      <c r="C114">
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+      <c r="F114">
+        <v>0</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>113</v>
+      </c>
+      <c r="B115" t="s">
+        <v>45</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>56</v>
+      </c>
+      <c r="B116" t="s">
+        <v>45</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+      <c r="F116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>6</v>
+      </c>
+      <c r="B117" t="s">
+        <v>43</v>
+      </c>
+      <c r="C117">
+        <v>68</v>
+      </c>
+      <c r="D117">
+        <v>4.5</v>
+      </c>
+      <c r="E117">
+        <v>12.9</v>
+      </c>
+      <c r="F117">
+        <v>0.2</v>
+      </c>
+      <c r="G117">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>59</v>
+      </c>
+      <c r="B118" t="s">
+        <v>45</v>
+      </c>
+      <c r="C118">
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <v>0</v>
+      </c>
+      <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>89</v>
+      </c>
+      <c r="B119" t="s">
+        <v>41</v>
+      </c>
+      <c r="C119">
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <v>0</v>
+      </c>
+      <c r="F119">
+        <v>0</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>58</v>
+      </c>
+      <c r="B120" t="s">
+        <v>46</v>
+      </c>
+      <c r="C120">
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <v>0</v>
+      </c>
+      <c r="F120">
+        <v>0</v>
+      </c>
+      <c r="G120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>28</v>
+      </c>
+      <c r="B121" t="s">
+        <v>43</v>
+      </c>
+      <c r="C121">
+        <v>138</v>
+      </c>
+      <c r="D121">
+        <v>2.6</v>
+      </c>
+      <c r="E121">
+        <v>30.9</v>
+      </c>
+      <c r="F121">
+        <v>1.3</v>
+      </c>
+      <c r="G121">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
         <v>80</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B122" t="s">
         <v>41</v>
       </c>
-      <c r="C113">
-        <v>0</v>
-      </c>
-      <c r="D113">
-        <v>0</v>
-      </c>
-      <c r="E113">
-        <v>0</v>
-      </c>
-      <c r="F113">
-        <v>0</v>
-      </c>
-      <c r="G113">
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Two of Dee's recipes.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,8 +10,8 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$73</definedName>
-    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$75</definedName>
+    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$51</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="133">
   <si>
     <t>carrots</t>
   </si>
@@ -415,9 +415,6 @@
     <t>olives</t>
   </si>
   <si>
-    <t>canned evapourated milk</t>
-  </si>
-  <si>
     <t>cinnamon</t>
   </si>
   <si>
@@ -431,6 +428,15 @@
   </si>
   <si>
     <t>fish fingers</t>
+  </si>
+  <si>
+    <t>canned evaporated milk</t>
+  </si>
+  <si>
+    <t>canned flageolet beans</t>
+  </si>
+  <si>
+    <t>condensed mushroom soup</t>
   </si>
 </sst>
 </file>
@@ -1263,16 +1269,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G122"/>
+  <dimension ref="A1:G124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48:G48"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -1651,7 +1657,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
         <v>43</v>
@@ -1697,7 +1703,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
       <c r="B19" t="s">
         <v>43</v>
@@ -1720,7 +1726,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
         <v>43</v>
@@ -1743,7 +1749,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>125</v>
+        <v>88</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
@@ -1766,7 +1772,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
         <v>43</v>
@@ -1789,7 +1795,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>43</v>
@@ -1812,30 +1818,30 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
       </c>
       <c r="C24">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="E24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F24">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>107</v>
+        <v>127</v>
       </c>
       <c r="B25" t="s">
         <v>43</v>
@@ -1858,53 +1864,53 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>43</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C27">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G27">
-        <v>2.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B28" t="s">
         <v>43</v>
@@ -1927,45 +1933,45 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B29" t="s">
         <v>45</v>
       </c>
       <c r="C29">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="D29">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="E29">
-        <v>0.9</v>
+        <v>7.9</v>
       </c>
       <c r="F29">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="G29">
-        <v>1.1000000000000001</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30">
-        <v>412</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>25.5</v>
+        <v>0</v>
       </c>
       <c r="E30">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>34.4</v>
+        <v>0</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -1973,45 +1979,45 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C31">
-        <v>183</v>
+        <v>7</v>
       </c>
       <c r="D31">
-        <v>29.2</v>
+        <v>0.5</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="F31">
-        <v>7.3</v>
+        <v>0.2</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>412</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>25.5</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -2019,22 +2025,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
         <v>44</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>29.2</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>7.3</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -2042,10 +2048,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2065,10 +2071,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>126</v>
+        <v>68</v>
       </c>
       <c r="B35" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2088,10 +2094,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2111,10 +2117,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B37" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2134,10 +2140,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="B38" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2157,10 +2163,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2180,10 +2186,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2203,45 +2209,45 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C41">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>35.6</v>
+        <v>0</v>
       </c>
       <c r="F41">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G41">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B42" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C42">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>68.8</v>
+        <v>0</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -2249,45 +2255,45 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>35.6</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -2295,7 +2301,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>94</v>
+        <v>27</v>
       </c>
       <c r="B45" t="s">
         <v>41</v>
@@ -2318,7 +2324,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B46" t="s">
         <v>41</v>
@@ -2341,22 +2347,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>21</v>
+        <v>94</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C47">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>0</v>
@@ -2364,10 +2370,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2387,22 +2393,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="B49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2410,10 +2416,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2433,10 +2439,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="B51" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2456,10 +2462,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="B52" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2479,7 +2485,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>36</v>
       </c>
       <c r="B53" t="s">
         <v>45</v>
@@ -2502,22 +2508,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C54">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2525,10 +2531,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>37</v>
+        <v>92</v>
       </c>
       <c r="B55" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2548,22 +2554,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="B56" t="s">
         <v>45</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2571,7 +2577,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
       <c r="B57" t="s">
         <v>43</v>
@@ -2594,10 +2600,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2617,10 +2623,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>39</v>
+        <v>120</v>
       </c>
       <c r="B59" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2640,102 +2646,102 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C60">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="G60">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C61">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G61">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B62" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
       <c r="B63" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2755,10 +2761,10 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="B65" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2778,22 +2784,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>3</v>
+        <v>38</v>
       </c>
       <c r="B66" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C66">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2801,22 +2807,22 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>110</v>
       </c>
       <c r="B67" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C67">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G67">
         <v>0</v>
@@ -2824,22 +2830,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
         <v>44</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>37.1</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -2847,22 +2853,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>5</v>
       </c>
       <c r="B69" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2870,10 +2876,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2893,10 +2899,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B71" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2916,7 +2922,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B72" t="s">
         <v>41</v>
@@ -2939,10 +2945,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2962,10 +2968,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2985,42 +2991,42 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>26</v>
+        <v>101</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C75">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G75">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C76">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3031,42 +3037,42 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>124</v>
+        <v>26</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>123</v>
+        <v>4</v>
       </c>
       <c r="B78" t="s">
         <v>41</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F78">
         <v>0</v>
@@ -3077,30 +3083,30 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>1</v>
+        <v>124</v>
       </c>
       <c r="B79" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C79">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G79">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>123</v>
       </c>
       <c r="B80" t="s">
         <v>41</v>
@@ -3123,33 +3129,33 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -3169,10 +3175,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B83" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3192,10 +3198,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B84" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C84">
         <v>0</v>
@@ -3215,99 +3221,99 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>32</v>
+        <v>112</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C85">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G85">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>16</v>
+        <v>97</v>
       </c>
       <c r="B86" t="s">
         <v>43</v>
       </c>
       <c r="C86">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>25.6</v>
+        <v>0</v>
       </c>
       <c r="E86">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>46.1</v>
+        <v>0</v>
       </c>
       <c r="G86">
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="B87" t="s">
         <v>43</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="B89" t="s">
         <v>43</v>
@@ -3330,30 +3336,30 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="B90" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C90">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G90">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="B91" t="s">
         <v>43</v>
@@ -3376,30 +3382,30 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
         <v>43</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="B93" t="s">
         <v>43</v>
@@ -3422,7 +3428,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="B94" t="s">
         <v>43</v>
@@ -3445,10 +3451,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3468,10 +3474,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B96" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3491,10 +3497,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3514,22 +3520,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>76</v>
+        <v>121</v>
       </c>
       <c r="B98" t="s">
         <v>45</v>
       </c>
       <c r="C98">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G98">
         <v>0</v>
@@ -3537,7 +3543,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B99" t="s">
         <v>43</v>
@@ -3560,22 +3566,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="B100" t="s">
         <v>45</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3583,10 +3589,10 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B101" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -3606,10 +3612,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B102" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3629,33 +3635,33 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B103" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C103">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G103">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B104" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3675,33 +3681,33 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="B105" t="s">
         <v>43</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B106" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3721,22 +3727,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B107" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C107">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -3744,10 +3750,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B108" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3767,30 +3773,30 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B109" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C109">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D109">
-        <v>3.6</v>
+        <v>2.9</v>
       </c>
       <c r="E109">
-        <v>22.2</v>
+        <v>3.8</v>
       </c>
       <c r="F109">
-        <v>7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G109">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
@@ -3813,30 +3819,30 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
         <v>43</v>
       </c>
       <c r="C111">
-        <v>826</v>
+        <v>104</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E111">
-        <v>12.1</v>
+        <v>22.2</v>
       </c>
       <c r="F111">
-        <v>86.7</v>
+        <v>7</v>
       </c>
       <c r="G111">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="B112" t="s">
         <v>41</v>
@@ -3859,30 +3865,30 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>64</v>
+        <v>11</v>
       </c>
       <c r="B113" t="s">
         <v>43</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G113">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="B114" t="s">
         <v>41</v>
@@ -3905,10 +3911,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>64</v>
       </c>
       <c r="B115" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3928,10 +3934,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B116" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3943,35 +3949,38 @@
         <v>0</v>
       </c>
       <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116">
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>6</v>
+        <v>113</v>
       </c>
       <c r="B117" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C117">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G117">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B118" t="s">
         <v>45</v>
@@ -3988,39 +3997,36 @@
       <c r="F118">
         <v>0</v>
       </c>
-      <c r="G118">
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>89</v>
+        <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G119">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B120" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -4040,47 +4046,93 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="B121" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C121">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F121">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G121">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
+        <v>58</v>
+      </c>
+      <c r="B122" t="s">
+        <v>46</v>
+      </c>
+      <c r="C122">
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <v>0</v>
+      </c>
+      <c r="F122">
+        <v>0</v>
+      </c>
+      <c r="G122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>28</v>
+      </c>
+      <c r="B123" t="s">
+        <v>43</v>
+      </c>
+      <c r="C123">
+        <v>138</v>
+      </c>
+      <c r="D123">
+        <v>2.6</v>
+      </c>
+      <c r="E123">
+        <v>30.9</v>
+      </c>
+      <c r="F123">
+        <v>1.3</v>
+      </c>
+      <c r="G123">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>80</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B124" t="s">
         <v>41</v>
       </c>
-      <c r="C122">
-        <v>0</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
-      <c r="E122">
-        <v>0</v>
-      </c>
-      <c r="F122">
-        <v>0</v>
-      </c>
-      <c r="G122">
+      <c r="C124">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <v>0</v>
+      </c>
+      <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusted the tuna bake.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="134">
   <si>
     <t>carrots</t>
   </si>
@@ -79,9 +79,6 @@
     <t>mixed herbs</t>
   </si>
   <si>
-    <t>canned tomatoes</t>
-  </si>
-  <si>
     <t>lasagna</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>IngredientType</t>
   </si>
   <si>
-    <t>canned chick peas</t>
-  </si>
-  <si>
     <t>raisins</t>
   </si>
   <si>
@@ -262,9 +256,6 @@
     <t>pearl barley</t>
   </si>
   <si>
-    <t>canned kidney beans</t>
-  </si>
-  <si>
     <t>green chilli</t>
   </si>
   <si>
@@ -304,9 +295,6 @@
     <t>dried thyme</t>
   </si>
   <si>
-    <t>canned coconut milk</t>
-  </si>
-  <si>
     <t>turmeric</t>
   </si>
   <si>
@@ -361,9 +349,6 @@
     <t>anchovy fillets</t>
   </si>
   <si>
-    <t>canned tuna fish</t>
-  </si>
-  <si>
     <t>pesto</t>
   </si>
   <si>
@@ -373,9 +358,6 @@
     <t>mayonaise</t>
   </si>
   <si>
-    <t>canned borlotti beans</t>
-  </si>
-  <si>
     <t>parsnips</t>
   </si>
   <si>
@@ -421,22 +403,43 @@
     <t>pineapple chunks</t>
   </si>
   <si>
-    <t>canned sweetcorn</t>
-  </si>
-  <si>
-    <t>canned baked beans</t>
-  </si>
-  <si>
     <t>fish fingers</t>
   </si>
   <si>
-    <t>canned evaporated milk</t>
-  </si>
-  <si>
-    <t>canned flageolet beans</t>
-  </si>
-  <si>
-    <t>condensed mushroom soup</t>
+    <t>can chick peas</t>
+  </si>
+  <si>
+    <t>can coconut milk</t>
+  </si>
+  <si>
+    <t>can evaporated milk</t>
+  </si>
+  <si>
+    <t>can flageolet beans</t>
+  </si>
+  <si>
+    <t>can kidney beans</t>
+  </si>
+  <si>
+    <t>can sweetcorn</t>
+  </si>
+  <si>
+    <t>can tomatoes</t>
+  </si>
+  <si>
+    <t>can tuna fish</t>
+  </si>
+  <si>
+    <t>can borlotti beans</t>
+  </si>
+  <si>
+    <t>can baked beans</t>
+  </si>
+  <si>
+    <t>can mushroom soup</t>
+  </si>
+  <si>
+    <t>frozen peas</t>
   </si>
 </sst>
 </file>
@@ -1269,11 +1272,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G124"/>
+  <dimension ref="A1:G125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,33 +1292,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
       <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -1335,10 +1338,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1358,10 +1361,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1381,10 +1384,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1404,10 +1407,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1427,10 +1430,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <v>75</v>
@@ -1450,10 +1453,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>136</v>
@@ -1473,10 +1476,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1496,10 +1499,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1519,10 +1522,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>90</v>
@@ -1542,10 +1545,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12">
         <v>77</v>
@@ -1565,10 +1568,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1588,10 +1591,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1611,10 +1614,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>0</v>
@@ -1634,10 +1637,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16">
         <v>26</v>
@@ -1657,10 +1660,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1680,10 +1683,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1703,10 +1706,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19">
         <v>0</v>
@@ -1726,10 +1729,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -1749,10 +1752,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>0</v>
@@ -1772,10 +1775,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -1795,10 +1798,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23">
         <v>0</v>
@@ -1818,10 +1821,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>132</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -1844,7 +1847,7 @@
         <v>127</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1864,10 +1867,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26">
         <v>16</v>
@@ -1887,10 +1890,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="B27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -1910,10 +1913,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1936,7 +1939,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29">
         <v>35</v>
@@ -1956,10 +1959,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30">
         <v>0</v>
@@ -1982,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C31">
         <v>7</v>
@@ -2002,10 +2005,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C32">
         <v>412</v>
@@ -2025,10 +2028,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33">
         <v>183</v>
@@ -2051,7 +2054,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -2071,10 +2074,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35">
         <v>0</v>
@@ -2094,10 +2097,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -2117,10 +2120,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2140,10 +2143,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2163,10 +2166,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2189,7 +2192,7 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2209,10 +2212,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2232,10 +2235,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2255,10 +2258,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43">
         <v>176</v>
@@ -2278,10 +2281,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C44">
         <v>669</v>
@@ -2301,10 +2304,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2324,10 +2327,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2347,10 +2350,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2370,10 +2373,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2393,10 +2396,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C49">
         <v>147</v>
@@ -2416,10 +2419,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2439,10 +2442,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2462,10 +2465,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B52" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2485,10 +2488,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>133</v>
       </c>
       <c r="B53" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2508,10 +2511,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="B54" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C54">
         <v>0</v>
@@ -2531,10 +2534,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2554,22 +2557,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C56">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -2577,22 +2580,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G57">
         <v>0</v>
@@ -2600,10 +2603,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="B58" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2623,10 +2626,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2646,10 +2649,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>40</v>
+        <v>114</v>
       </c>
       <c r="B60" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -2672,7 +2675,7 @@
         <v>39</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2692,79 +2695,79 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>109</v>
+        <v>38</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C62">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="G62">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C63">
-        <v>348</v>
+        <v>12</v>
       </c>
       <c r="D63">
-        <v>13</v>
+        <v>2.8</v>
       </c>
       <c r="E63">
-        <v>70</v>
+        <v>1.4</v>
       </c>
       <c r="F63">
-        <v>1.8</v>
+        <v>11.8</v>
       </c>
       <c r="G63">
-        <v>3.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="B64" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B65" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2784,10 +2787,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2807,10 +2810,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>37</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2830,22 +2833,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>3</v>
+        <v>105</v>
       </c>
       <c r="B68" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C68">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G68">
         <v>0</v>
@@ -2853,22 +2856,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B69" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C69">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D69">
-        <v>3.3</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E69">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>1.6</v>
+        <v>37.1</v>
       </c>
       <c r="G69">
         <v>0</v>
@@ -2876,22 +2879,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>5</v>
       </c>
       <c r="B70" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G70">
         <v>0</v>
@@ -2899,10 +2902,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B71" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2922,10 +2925,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2945,10 +2948,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2968,10 +2971,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2991,10 +2994,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="B75" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -3014,10 +3017,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -3037,65 +3040,65 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B77" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C77">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G77">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C78">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E78">
-        <v>99.9</v>
+        <v>13</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>124</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3106,10 +3109,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -3129,56 +3132,56 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>1</v>
+        <v>118</v>
       </c>
       <c r="B81" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C81">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G81">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3198,7 +3201,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B84" t="s">
         <v>42</v>
@@ -3221,10 +3224,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3244,10 +3247,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B86" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3267,79 +3270,79 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>32</v>
+        <v>93</v>
       </c>
       <c r="B87" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C87">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="B88" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C88">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="D88">
-        <v>25.6</v>
+        <v>5.2</v>
       </c>
       <c r="E88">
-        <v>12.5</v>
+        <v>24.4</v>
       </c>
       <c r="F88">
-        <v>46.1</v>
+        <v>1.5</v>
       </c>
       <c r="G88">
-        <v>6.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -3359,10 +3362,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>108</v>
+        <v>79</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C91">
         <v>0</v>
@@ -3382,33 +3385,33 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>22</v>
+        <v>103</v>
       </c>
       <c r="B92" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C92">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E92">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G92">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3428,33 +3431,33 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>105</v>
+        <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3474,10 +3477,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
       <c r="B96" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3497,7 +3500,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>113</v>
       </c>
       <c r="B97" t="s">
         <v>42</v>
@@ -3520,10 +3523,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3543,10 +3546,10 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
       <c r="B99" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3566,22 +3569,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="B100" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C100">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G100">
         <v>0</v>
@@ -3589,22 +3592,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G101">
         <v>0</v>
@@ -3612,10 +3615,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B102" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3635,10 +3638,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3658,10 +3661,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="B104" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3681,56 +3684,56 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>110</v>
       </c>
       <c r="B105" t="s">
         <v>43</v>
       </c>
       <c r="C105">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G105">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>72</v>
+        <v>10</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B107" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3750,7 +3753,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B108" t="s">
         <v>42</v>
@@ -3773,22 +3776,22 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="B109" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C109">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G109">
         <v>0</v>
@@ -3796,22 +3799,22 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>71</v>
+        <v>22</v>
       </c>
       <c r="B110" t="s">
         <v>41</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3819,102 +3822,102 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="B111" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C111">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E111">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G111">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B112" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G112">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B113" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C113">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D113">
         <v>0</v>
       </c>
       <c r="E113">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G113">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>85</v>
+        <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D114">
         <v>0</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G114">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="B115" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3934,10 +3937,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B116" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3957,10 +3960,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="B117" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -3980,10 +3983,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="B118" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -3995,61 +3998,61 @@
         <v>0</v>
       </c>
       <c r="F118">
+        <v>0</v>
+      </c>
+      <c r="G118">
         <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="B119" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C119">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>0.2</v>
-      </c>
-      <c r="G119">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G120">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="B121" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4069,10 +4072,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
       <c r="B122" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -4092,53 +4095,76 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C123">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G123">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>27</v>
       </c>
       <c r="B124" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>30.9</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="G124">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>77</v>
+      </c>
+      <c r="B125" t="s">
+        <v>40</v>
+      </c>
+      <c r="C125">
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G113">
-    <sortCondition ref="A2:A113"/>
+  <sortState ref="A2:G125">
+    <sortCondition ref="A2:A125"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
New recipe and slight adjustment in case there is no quantity for an ingredient.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,8 +10,8 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$84</definedName>
-    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$86</definedName>
+    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$56</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
   <si>
     <t>carrots</t>
   </si>
@@ -466,9 +466,6 @@
     <t>ground turmeric</t>
   </si>
   <si>
-    <t>ground cinamon</t>
-  </si>
-  <si>
     <t>can sardines</t>
   </si>
   <si>
@@ -479,6 +476,15 @@
   </si>
   <si>
     <t>garam masala</t>
+  </si>
+  <si>
+    <t>ground ginger</t>
+  </si>
+  <si>
+    <t>dried apricots</t>
+  </si>
+  <si>
+    <t>fresh coriander</t>
   </si>
 </sst>
 </file>
@@ -1311,11 +1317,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G137"/>
+  <dimension ref="A1:G139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B59" sqref="B59:G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,7 +1981,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B29" t="s">
         <v>41</v>
@@ -2527,22 +2533,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C53">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E53">
         <v>0</v>
       </c>
       <c r="F53">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G53">
         <v>0</v>
@@ -2550,22 +2556,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2573,7 +2579,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B55" t="s">
         <v>41</v>
@@ -2596,10 +2602,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B56" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2619,10 +2625,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2642,10 +2648,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>34</v>
+        <v>132</v>
       </c>
       <c r="B58" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2665,10 +2671,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2688,7 +2694,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>138</v>
+        <v>34</v>
       </c>
       <c r="B60" t="s">
         <v>43</v>
@@ -2711,10 +2717,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2734,7 +2740,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="B62" t="s">
         <v>43</v>
@@ -2757,22 +2763,22 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="B63" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C63">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G63">
         <v>0</v>
@@ -2780,10 +2786,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="B64" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2803,22 +2809,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B65" t="s">
         <v>43</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2826,10 +2832,10 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>35</v>
       </c>
       <c r="B66" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2849,10 +2855,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B67" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2872,7 +2878,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="B68" t="s">
         <v>39</v>
@@ -2895,7 +2901,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>141</v>
+        <v>38</v>
       </c>
       <c r="B69" t="s">
         <v>39</v>
@@ -2918,7 +2924,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>37</v>
       </c>
       <c r="B70" t="s">
         <v>39</v>
@@ -2941,7 +2947,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
         <v>39</v>
@@ -2964,102 +2970,102 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>103</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C72">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>12</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C73">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="G73">
-        <v>3.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="B74" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>11.8</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -3079,10 +3085,10 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>104</v>
+        <v>33</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -3102,22 +3108,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B78" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C78">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E78">
         <v>0</v>
       </c>
       <c r="F78">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G78">
         <v>0</v>
@@ -3125,22 +3131,22 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C79">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -3148,22 +3154,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
         <v>42</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>37.1</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3171,22 +3177,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>74</v>
+        <v>5</v>
       </c>
       <c r="B81" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3194,10 +3200,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C82">
         <v>0</v>
@@ -3217,10 +3223,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3240,7 +3246,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="B84" t="s">
         <v>39</v>
@@ -3263,10 +3269,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="B85" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3286,10 +3292,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3309,42 +3315,42 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C87">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G87">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C88">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>99.9</v>
+        <v>0</v>
       </c>
       <c r="F88">
         <v>0</v>
@@ -3355,42 +3361,42 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>117</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F90">
         <v>0</v>
@@ -3401,33 +3407,33 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>1</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C91">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E91">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G91">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>117</v>
       </c>
       <c r="B92" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3447,33 +3453,33 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3493,10 +3499,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B95" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3516,10 +3522,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B96" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3539,99 +3545,99 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>105</v>
       </c>
       <c r="B97" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C97">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D97">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G97">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>14</v>
+        <v>92</v>
       </c>
       <c r="B98" t="s">
         <v>41</v>
       </c>
       <c r="C98">
-        <v>564</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>25.6</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>46.1</v>
+        <v>0</v>
       </c>
       <c r="G98">
-        <v>6.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="B99" t="s">
         <v>41</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>132</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>5.2</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>24.4</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>78</v>
+        <v>14</v>
       </c>
       <c r="B100" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
@@ -3654,10 +3660,10 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3677,30 +3683,30 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>20</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>41</v>
       </c>
       <c r="C103">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G103">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -3723,30 +3729,30 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G105">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B106" t="s">
         <v>41</v>
@@ -3769,10 +3775,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B107" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3792,10 +3798,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B108" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3815,10 +3821,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3838,22 +3844,22 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>72</v>
+        <v>114</v>
       </c>
       <c r="B110" t="s">
         <v>43</v>
       </c>
       <c r="C110">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G110">
         <v>0</v>
@@ -3861,7 +3867,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B111" t="s">
         <v>41</v>
@@ -3884,22 +3890,22 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B112" t="s">
         <v>43</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -3907,10 +3913,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B113" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3930,10 +3936,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>57</v>
       </c>
       <c r="B114" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3953,33 +3959,33 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C115">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G115">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="B116" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3999,33 +4005,33 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>69</v>
+        <v>9</v>
       </c>
       <c r="B117" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G117">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B118" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -4045,10 +4051,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B119" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C119">
         <v>0</v>
@@ -4068,22 +4074,22 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="B120" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C120">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G120">
         <v>0</v>
@@ -4091,10 +4097,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B121" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4114,33 +4120,33 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="B122" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C122">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D122">
-        <v>3.6</v>
+        <v>2.9</v>
       </c>
       <c r="E122">
-        <v>22.2</v>
+        <v>3.8</v>
       </c>
       <c r="F122">
-        <v>7</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G122">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>145</v>
+        <v>68</v>
       </c>
       <c r="B123" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -4160,53 +4166,53 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="B124" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G124">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>144</v>
       </c>
       <c r="B125" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C125">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D125">
         <v>0</v>
       </c>
       <c r="E125">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F125">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G125">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>81</v>
+        <v>143</v>
       </c>
       <c r="B126" t="s">
         <v>39</v>
@@ -4229,30 +4235,30 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B127" t="s">
         <v>41</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G127">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B128" t="s">
         <v>39</v>
@@ -4275,10 +4281,10 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B129" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -4298,10 +4304,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B130" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -4313,35 +4319,38 @@
         <v>0</v>
       </c>
       <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130">
         <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>6</v>
+        <v>106</v>
       </c>
       <c r="B131" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C131">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G131">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B132" t="s">
         <v>43</v>
@@ -4358,39 +4367,36 @@
       <c r="F132">
         <v>0</v>
       </c>
-      <c r="G132">
-        <v>0</v>
-      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>139</v>
+        <v>6</v>
       </c>
       <c r="B133" t="s">
         <v>41</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G133">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B134" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -4410,10 +4416,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4433,47 +4439,93 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>26</v>
+        <v>84</v>
       </c>
       <c r="B136" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C136">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E136">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F136">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G136">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
+        <v>55</v>
+      </c>
+      <c r="B137" t="s">
+        <v>44</v>
+      </c>
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>26</v>
+      </c>
+      <c r="B138" t="s">
+        <v>41</v>
+      </c>
+      <c r="C138">
+        <v>138</v>
+      </c>
+      <c r="D138">
+        <v>2.6</v>
+      </c>
+      <c r="E138">
+        <v>30.9</v>
+      </c>
+      <c r="F138">
+        <v>1.3</v>
+      </c>
+      <c r="G138">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>76</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B139" t="s">
         <v>39</v>
       </c>
-      <c r="C137">
-        <v>0</v>
-      </c>
-      <c r="D137">
-        <v>0</v>
-      </c>
-      <c r="E137">
-        <v>0</v>
-      </c>
-      <c r="F137">
-        <v>0</v>
-      </c>
-      <c r="G137">
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added chilli to the tuna bake
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -10,8 +10,8 @@
     <sheet name="tblIngredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$86</definedName>
-    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">tblIngredients!$A$1:$G$87</definedName>
+    <definedName name="tblIngredients" localSheetId="0">tblIngredients!$A$2:$H$57</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="150">
   <si>
     <t>carrots</t>
   </si>
@@ -485,6 +485,9 @@
   </si>
   <si>
     <t>fresh coriander</t>
+  </si>
+  <si>
+    <t>chillis</t>
   </si>
 </sst>
 </file>
@@ -1317,11 +1320,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B59" sqref="B59:G59"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37:G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,10 +2168,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2188,10 +2191,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2211,10 +2214,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>136</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C39">
         <v>0</v>
@@ -2234,10 +2237,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>111</v>
+        <v>65</v>
       </c>
       <c r="B40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -2257,7 +2260,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B41" t="s">
         <v>41</v>
@@ -2280,10 +2283,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2303,7 +2306,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B43" t="s">
         <v>39</v>
@@ -2326,10 +2329,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2349,10 +2352,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2372,10 +2375,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2395,48 +2398,48 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C47">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>35.6</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G47">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B48" t="s">
         <v>41</v>
       </c>
       <c r="C48">
-        <v>669</v>
+        <v>176</v>
       </c>
       <c r="D48">
         <v>6</v>
       </c>
       <c r="E48">
-        <v>7</v>
+        <v>35.6</v>
       </c>
       <c r="F48">
-        <v>68.8</v>
+        <v>0.3</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -2444,19 +2447,19 @@
         <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>68.8</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -2464,7 +2467,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="B50" t="s">
         <v>39</v>
@@ -2487,7 +2490,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="B51" t="s">
         <v>39</v>
@@ -2510,7 +2513,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B52" t="s">
         <v>39</v>
@@ -2533,10 +2536,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2556,22 +2559,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C54">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>12.5</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <v>0</v>
       </c>
       <c r="F54">
-        <v>10.8</v>
+        <v>0</v>
       </c>
       <c r="G54">
         <v>0</v>
@@ -2579,22 +2582,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>120</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>10.8</v>
       </c>
       <c r="G55">
         <v>0</v>
@@ -2602,7 +2605,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="B56" t="s">
         <v>41</v>
@@ -2625,10 +2628,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>32</v>
+        <v>108</v>
       </c>
       <c r="B57" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2648,10 +2651,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>132</v>
+        <v>32</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2671,10 +2674,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>34</v>
+        <v>148</v>
       </c>
       <c r="B60" t="s">
         <v>43</v>
@@ -2717,10 +2720,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>145</v>
+        <v>34</v>
       </c>
       <c r="B61" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2740,10 +2743,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B62" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C62">
         <v>0</v>
@@ -2763,10 +2766,10 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
       <c r="B63" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -2786,10 +2789,10 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2809,22 +2812,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B65" t="s">
         <v>43</v>
       </c>
       <c r="C65">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>0.7</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -2832,22 +2835,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>35</v>
+        <v>71</v>
       </c>
       <c r="B66" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="G66">
         <v>0</v>
@@ -2855,10 +2858,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B67" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2878,10 +2881,10 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2901,7 +2904,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="B69" t="s">
         <v>39</v>
@@ -2924,7 +2927,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B70" t="s">
         <v>39</v>
@@ -2947,7 +2950,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
         <v>39</v>
@@ -2970,7 +2973,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B72" t="s">
         <v>39</v>
@@ -2993,7 +2996,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B73" t="s">
         <v>39</v>
@@ -3016,76 +3019,76 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>103</v>
+        <v>134</v>
       </c>
       <c r="B74" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C74">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>11.8</v>
+        <v>0</v>
       </c>
       <c r="G74">
-        <v>1.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>103</v>
+      </c>
+      <c r="B75" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75">
         <v>12</v>
       </c>
-      <c r="B75" t="s">
-        <v>41</v>
-      </c>
-      <c r="C75">
-        <v>348</v>
-      </c>
       <c r="D75">
-        <v>13</v>
+        <v>2.8</v>
       </c>
       <c r="E75">
-        <v>70</v>
+        <v>1.4</v>
       </c>
       <c r="F75">
-        <v>1.8</v>
+        <v>11.8</v>
       </c>
       <c r="G75">
-        <v>3.4</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="B76" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>33</v>
+        <v>95</v>
       </c>
       <c r="B77" t="s">
         <v>43</v>
@@ -3108,10 +3111,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B78" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -3131,10 +3134,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="B79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -3154,22 +3157,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="B80" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C80">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>19.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="E80">
         <v>0</v>
       </c>
       <c r="F80">
-        <v>37.1</v>
+        <v>0</v>
       </c>
       <c r="G80">
         <v>0</v>
@@ -3177,22 +3180,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B81" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C81">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D81">
-        <v>3.3</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="E81">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>1.6</v>
+        <v>37.1</v>
       </c>
       <c r="G81">
         <v>0</v>
@@ -3200,22 +3203,22 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>3.3</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="G82">
         <v>0</v>
@@ -3223,10 +3226,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C83">
         <v>0</v>
@@ -3246,7 +3249,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s">
         <v>39</v>
@@ -3269,10 +3272,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="B85" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C85">
         <v>0</v>
@@ -3292,10 +3295,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="B86" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -3315,7 +3318,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="B87" t="s">
         <v>39</v>
@@ -3338,10 +3341,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="B88" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3361,65 +3364,65 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
         <v>41</v>
       </c>
       <c r="C89">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G89">
-        <v>0.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B90" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C90">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E90">
-        <v>99.9</v>
+        <v>13</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>116</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
         <v>39</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>99.9</v>
       </c>
       <c r="F91">
         <v>0</v>
@@ -3430,10 +3433,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B92" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3453,56 +3456,56 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="B93" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C93">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>7.9</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G93">
-        <v>1.4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>7.9</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3522,10 +3525,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B96" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3545,10 +3548,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3568,10 +3571,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B98" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3591,79 +3594,79 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B99" t="s">
         <v>41</v>
       </c>
       <c r="C99">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>5.2</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>24.4</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G99">
-        <v>1.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="B100" t="s">
         <v>41</v>
       </c>
       <c r="C100">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="D100">
-        <v>25.6</v>
+        <v>5.2</v>
       </c>
       <c r="E100">
-        <v>12.5</v>
+        <v>24.4</v>
       </c>
       <c r="F100">
-        <v>46.1</v>
+        <v>1.5</v>
       </c>
       <c r="G100">
-        <v>6.2</v>
+        <v>1.3</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>70</v>
+        <v>14</v>
       </c>
       <c r="B101" t="s">
         <v>41</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>25.6</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>12.5</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B102" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3683,10 +3686,10 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="B103" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3706,7 +3709,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>41</v>
@@ -3729,53 +3732,53 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>20</v>
+        <v>119</v>
       </c>
       <c r="B105" t="s">
         <v>41</v>
       </c>
       <c r="C105">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>9.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>57.9</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G105">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="B106" t="s">
         <v>41</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>57.9</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G106">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="B107" t="s">
         <v>41</v>
@@ -3798,7 +3801,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B108" t="s">
         <v>41</v>
@@ -3821,10 +3824,10 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="B109" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3844,10 +3847,10 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>114</v>
+        <v>85</v>
       </c>
       <c r="B110" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3867,10 +3870,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>52</v>
+        <v>114</v>
       </c>
       <c r="B111" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -3890,22 +3893,22 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B112" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C112">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>1.8</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>4.2</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -3913,22 +3916,22 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="B113" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G113">
         <v>0</v>
@@ -3936,10 +3939,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B114" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3959,10 +3962,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B115" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3982,10 +3985,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>109</v>
+        <v>77</v>
       </c>
       <c r="B116" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -4005,53 +4008,53 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>9</v>
+        <v>109</v>
       </c>
       <c r="B117" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C117">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>8.9</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>75.599999999999994</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="G117">
-        <v>3.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
       <c r="B118" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>8.9</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>75.599999999999994</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="G118">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
       <c r="B119" t="s">
         <v>39</v>
@@ -4074,10 +4077,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>133</v>
+        <v>69</v>
       </c>
       <c r="B120" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -4097,10 +4100,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>63</v>
+        <v>133</v>
       </c>
       <c r="B121" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -4120,22 +4123,22 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>21</v>
+        <v>63</v>
       </c>
       <c r="B122" t="s">
         <v>40</v>
       </c>
       <c r="C122">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="E122">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>19.899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -4143,22 +4146,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="B123" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>2.9</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="G123">
         <v>0</v>
@@ -4166,56 +4169,56 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="B124" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C124">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="E124">
-        <v>22.2</v>
+        <v>0</v>
       </c>
       <c r="F124">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G124">
-        <v>1.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>144</v>
+        <v>29</v>
       </c>
       <c r="B125" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>3.6</v>
       </c>
       <c r="E125">
-        <v>0</v>
+        <v>22.2</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G125">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B126" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -4235,56 +4238,56 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="B127" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C127">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
       <c r="E127">
-        <v>12.1</v>
+        <v>0</v>
       </c>
       <c r="F127">
-        <v>86.7</v>
+        <v>0</v>
       </c>
       <c r="G127">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="B128" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D128">
         <v>0</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>12.1</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>86.7</v>
       </c>
       <c r="G128">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="B129" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -4307,7 +4310,7 @@
         <v>61</v>
       </c>
       <c r="B130" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -4327,10 +4330,10 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="B131" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -4350,7 +4353,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="B132" t="s">
         <v>43</v>
@@ -4367,59 +4370,59 @@
       <c r="F132">
         <v>0</v>
       </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="B133" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C133">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E133">
-        <v>12.9</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>0.2</v>
-      </c>
-      <c r="G133">
-        <v>2.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B134" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>12.9</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="G134">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>139</v>
+        <v>56</v>
       </c>
       <c r="B135" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4439,10 +4442,10 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="B136" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -4462,10 +4465,10 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="B137" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -4485,47 +4488,70 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
       <c r="B138" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C138">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>2.6</v>
+        <v>0</v>
       </c>
       <c r="E138">
-        <v>30.9</v>
+        <v>0</v>
       </c>
       <c r="F138">
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="G138">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
+        <v>26</v>
+      </c>
+      <c r="B139" t="s">
+        <v>41</v>
+      </c>
+      <c r="C139">
+        <v>138</v>
+      </c>
+      <c r="D139">
+        <v>2.6</v>
+      </c>
+      <c r="E139">
+        <v>30.9</v>
+      </c>
+      <c r="F139">
+        <v>1.3</v>
+      </c>
+      <c r="G139">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>76</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>39</v>
       </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-      <c r="D139">
-        <v>0</v>
-      </c>
-      <c r="E139">
-        <v>0</v>
-      </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-      <c r="G139">
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added together ingredients and concatenated meal labels.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc_d4jqqip\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="170">
   <si>
     <t>IngredientName</t>
   </si>
@@ -523,6 +523,12 @@
   </si>
   <si>
     <t>branston pickle</t>
+  </si>
+  <si>
+    <t>can cannellini beans</t>
+  </si>
+  <si>
+    <t>peanut butter</t>
   </si>
 </sst>
 </file>
@@ -1329,11 +1335,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H54" sqref="H54"/>
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H113" sqref="H113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1754,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>168</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1768,7 +1774,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1788,47 +1794,47 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>162</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F23">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1848,7 +1854,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1868,59 +1874,59 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>33</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>163</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E28">
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -1928,19 +1934,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>38</v>
+        <v>160</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -1948,7 +1954,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -1968,19 +1974,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -1988,19 +1994,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2008,7 +2014,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -2028,19 +2034,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C35">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2048,19 +2054,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2068,10 +2074,10 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37">
         <v>0</v>
@@ -2088,19 +2094,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
       <c r="C38">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2108,70 +2114,70 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="C39">
-        <v>412</v>
+        <v>7</v>
       </c>
       <c r="D39">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C40">
-        <v>183</v>
+        <v>412</v>
       </c>
       <c r="D40">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E41">
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2188,7 +2194,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
@@ -2208,10 +2214,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2228,10 +2234,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2248,7 +2254,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -2268,10 +2274,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C47">
         <v>0</v>
@@ -2288,7 +2294,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
         <v>10</v>
@@ -2308,10 +2314,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2328,50 +2334,50 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>150</v>
+        <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C50">
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="B51" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2388,19 +2394,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C53">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -2408,19 +2414,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2428,22 +2434,22 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C55">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2451,24 +2457,24 @@
         <v>59</v>
       </c>
       <c r="B56" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -2488,7 +2494,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
         <v>10</v>
@@ -2508,10 +2514,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2528,10 +2534,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C60">
         <v>0</v>
@@ -2548,47 +2554,47 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C61">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E61">
         <v>0</v>
       </c>
       <c r="F61">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -2608,10 +2614,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B64" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C64">
         <v>0</v>
@@ -2628,10 +2634,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B65" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2648,10 +2654,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2668,10 +2674,10 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2688,10 +2694,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2708,7 +2714,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B69" t="s">
         <v>8</v>
@@ -2728,10 +2734,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2748,50 +2754,50 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2808,10 +2814,10 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B74" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2828,7 +2834,7 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
@@ -2848,7 +2854,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
@@ -2868,7 +2874,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B77" t="s">
         <v>10</v>
@@ -2888,7 +2894,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>159</v>
+        <v>81</v>
       </c>
       <c r="B78" t="s">
         <v>10</v>
@@ -2908,7 +2914,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>159</v>
       </c>
       <c r="B79" t="s">
         <v>10</v>
@@ -2928,7 +2934,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
@@ -2948,107 +2954,107 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C81">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>154</v>
+        <v>84</v>
       </c>
       <c r="B83" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C83">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E83">
         <v>0</v>
       </c>
       <c r="F83">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>85</v>
+        <v>154</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C84">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D84">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E84">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B86" t="s">
         <v>8</v>
@@ -3068,10 +3074,10 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3088,10 +3094,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3108,70 +3114,70 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E89">
         <v>0</v>
       </c>
       <c r="F89">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C90">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E90">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C92">
         <v>0</v>
@@ -3188,7 +3194,7 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93" t="s">
         <v>10</v>
@@ -3208,10 +3214,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3228,10 +3234,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3248,7 +3254,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B96" t="s">
         <v>10</v>
@@ -3268,10 +3274,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3288,59 +3294,59 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
       </c>
       <c r="C98">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C99">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E99">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B100" t="s">
         <v>10</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D100">
         <v>0</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -3348,10 +3354,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -3368,19 +3374,19 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C102">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -3388,19 +3394,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -3408,10 +3414,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3428,10 +3434,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>153</v>
+        <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3448,10 +3454,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>153</v>
       </c>
       <c r="B106" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3468,10 +3474,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3488,19 +3494,19 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C108">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -3508,19 +3514,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>157</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3528,87 +3534,87 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
       </c>
       <c r="C110">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
       </c>
       <c r="C111">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="D111">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E111">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F111">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>169</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>558</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
@@ -3628,10 +3634,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3648,7 +3654,7 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
@@ -3668,27 +3674,27 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
       </c>
       <c r="C117">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -3708,27 +3714,27 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
@@ -3748,10 +3754,10 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -3768,10 +3774,10 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -3788,10 +3794,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3808,19 +3814,19 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
         <v>8</v>
       </c>
       <c r="C124">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E124">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F124">
         <v>0</v>
@@ -3828,7 +3834,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -3848,19 +3854,19 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
         <v>8</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F126">
         <v>0</v>
@@ -3868,7 +3874,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
@@ -3888,19 +3894,19 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
         <v>8</v>
       </c>
       <c r="C128">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E128">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F128">
         <v>0</v>
@@ -3908,10 +3914,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -3928,19 +3934,19 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>127</v>
+        <v>152</v>
       </c>
       <c r="B130" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F130">
         <v>0</v>
@@ -3948,30 +3954,30 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C131">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B132" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -3988,50 +3994,50 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B133" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C134">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D134">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F134">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4048,13 +4054,13 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>133</v>
+        <v>166</v>
       </c>
       <c r="B136" t="s">
         <v>25</v>
       </c>
       <c r="C136">
-        <v>205</v>
+        <v>133</v>
       </c>
       <c r="D136">
         <v>3</v>
@@ -4063,15 +4069,15 @@
         <v>4</v>
       </c>
       <c r="F136">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B137" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -4088,30 +4094,30 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="C138">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D138">
+        <v>3</v>
+      </c>
+      <c r="E138">
         <v>4</v>
       </c>
-      <c r="E138">
-        <v>22</v>
-      </c>
       <c r="F138">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B139" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -4128,59 +4134,59 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B140" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="D140">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E140">
+        <v>22</v>
+      </c>
+      <c r="F140">
         <v>7</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C141">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E141">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F141">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>137</v>
+        <v>151</v>
       </c>
       <c r="B142" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -4188,27 +4194,27 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="B143" t="s">
         <v>6</v>
       </c>
       <c r="C143">
-        <v>826</v>
+        <v>127</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E143">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F143">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B144" t="s">
         <v>10</v>
@@ -4228,30 +4234,30 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B145" t="s">
         <v>6</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F145">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B146" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C146">
         <v>0</v>
@@ -4268,10 +4274,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B147" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -4288,30 +4294,30 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B148" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C148">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D148">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E148">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F148">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="B149" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -4328,50 +4334,50 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="B150" t="s">
         <v>6</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F150">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C151">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D151">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E151">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F151">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B152" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -4388,30 +4394,30 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B153" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B154" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -4428,30 +4434,30 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C155">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D155">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E155">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F155">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B156" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4468,41 +4474,81 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B157" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D157">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
+        <v>149</v>
+      </c>
+      <c r="B158" t="s">
+        <v>10</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+      <c r="F158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>155</v>
+      </c>
+      <c r="B159" t="s">
+        <v>10</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>164</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B160" t="s">
         <v>25</v>
       </c>
-      <c r="C158">
+      <c r="C160">
         <v>59</v>
       </c>
-      <c r="D158">
+      <c r="D160">
         <v>10</v>
       </c>
-      <c r="E158">
+      <c r="E160">
         <v>4</v>
       </c>
-      <c r="F158">
+      <c r="F160">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified a couple of the style sheets
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="171">
   <si>
     <t>IngredientName</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Grocery</t>
   </si>
   <si>
-    <t>apple</t>
-  </si>
-  <si>
     <t>Vegetable</t>
   </si>
   <si>
@@ -529,6 +526,12 @@
   </si>
   <si>
     <t>peanut butter</t>
+  </si>
+  <si>
+    <t>dessicated coconut</t>
+  </si>
+  <si>
+    <t>apples</t>
   </si>
 </sst>
 </file>
@@ -1335,11 +1338,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H113" sqref="H113"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1363,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1394,10 +1397,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
       </c>
       <c r="C3">
         <v>52</v>
@@ -1414,10 +1417,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1434,10 +1437,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>25</v>
@@ -1454,10 +1457,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
       <c r="C6">
         <v>548</v>
@@ -1474,7 +1477,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -1494,10 +1497,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <v>136</v>
@@ -1514,10 +1517,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1534,10 +1537,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1554,10 +1557,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11">
         <v>90</v>
@@ -1574,10 +1577,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <v>77</v>
@@ -1594,10 +1597,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
         <v>20</v>
-      </c>
-      <c r="B13" t="s">
-        <v>21</v>
       </c>
       <c r="C13">
         <v>0</v>
@@ -1614,7 +1617,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1634,10 +1637,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>34</v>
@@ -1654,10 +1657,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <v>295</v>
@@ -1674,10 +1677,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" t="s">
         <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
       </c>
       <c r="C17">
         <v>717</v>
@@ -1694,10 +1697,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>26</v>
@@ -1714,7 +1717,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1734,7 +1737,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1754,7 +1757,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1774,7 +1777,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1794,7 +1797,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -1814,7 +1817,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -1834,7 +1837,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -1854,7 +1857,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1874,7 +1877,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -1894,7 +1897,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1914,7 +1917,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1934,7 +1937,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1954,7 +1957,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -1974,7 +1977,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -1994,7 +1997,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -2014,7 +2017,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -2034,7 +2037,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -2054,10 +2057,10 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -2074,7 +2077,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -2094,10 +2097,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C38">
         <v>0</v>
@@ -2114,10 +2117,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>7</v>
@@ -2134,10 +2137,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40">
         <v>412</v>
@@ -2154,10 +2157,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C41">
         <v>183</v>
@@ -2174,10 +2177,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C42">
         <v>0</v>
@@ -2194,10 +2197,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2214,10 +2217,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -2234,10 +2237,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C45">
         <v>0</v>
@@ -2254,7 +2257,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -2274,7 +2277,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -2294,10 +2297,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2314,10 +2317,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2334,10 +2337,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2354,7 +2357,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -2374,10 +2377,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B52" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2394,10 +2397,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B53" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -2434,10 +2437,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -2474,10 +2477,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57">
         <v>0</v>
@@ -2494,10 +2497,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2514,10 +2517,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C59">
         <v>0</v>
@@ -2534,22 +2537,22 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -2557,7 +2560,7 @@
         <v>62</v>
       </c>
       <c r="B61" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C61">
         <v>0</v>
@@ -2574,47 +2577,47 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C62">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E62">
         <v>0</v>
       </c>
       <c r="F62">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E63">
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -2634,10 +2637,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2654,10 +2657,10 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C66">
         <v>0</v>
@@ -2677,7 +2680,7 @@
         <v>68</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C67">
         <v>0</v>
@@ -2694,10 +2697,10 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2717,7 +2720,7 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2734,10 +2737,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2754,10 +2757,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2774,50 +2777,50 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C72">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2834,10 +2837,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2854,10 +2857,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2874,10 +2877,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C77">
         <v>0</v>
@@ -2894,10 +2897,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2914,10 +2917,10 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>159</v>
+        <v>80</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2934,10 +2937,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>158</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2954,10 +2957,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -2974,110 +2977,110 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C82">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>154</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C84">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E84">
         <v>0</v>
       </c>
       <c r="F84">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>153</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C85">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D85">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E85">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C87">
         <v>0</v>
@@ -3094,10 +3097,10 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C88">
         <v>0</v>
@@ -3114,10 +3117,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -3134,70 +3137,70 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C91">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D91">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E91">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C93">
         <v>0</v>
@@ -3214,10 +3217,10 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3234,10 +3237,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3254,10 +3257,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3274,10 +3277,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3294,10 +3297,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3314,59 +3317,59 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
       </c>
       <c r="C99">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C100">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E100">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D101">
         <v>0</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -3374,10 +3377,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3394,19 +3397,19 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C103">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -3414,19 +3417,19 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -3434,10 +3437,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3454,10 +3457,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3474,10 +3477,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>152</v>
       </c>
       <c r="B107" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3494,10 +3497,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3514,19 +3517,19 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>157</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C109">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3534,19 +3537,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3554,90 +3557,90 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
       </c>
       <c r="C111">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E111">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>169</v>
+        <v>108</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
       </c>
       <c r="C112">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D112">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E112">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F112">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="C113">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D113">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E113">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F113">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B115" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3654,10 +3657,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3674,7 +3677,7 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
@@ -3714,47 +3717,47 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
@@ -3774,7 +3777,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -3794,10 +3797,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B123" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3814,10 +3817,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B124" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3834,10 +3837,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -3854,19 +3857,19 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B126" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C126">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F126">
         <v>0</v>
@@ -3874,19 +3877,19 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B127" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F127">
         <v>0</v>
@@ -3894,10 +3897,10 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B128" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C128">
         <v>0</v>
@@ -3914,10 +3917,10 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B129" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C129">
         <v>0</v>
@@ -3934,19 +3937,19 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>152</v>
+        <v>130</v>
       </c>
       <c r="B130" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C130">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E130">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F130">
         <v>0</v>
@@ -3954,19 +3957,19 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B131" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -3974,10 +3977,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B132" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -3994,50 +3997,50 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C133">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E133">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B134" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>330</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4054,139 +4057,139 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>166</v>
+        <v>129</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C136">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E136">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F136">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="B137" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B138" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C138">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E138">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F138">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B139" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B140" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C140">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E140">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F140">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B141" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B142" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C142">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E142">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -4194,90 +4197,90 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C143">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D143">
         <v>2</v>
       </c>
       <c r="E143">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F143">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="B144" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F144">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B145" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B146" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D146">
         <v>0</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -4294,10 +4297,10 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B148" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -4314,10 +4317,10 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B149" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -4334,50 +4337,50 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C150">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D150">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B151" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>145</v>
+        <v>155</v>
       </c>
       <c r="B152" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -4394,50 +4397,50 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B153" t="s">
         <v>6</v>
       </c>
       <c r="C153">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D153">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E153">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F153">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B154" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B155" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -4454,10 +4457,10 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B156" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4474,50 +4477,50 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C157">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D157">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E157">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F157">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B158" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C158">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D158">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E158">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -4534,21 +4537,41 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B160" t="s">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>163</v>
+      </c>
+      <c r="B161" t="s">
+        <v>24</v>
+      </c>
+      <c r="C161">
         <v>59</v>
       </c>
-      <c r="D160">
+      <c r="D161">
         <v>10</v>
       </c>
-      <c r="E160">
+      <c r="E161">
         <v>4</v>
       </c>
-      <c r="F160">
+      <c r="F161">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a kind of Woolton pie
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="174">
   <si>
     <t>IngredientName</t>
   </si>
@@ -532,6 +532,15 @@
   </si>
   <si>
     <t>apples</t>
+  </si>
+  <si>
+    <t>plain flour</t>
+  </si>
+  <si>
+    <t>whole grain mustard</t>
+  </si>
+  <si>
+    <t>gravy granules</t>
   </si>
 </sst>
 </file>
@@ -1338,11 +1347,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B73" sqref="B73:F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2797,50 +2806,50 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>173</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2857,10 +2866,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2877,7 +2886,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
@@ -2897,7 +2906,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
@@ -2917,7 +2926,7 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
@@ -2937,7 +2946,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>80</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
@@ -2957,7 +2966,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>158</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
@@ -2977,7 +2986,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -2997,107 +3006,107 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C83">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>153</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C85">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C86">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D86">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E86">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -3117,10 +3126,10 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C89">
         <v>0</v>
@@ -3137,10 +3146,10 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C90">
         <v>0</v>
@@ -3157,70 +3166,70 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C92">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D92">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E92">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C94">
         <v>0</v>
@@ -3237,7 +3246,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
@@ -3257,10 +3266,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3277,10 +3286,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3297,7 +3306,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
@@ -3317,10 +3326,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C99">
         <v>0</v>
@@ -3337,59 +3346,59 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
       </c>
       <c r="C100">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C101">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E101">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -3397,10 +3406,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3417,19 +3426,19 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C104">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F104">
         <v>0</v>
@@ -3437,19 +3446,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -3457,10 +3466,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3477,10 +3486,10 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3497,10 +3506,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>105</v>
+        <v>152</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C108">
         <v>0</v>
@@ -3517,10 +3526,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3537,19 +3546,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C110">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3557,19 +3566,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>107</v>
+        <v>156</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3577,90 +3586,90 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
       </c>
       <c r="C112">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="C113">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D113">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E113">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F113">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
       </c>
       <c r="C114">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D114">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E114">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F114">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3677,10 +3686,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -3697,7 +3706,7 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -3717,7 +3726,7 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -3737,47 +3746,47 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -3797,7 +3806,7 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -3817,10 +3826,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B124" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3837,30 +3846,30 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E125">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -3877,19 +3886,19 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B127" t="s">
         <v>7</v>
       </c>
       <c r="C127">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E127">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F127">
         <v>0</v>
@@ -3897,7 +3906,7 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -3917,19 +3926,19 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B129" t="s">
         <v>7</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F129">
         <v>0</v>
@@ -3937,7 +3946,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -3957,19 +3966,19 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="B131" t="s">
         <v>7</v>
       </c>
       <c r="C131">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F131">
         <v>0</v>
@@ -3977,10 +3986,10 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -3997,19 +4006,19 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="B133" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F133">
         <v>0</v>
@@ -4017,30 +4026,30 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C134">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D134">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F134">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B135" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4057,50 +4066,50 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <v>330</v>
+      </c>
+      <c r="D136">
         <v>9</v>
       </c>
-      <c r="C136">
-        <v>0</v>
-      </c>
-      <c r="D136">
-        <v>0</v>
-      </c>
       <c r="E136">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F136">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="B137" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C137">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D137">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E137">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F137">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B138" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -4117,13 +4126,13 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>132</v>
+        <v>165</v>
       </c>
       <c r="B139" t="s">
         <v>24</v>
       </c>
       <c r="C139">
-        <v>205</v>
+        <v>133</v>
       </c>
       <c r="D139">
         <v>3</v>
@@ -4132,15 +4141,15 @@
         <v>4</v>
       </c>
       <c r="F139">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B140" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -4157,30 +4166,30 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C141">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D141">
+        <v>3</v>
+      </c>
+      <c r="E141">
         <v>4</v>
       </c>
-      <c r="E141">
-        <v>22</v>
-      </c>
       <c r="F141">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B142" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -4197,59 +4206,59 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>104</v>
+      </c>
+      <c r="D143">
+        <v>4</v>
+      </c>
+      <c r="E143">
+        <v>22</v>
+      </c>
+      <c r="F143">
         <v>7</v>
-      </c>
-      <c r="C143">
-        <v>32</v>
-      </c>
-      <c r="D143">
-        <v>2</v>
-      </c>
-      <c r="E143">
-        <v>7</v>
-      </c>
-      <c r="F143">
-        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="B144" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C144">
-        <v>127</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F144">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="B145" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F145">
         <v>0</v>
@@ -4257,27 +4266,27 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>137</v>
+        <v>164</v>
       </c>
       <c r="B146" t="s">
         <v>6</v>
       </c>
       <c r="C146">
-        <v>826</v>
+        <v>127</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F146">
-        <v>87</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B147" t="s">
         <v>9</v>
@@ -4297,30 +4306,30 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B148" t="s">
         <v>6</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D148">
         <v>0</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B149" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C149">
         <v>0</v>
@@ -4337,10 +4346,10 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B150" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -4357,30 +4366,30 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C151">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D151">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E151">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F151">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C152">
         <v>0</v>
@@ -4397,50 +4406,50 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="B153" t="s">
         <v>6</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C154">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D154">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E154">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B155" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C155">
         <v>0</v>
@@ -4457,30 +4466,30 @@
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B156" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D156">
-        <v>0</v>
+        <v>4.5</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F156">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B157" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -4497,30 +4506,30 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C158">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D158">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E158">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F158">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B159" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -4537,41 +4546,101 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B160" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F160">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
+        <v>172</v>
+      </c>
+      <c r="B161" t="s">
+        <v>6</v>
+      </c>
+      <c r="C161">
+        <v>150</v>
+      </c>
+      <c r="D161">
+        <v>8</v>
+      </c>
+      <c r="E161">
+        <v>8</v>
+      </c>
+      <c r="F161">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>148</v>
+      </c>
+      <c r="B162" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>154</v>
+      </c>
+      <c r="B163" t="s">
+        <v>9</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+      <c r="F163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
         <v>163</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B164" t="s">
         <v>24</v>
       </c>
-      <c r="C161">
+      <c r="C164">
         <v>59</v>
       </c>
-      <c r="D161">
+      <c r="D164">
         <v>10</v>
       </c>
-      <c r="E161">
+      <c r="E164">
         <v>4</v>
       </c>
-      <c r="F161">
+      <c r="F164">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Staples aren't halving for the quick meals.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="182">
   <si>
     <t>IngredientName</t>
   </si>
@@ -562,6 +562,9 @@
   </si>
   <si>
     <t>bread</t>
+  </si>
+  <si>
+    <t>ham</t>
   </si>
 </sst>
 </file>
@@ -1369,11 +1372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G170"/>
+  <dimension ref="A1:G171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I26" sqref="I26"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L88" sqref="L88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3115,139 +3118,139 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C88">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B89" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="B90" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C90">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E90">
         <v>0</v>
       </c>
       <c r="F90">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C91">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D91">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E91">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="B92" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C92">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D92">
+        <v>13</v>
+      </c>
+      <c r="E92">
+        <v>70</v>
+      </c>
+      <c r="F92">
         <v>2</v>
-      </c>
-      <c r="E92">
-        <v>14</v>
-      </c>
-      <c r="F92">
-        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="B93" t="s">
         <v>7</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F93">
         <v>0</v>
@@ -3255,7 +3258,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
@@ -3275,10 +3278,10 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B95" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C95">
         <v>0</v>
@@ -3295,10 +3298,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3315,70 +3318,70 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C97">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D97">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E97">
         <v>0</v>
       </c>
       <c r="F97">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B98" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C98">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D98">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E98">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C100">
         <v>0</v>
@@ -3395,7 +3398,7 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
@@ -3415,10 +3418,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3435,10 +3438,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3455,7 +3458,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
@@ -3475,10 +3478,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3495,59 +3498,59 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
       </c>
       <c r="C106">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C107">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E107">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F108">
         <v>0</v>
@@ -3555,10 +3558,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B109" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3575,19 +3578,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C110">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3595,19 +3598,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B111" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3615,10 +3618,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -3635,10 +3638,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3655,10 +3658,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3675,10 +3678,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B115" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3695,19 +3698,19 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -3715,19 +3718,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -3735,90 +3738,90 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
       </c>
       <c r="C118">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E118">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F118">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D119">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E119">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F119">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D120">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E120">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F120">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B122" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -3835,10 +3838,10 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3855,7 +3858,7 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
@@ -3875,7 +3878,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -3895,47 +3898,47 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
       <c r="C126">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
@@ -3955,7 +3958,7 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -3975,50 +3978,50 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
       </c>
       <c r="C130">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E130">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F130">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B131" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B132" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -4035,10 +4038,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -4055,19 +4058,19 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C134">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D134">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F134">
         <v>0</v>
@@ -4075,19 +4078,19 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -4095,10 +4098,10 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C136">
         <v>0</v>
@@ -4115,10 +4118,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -4135,19 +4138,19 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C138">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E138">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F138">
         <v>0</v>
@@ -4155,19 +4158,19 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B139" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F139">
         <v>0</v>
@@ -4175,10 +4178,10 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B140" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -4195,47 +4198,47 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B141" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C141">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E141">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F141">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142">
+        <v>330</v>
+      </c>
+      <c r="D142">
         <v>9</v>
       </c>
-      <c r="C142">
-        <v>0</v>
-      </c>
-      <c r="D142">
-        <v>0</v>
-      </c>
       <c r="E142">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F142">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B143" t="s">
         <v>9</v>
@@ -4255,139 +4258,139 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B144" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C144">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F144">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B145" t="s">
         <v>24</v>
       </c>
       <c r="C145">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E145">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F145">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B146" t="s">
         <v>24</v>
       </c>
       <c r="C146">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D146">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E146">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F146">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B148" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C148">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D148">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E148">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F148">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>104</v>
+      </c>
+      <c r="D149">
+        <v>4</v>
+      </c>
+      <c r="E149">
+        <v>22</v>
+      </c>
+      <c r="F149">
         <v>7</v>
-      </c>
-      <c r="C149">
-        <v>23</v>
-      </c>
-      <c r="D149">
-        <v>3</v>
-      </c>
-      <c r="E149">
-        <v>4</v>
-      </c>
-      <c r="F149">
-        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="B150" t="s">
         <v>7</v>
       </c>
       <c r="C150">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E150">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F150">
         <v>0</v>
@@ -4395,19 +4398,19 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
       </c>
       <c r="C151">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D151">
         <v>2</v>
       </c>
       <c r="E151">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F151">
         <v>0</v>
@@ -4415,90 +4418,90 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B152" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C152">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D152">
         <v>2</v>
       </c>
       <c r="E152">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F152">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B153" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C153">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F153">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C154">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="E154">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B155" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4515,10 +4518,10 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B157" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -4535,7 +4538,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -4555,50 +4558,50 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C159">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D159">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E159">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F159">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B160" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C160">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D160">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E160">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F160">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C161">
         <v>0</v>
@@ -4615,19 +4618,19 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B162" t="s">
         <v>6</v>
       </c>
       <c r="C162">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D162">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E162">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F162">
         <v>0</v>
@@ -4635,19 +4638,19 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B163" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -4655,10 +4658,10 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -4675,10 +4678,10 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="B165" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -4691,74 +4694,74 @@
       </c>
       <c r="F165">
         <v>0</v>
-      </c>
-      <c r="G165" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>146</v>
+        <v>178</v>
       </c>
       <c r="B166" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C166">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D166">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E166">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="B167" t="s">
         <v>6</v>
       </c>
       <c r="C167">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D167">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E167">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="F167">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B168" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E168">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B169" t="s">
         <v>9</v>
@@ -4778,21 +4781,41 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
+        <v>153</v>
+      </c>
+      <c r="B170" t="s">
+        <v>9</v>
+      </c>
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>162</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B171" t="s">
         <v>24</v>
       </c>
-      <c r="C170">
+      <c r="C171">
         <v>59</v>
       </c>
-      <c r="D170">
+      <c r="D171">
         <v>10</v>
       </c>
-      <c r="E170">
+      <c r="E171">
         <v>4</v>
       </c>
-      <c r="F170">
+      <c r="F171">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ridiculously inefficient way of getting the calories for the ingredients.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$174</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="185">
   <si>
     <t>IngredientName</t>
   </si>
@@ -565,6 +568,15 @@
   </si>
   <si>
     <t>ham</t>
+  </si>
+  <si>
+    <t>tagliatelli</t>
+  </si>
+  <si>
+    <t>brown rice</t>
+  </si>
+  <si>
+    <t>tortellini</t>
   </si>
 </sst>
 </file>
@@ -1372,11 +1384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L88" sqref="L88"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H170" sqref="H170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,119 +1770,119 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>295</v>
+        <v>111</v>
       </c>
       <c r="D19">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F19">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20">
+        <v>295</v>
+      </c>
+      <c r="D20">
+        <v>17</v>
+      </c>
+      <c r="E20">
         <v>24</v>
       </c>
-      <c r="C20">
-        <v>717</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
       <c r="F20">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C21">
-        <v>26</v>
+        <v>717</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22">
-        <v>155</v>
-      </c>
       <c r="D22">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="D23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
       <c r="C24">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D24">
         <v>7</v>
       </c>
       <c r="E24">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1878,27 +1890,27 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1918,47 +1930,47 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>160</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>160</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -1978,7 +1990,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -1998,59 +2010,59 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>161</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
       </c>
       <c r="C31">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E32">
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E33">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2058,19 +2070,19 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -2078,7 +2090,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -2098,19 +2110,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2118,19 +2130,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -2138,7 +2150,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -2158,19 +2170,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C39">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2178,19 +2190,19 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -2198,10 +2210,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>0</v>
@@ -2218,19 +2230,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2238,70 +2250,70 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>412</v>
+        <v>7</v>
       </c>
       <c r="D43">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C44">
-        <v>183</v>
+        <v>412</v>
       </c>
       <c r="D44">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <v>0</v>
@@ -2318,7 +2330,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -2338,10 +2350,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2358,10 +2370,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2378,7 +2390,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -2398,10 +2410,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2418,7 +2430,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
@@ -2438,10 +2450,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2458,50 +2470,50 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C54">
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C56">
         <v>0</v>
@@ -2518,19 +2530,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C57">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -2538,19 +2550,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -2558,22 +2570,22 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C59">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -2581,24 +2593,24 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -2618,7 +2630,7 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
@@ -2638,50 +2650,50 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>168</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C63">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>0</v>
@@ -2698,47 +2710,47 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E67">
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -2758,10 +2770,10 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B69" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C69">
         <v>0</v>
@@ -2778,10 +2790,10 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C70">
         <v>0</v>
@@ -2798,10 +2810,10 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C71">
         <v>0</v>
@@ -2818,10 +2830,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2838,10 +2850,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2858,7 +2870,7 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -2878,10 +2890,10 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2898,7 +2910,7 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>172</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -2918,50 +2930,50 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C79">
         <v>0</v>
@@ -2978,10 +2990,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>179</v>
+        <v>75</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C80">
         <v>0</v>
@@ -2998,7 +3010,7 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
@@ -3018,7 +3030,7 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
@@ -3038,7 +3050,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -3058,7 +3070,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -3078,7 +3090,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3098,7 +3110,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -3118,159 +3130,159 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="B87" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C87">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C89">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B90" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="B91" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C91">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C92">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D92">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E92">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="B93" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D93">
+        <v>13</v>
+      </c>
+      <c r="E93">
+        <v>70</v>
+      </c>
+      <c r="F93">
         <v>2</v>
-      </c>
-      <c r="E93">
-        <v>14</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="B94" t="s">
         <v>7</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F94">
         <v>0</v>
@@ -3278,7 +3290,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
@@ -3298,10 +3310,10 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3318,10 +3330,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3338,70 +3350,70 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B98" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C98">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E98">
         <v>0</v>
       </c>
       <c r="F98">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C99">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D99">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E99">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B100" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C101">
         <v>0</v>
@@ -3418,7 +3430,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
@@ -3438,10 +3450,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B103" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3458,10 +3470,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3478,7 +3490,7 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
@@ -3498,10 +3510,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B106" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C106">
         <v>0</v>
@@ -3518,59 +3530,59 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
       </c>
       <c r="C107">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B108" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C108">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E108">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B109" t="s">
         <v>9</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D109">
         <v>0</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3578,10 +3590,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3598,19 +3610,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B111" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C111">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F111">
         <v>0</v>
@@ -3618,19 +3630,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B112" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -3638,10 +3650,10 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3658,10 +3670,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3678,10 +3690,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="B115" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3698,10 +3710,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3718,19 +3730,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C117">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F117">
         <v>0</v>
@@ -3738,19 +3750,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -3758,90 +3770,90 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D120">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E120">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F120">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D121">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E121">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F121">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B123" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3858,10 +3870,10 @@
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3878,7 +3890,7 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -3898,7 +3910,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -3918,47 +3930,47 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E127">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F127">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
@@ -3978,7 +3990,7 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -3998,50 +4010,50 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
       </c>
       <c r="C131">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B132" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B133" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -4058,10 +4070,10 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -4078,19 +4090,19 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B135" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C135">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -4098,19 +4110,19 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B136" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C136">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E136">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F136">
         <v>0</v>
@@ -4118,10 +4130,10 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C137">
         <v>0</v>
@@ -4138,10 +4150,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -4158,19 +4170,19 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B139" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C139">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E139">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F139">
         <v>0</v>
@@ -4178,19 +4190,19 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B140" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F140">
         <v>0</v>
@@ -4198,10 +4210,10 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B141" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C141">
         <v>0</v>
@@ -4218,47 +4230,47 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C142">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E142">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F142">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>330</v>
+      </c>
+      <c r="D143">
         <v>9</v>
       </c>
-      <c r="C143">
-        <v>0</v>
-      </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
       <c r="E143">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B144" t="s">
         <v>9</v>
@@ -4278,139 +4290,139 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B145" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C145">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E145">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F145">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B146" t="s">
         <v>24</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B147" t="s">
         <v>24</v>
       </c>
       <c r="C147">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D147">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E147">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F147">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F148">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C149">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D149">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E149">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F149">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B150" t="s">
+        <v>6</v>
+      </c>
+      <c r="C150">
+        <v>104</v>
+      </c>
+      <c r="D150">
+        <v>4</v>
+      </c>
+      <c r="E150">
+        <v>22</v>
+      </c>
+      <c r="F150">
         <v>7</v>
-      </c>
-      <c r="C150">
-        <v>23</v>
-      </c>
-      <c r="D150">
-        <v>3</v>
-      </c>
-      <c r="E150">
-        <v>4</v>
-      </c>
-      <c r="F150">
-        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="B151" t="s">
         <v>7</v>
       </c>
       <c r="C151">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D151">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E151">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F151">
         <v>0</v>
@@ -4418,19 +4430,19 @@
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
       </c>
       <c r="C152">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D152">
         <v>2</v>
       </c>
       <c r="E152">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F152">
         <v>0</v>
@@ -4438,90 +4450,90 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C153">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D153">
         <v>2</v>
       </c>
       <c r="E153">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F153">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B154" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C155">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F155">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B156" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C156">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F156">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C157">
         <v>0</v>
@@ -4538,10 +4550,10 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B158" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -4558,7 +4570,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
@@ -4578,90 +4590,93 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C160">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D160">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E160">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F160">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="B161" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>288</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F161">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B162" t="s">
         <v>6</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E162">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F162">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>142</v>
+        <v>178</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C163">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D163">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E163">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F163">
         <v>0</v>
+      </c>
+      <c r="G163" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="B164" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -4678,10 +4693,10 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B165" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -4698,70 +4713,67 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="B166" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F166">
         <v>0</v>
-      </c>
-      <c r="G166" s="1">
-        <v>1</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>138</v>
+        <v>0</v>
       </c>
       <c r="D167">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E167">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="F167">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="B168" t="s">
         <v>6</v>
       </c>
       <c r="C168">
-        <v>150</v>
+        <v>307</v>
       </c>
       <c r="D168">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E168">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="F168">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B169" t="s">
         <v>9</v>
@@ -4781,47 +4793,108 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="B170" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>138</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E170">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="F170">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>171</v>
+      </c>
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>150</v>
+      </c>
+      <c r="D171">
+        <v>8</v>
+      </c>
+      <c r="E171">
+        <v>8</v>
+      </c>
+      <c r="F171">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>147</v>
+      </c>
+      <c r="B172" t="s">
+        <v>9</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>153</v>
+      </c>
+      <c r="B173" t="s">
+        <v>9</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>162</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B174" t="s">
         <v>24</v>
       </c>
-      <c r="C171">
+      <c r="C174">
         <v>59</v>
       </c>
-      <c r="D171">
+      <c r="D174">
         <v>10</v>
       </c>
-      <c r="E171">
+      <c r="E174">
         <v>4</v>
       </c>
-      <c r="F171">
+      <c r="F174">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F156">
-    <sortCondition ref="A2:A156"/>
+  <autoFilter ref="A2:G174"/>
+  <sortState ref="A2:G173">
+    <sortCondition ref="A2:A173"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Renamed Type to Name for consistency
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -1387,8 +1387,8 @@
   <dimension ref="A1:G174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E164" sqref="E164"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G2:G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1704,9 +1704,6 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">

</xml_diff>

<commit_message>
Egg stir fried rice.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$174</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$175</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="186">
   <si>
     <t>IngredientName</t>
   </si>
@@ -577,6 +577,9 @@
   </si>
   <si>
     <t>tortellini</t>
+  </si>
+  <si>
+    <t>ground cloves</t>
   </si>
 </sst>
 </file>
@@ -1384,11 +1387,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G174"/>
+  <dimension ref="A1:G175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G40" sqref="G2:G40"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83:F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3050,7 +3053,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>77</v>
+        <v>185</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -3070,7 +3073,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -3090,7 +3093,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3110,7 +3113,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>157</v>
+        <v>80</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -3130,7 +3133,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>79</v>
+        <v>157</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -3150,159 +3153,159 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>181</v>
+        <v>79</v>
       </c>
       <c r="B88" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C88">
-        <v>145</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>21</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>81</v>
+        <v>181</v>
       </c>
       <c r="B89" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C90">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B91" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>152</v>
+        <v>83</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C92">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>84</v>
+        <v>152</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D93">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E93">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>84</v>
       </c>
       <c r="B94" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C94">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D94">
+        <v>13</v>
+      </c>
+      <c r="E94">
+        <v>70</v>
+      </c>
+      <c r="F94">
         <v>2</v>
-      </c>
-      <c r="E94">
-        <v>14</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>85</v>
+        <v>174</v>
       </c>
       <c r="B95" t="s">
         <v>7</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F95">
         <v>0</v>
@@ -3310,7 +3313,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B96" t="s">
         <v>7</v>
@@ -3330,10 +3333,10 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B97" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C97">
         <v>0</v>
@@ -3350,10 +3353,10 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C98">
         <v>0</v>
@@ -3370,70 +3373,70 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B99" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C99">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B100" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C100">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D100">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E100">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B101" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3450,7 +3453,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
@@ -3470,10 +3473,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3490,10 +3493,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C105">
         <v>0</v>
@@ -3510,7 +3513,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
@@ -3530,10 +3533,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3550,76 +3553,73 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
       </c>
       <c r="C108">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>899</v>
+        <v>62</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E109">
-        <v>99</v>
+        <v>13</v>
       </c>
       <c r="F109">
-        <v>0</v>
-      </c>
-      <c r="G109" s="1">
-        <v>0.93</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D110">
         <v>0</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F110">
         <v>0</v>
       </c>
       <c r="G110" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -3632,23 +3632,26 @@
       </c>
       <c r="F111">
         <v>0</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0.92</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B112" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C112">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -3656,19 +3659,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B113" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -3676,10 +3679,10 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -3696,10 +3699,10 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>151</v>
+        <v>104</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3716,10 +3719,10 @@
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>105</v>
+        <v>151</v>
       </c>
       <c r="B116" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C116">
         <v>0</v>
@@ -3736,10 +3739,10 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -3756,19 +3759,19 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>155</v>
+        <v>106</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C118">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E118">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -3776,19 +3779,19 @@
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -3796,90 +3799,90 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D121">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E121">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F121">
-        <v>50</v>
+        <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
       </c>
       <c r="C122">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D122">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E122">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F122">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3896,10 +3899,10 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -3916,7 +3919,7 @@
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
@@ -3936,7 +3939,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
@@ -3956,47 +3959,47 @@
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
       </c>
       <c r="C128">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E128">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F128">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -4016,7 +4019,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B131" t="s">
         <v>6</v>
@@ -4036,50 +4039,50 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
       </c>
       <c r="C132">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E132">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F132">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
       <c r="B133" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>364</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>86</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B134" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -4096,19 +4099,19 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C135">
-        <v>299</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="F135">
         <v>0</v>
@@ -4116,19 +4119,19 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B136" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C136">
-        <v>26</v>
+        <v>299</v>
       </c>
       <c r="D136">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E136">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="F136">
         <v>0</v>
@@ -4136,19 +4139,19 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B137" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F137">
         <v>0</v>
@@ -4156,10 +4159,10 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -4176,10 +4179,10 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B139" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -4196,19 +4199,19 @@
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>150</v>
+        <v>130</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C140">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E140">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F140">
         <v>0</v>
@@ -4216,19 +4219,19 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B141" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -4236,10 +4239,10 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B142" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C142">
         <v>0</v>
@@ -4256,47 +4259,47 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C143">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D143">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E143">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F143">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <v>330</v>
+      </c>
+      <c r="D144">
         <v>9</v>
       </c>
-      <c r="C144">
-        <v>0</v>
-      </c>
-      <c r="D144">
-        <v>0</v>
-      </c>
       <c r="E144">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F144">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B145" t="s">
         <v>9</v>
@@ -4316,139 +4319,139 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="B146" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C146">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D146">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E146">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F146">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>131</v>
+        <v>164</v>
       </c>
       <c r="B147" t="s">
         <v>24</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B148" t="s">
         <v>24</v>
       </c>
       <c r="C148">
-        <v>205</v>
+        <v>0</v>
       </c>
       <c r="D148">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E148">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F148">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B149" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F149">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C150">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="D150">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>104</v>
+      </c>
+      <c r="D151">
+        <v>4</v>
+      </c>
+      <c r="E151">
+        <v>22</v>
+      </c>
+      <c r="F151">
         <v>7</v>
-      </c>
-      <c r="C151">
-        <v>23</v>
-      </c>
-      <c r="D151">
-        <v>3</v>
-      </c>
-      <c r="E151">
-        <v>4</v>
-      </c>
-      <c r="F151">
-        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="B152" t="s">
         <v>7</v>
       </c>
       <c r="C152">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D152">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E152">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F152">
         <v>0</v>
@@ -4456,19 +4459,19 @@
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>149</v>
+        <v>175</v>
       </c>
       <c r="B153" t="s">
         <v>7</v>
       </c>
       <c r="C153">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D153">
         <v>2</v>
       </c>
       <c r="E153">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F153">
         <v>0</v>
@@ -4476,90 +4479,90 @@
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C154">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D154">
         <v>2</v>
       </c>
       <c r="E154">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F154">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B155" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C155">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D155">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E155">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C156">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F156">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B157" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C157">
-        <v>0</v>
+        <v>826</v>
       </c>
       <c r="D157">
         <v>0</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>87</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C158">
         <v>0</v>
@@ -4576,10 +4579,10 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B159" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C159">
         <v>0</v>
@@ -4596,7 +4599,7 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B160" t="s">
         <v>7</v>
@@ -4616,73 +4619,70 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>182</v>
+        <v>141</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C161">
-        <v>371</v>
+        <v>0</v>
       </c>
       <c r="D161">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E161">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="F161">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>156</v>
+        <v>182</v>
       </c>
       <c r="B162" t="s">
         <v>6</v>
       </c>
       <c r="C162">
-        <v>595</v>
+        <v>371</v>
       </c>
       <c r="D162">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E162">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F162">
-        <v>54</v>
+        <v>2</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B163" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F163">
-        <v>0</v>
-      </c>
-      <c r="G163" s="1">
-        <v>1</v>
+        <v>54</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>154</v>
+        <v>178</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -4695,14 +4695,17 @@
       </c>
       <c r="F164">
         <v>0</v>
+      </c>
+      <c r="G164" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -4719,19 +4722,19 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B166" t="s">
         <v>6</v>
       </c>
       <c r="C166">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D166">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E166">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F166">
         <v>0</v>
@@ -4739,19 +4742,19 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B167" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D167">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E167">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F167">
         <v>0</v>
@@ -4759,59 +4762,59 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>184</v>
+        <v>143</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C168">
-        <v>307</v>
+        <v>0</v>
       </c>
       <c r="D168">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E168">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="F168">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>145</v>
+        <v>184</v>
       </c>
       <c r="B169" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B170" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C170">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="D170">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E170">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -4819,47 +4822,47 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>171</v>
+        <v>146</v>
       </c>
       <c r="B171" t="s">
         <v>6</v>
       </c>
       <c r="C171">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D171">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E171">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F171">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C172">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F172">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B173" t="s">
         <v>9</v>
@@ -4879,21 +4882,41 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
+        <v>153</v>
+      </c>
+      <c r="B174" t="s">
+        <v>9</v>
+      </c>
+      <c r="C174">
+        <v>0</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174">
+        <v>0</v>
+      </c>
+      <c r="F174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>162</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B175" t="s">
         <v>24</v>
       </c>
-      <c r="C174">
+      <c r="C175">
         <v>59</v>
       </c>
-      <c r="D174">
+      <c r="D175">
         <v>10</v>
       </c>
-      <c r="E174">
+      <c r="E175">
         <v>4</v>
       </c>
-      <c r="F174">
+      <c r="F175">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
A bit of April done.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -1396,8 +1396,8 @@
   <dimension ref="A1:G178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A137" sqref="A137:XFD137"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Just say no to suet
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$177</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="187">
   <si>
     <t>IngredientName</t>
   </si>
@@ -427,9 +427,6 @@
   </si>
   <si>
     <t>stock</t>
-  </si>
-  <si>
-    <t>suet</t>
   </si>
   <si>
     <t>sugar</t>
@@ -1393,11 +1390,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18:XFD18"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A161" sqref="A161:XFD161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1422,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -1431,7 +1428,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1456,7 +1453,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1636,7 +1633,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1656,7 +1653,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
         <v>24</v>
@@ -1716,7 +1713,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -1736,7 +1733,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -1836,7 +1833,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1916,7 +1913,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -1976,7 +1973,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -2056,7 +2053,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -2096,7 +2093,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -2516,7 +2513,7 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -2656,7 +2653,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -2716,7 +2713,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -2979,7 +2976,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -3059,7 +3056,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
@@ -3099,7 +3096,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3179,7 +3176,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -3219,7 +3216,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91" t="s">
         <v>24</v>
@@ -3239,7 +3236,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B92" t="s">
         <v>12</v>
@@ -3319,7 +3316,7 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B96" t="s">
         <v>12</v>
@@ -3359,7 +3356,7 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B98" t="s">
         <v>7</v>
@@ -3785,7 +3782,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B119" t="s">
         <v>9</v>
@@ -3845,7 +3842,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -3905,7 +3902,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
@@ -4125,7 +4122,7 @@
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -4265,7 +4262,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B143" t="s">
         <v>7</v>
@@ -4385,7 +4382,7 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B149" t="s">
         <v>24</v>
@@ -4405,7 +4402,7 @@
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B150" t="s">
         <v>12</v>
@@ -4505,7 +4502,7 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B155" t="s">
         <v>6</v>
@@ -4545,7 +4542,7 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B157" t="s">
         <v>7</v>
@@ -4565,7 +4562,7 @@
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B158" t="s">
         <v>7</v>
@@ -4585,7 +4582,7 @@
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B159" t="s">
         <v>6</v>
@@ -4628,19 +4625,19 @@
         <v>135</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C161">
-        <v>826</v>
+        <v>0</v>
       </c>
       <c r="D161">
         <v>0</v>
       </c>
       <c r="E161">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F161">
-        <v>87</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
@@ -4648,7 +4645,7 @@
         <v>136</v>
       </c>
       <c r="B162" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C162">
         <v>0</v>
@@ -4668,7 +4665,7 @@
         <v>137</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -4705,70 +4702,70 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="B165" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E165">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F165">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="B166" t="s">
         <v>6</v>
       </c>
       <c r="C166">
-        <v>371</v>
+        <v>595</v>
       </c>
       <c r="D166">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E166">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="F166">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C167">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D167">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E167">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F167">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B168" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C168">
         <v>0</v>
@@ -4785,19 +4782,19 @@
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B169" t="s">
         <v>6</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F169">
         <v>0</v>
@@ -4808,16 +4805,16 @@
         <v>140</v>
       </c>
       <c r="B170" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C170">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D170">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E170">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -4825,42 +4822,42 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>307</v>
+      </c>
+      <c r="D171">
+        <v>14</v>
+      </c>
+      <c r="E171">
+        <v>47</v>
+      </c>
+      <c r="F171">
         <v>7</v>
-      </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-      <c r="D171">
-        <v>0</v>
-      </c>
-      <c r="E171">
-        <v>0</v>
-      </c>
-      <c r="F171">
-        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>181</v>
+        <v>142</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C172">
-        <v>307</v>
+        <v>0</v>
       </c>
       <c r="D172">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="E172">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="F172">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
@@ -4868,16 +4865,16 @@
         <v>143</v>
       </c>
       <c r="B173" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F173">
         <v>0</v>
@@ -4885,47 +4882,47 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
       </c>
       <c r="C174">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D174">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E174">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F174">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B175" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C175">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D175">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E175">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F175">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="B176" t="s">
         <v>9</v>
@@ -4945,41 +4942,21 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="B177" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="D177">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E177">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>160</v>
-      </c>
-      <c r="B178" t="s">
-        <v>24</v>
-      </c>
-      <c r="C178">
-        <v>59</v>
-      </c>
-      <c r="D178">
-        <v>10</v>
-      </c>
-      <c r="E178">
-        <v>4</v>
-      </c>
-      <c r="F178">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Expanding the staples easier to read.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc_d4jqqip\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$180</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="190">
   <si>
     <t>IngredientName</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>lime pickle</t>
+  </si>
+  <si>
+    <t>bulgur wheat</t>
+  </si>
+  <si>
+    <t>new potatoes</t>
   </si>
 </sst>
 </file>
@@ -1393,11 +1399,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H115" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1796,139 +1802,139 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>188</v>
       </c>
       <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20">
+        <v>342</v>
+      </c>
+      <c r="D20">
         <v>12</v>
       </c>
-      <c r="C20">
-        <v>295</v>
-      </c>
-      <c r="D20">
-        <v>17</v>
-      </c>
       <c r="E20">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="F20">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>295</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
+      </c>
+      <c r="E21">
         <v>24</v>
       </c>
-      <c r="C21">
-        <v>717</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
       <c r="F21">
-        <v>81</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>96</v>
+        <v>717</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>185</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23">
-        <v>26</v>
+        <v>96</v>
       </c>
       <c r="D23">
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
         <v>1</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24">
         <v>26</v>
       </c>
-      <c r="B24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24">
-        <v>155</v>
-      </c>
       <c r="D24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
       </c>
       <c r="C25">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="D25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>163</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
       </c>
       <c r="C26">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="D26">
         <v>7</v>
       </c>
       <c r="E26">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1936,27 +1942,27 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>163</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>85</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -1976,47 +1982,47 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>157</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
       </c>
       <c r="C29">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>157</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -2036,7 +2042,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -2056,59 +2062,59 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>158</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
       </c>
       <c r="C33">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E33">
         <v>0</v>
       </c>
       <c r="F33">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>158</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>155</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
       <c r="C35">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2116,19 +2122,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -2136,7 +2142,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -2156,19 +2162,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
       </c>
       <c r="C38">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -2176,19 +2182,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2196,7 +2202,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -2216,19 +2222,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E41">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -2236,19 +2242,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -2256,10 +2262,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -2276,19 +2282,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
         <v>7</v>
       </c>
       <c r="C44">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -2296,70 +2302,70 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>412</v>
+        <v>7</v>
       </c>
       <c r="D45">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F45">
-        <v>34</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C46">
-        <v>183</v>
+        <v>412</v>
       </c>
       <c r="D46">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E46">
         <v>0</v>
       </c>
       <c r="F46">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E47">
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C48">
         <v>0</v>
@@ -2376,7 +2382,7 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -2396,10 +2402,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2416,10 +2422,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C51">
         <v>0</v>
@@ -2436,7 +2442,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -2456,10 +2462,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <v>0</v>
@@ -2476,7 +2482,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
@@ -2496,10 +2502,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2516,50 +2522,50 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>145</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C56">
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="B57" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>395</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C58">
         <v>0</v>
@@ -2576,19 +2582,19 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B59" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C59">
-        <v>176</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2596,19 +2602,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -2616,22 +2622,22 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C61">
-        <v>669</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>69</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -2639,64 +2645,64 @@
         <v>58</v>
       </c>
       <c r="B62" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>669</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>184</v>
+        <v>58</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C63">
-        <v>175</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>184</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
@@ -2716,50 +2722,50 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>165</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C66">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>165</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>354</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C68">
         <v>0</v>
@@ -2776,47 +2782,47 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B69" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B70" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -2836,10 +2842,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B72" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C72">
         <v>0</v>
@@ -2852,17 +2858,14 @@
       </c>
       <c r="F72">
         <v>0</v>
-      </c>
-      <c r="G72" s="1">
-        <v>0.59</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -2875,14 +2878,17 @@
       </c>
       <c r="F73">
         <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0.59</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C74">
         <v>0</v>
@@ -2899,10 +2905,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B75" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C75">
         <v>0</v>
@@ -2919,10 +2925,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B76" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -2939,7 +2945,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2959,10 +2965,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="B78" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C78">
         <v>0</v>
@@ -2979,7 +2985,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -2999,59 +3005,59 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>72</v>
+        <v>169</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B82" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -3059,19 +3065,19 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -3079,7 +3085,7 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
@@ -3099,7 +3105,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>181</v>
+        <v>75</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3119,7 +3125,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -3139,7 +3145,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -3159,7 +3165,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -3179,7 +3185,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -3199,7 +3205,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
@@ -3219,179 +3225,179 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>186</v>
+        <v>78</v>
       </c>
       <c r="B91" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C91">
-        <v>413</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B92" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C92">
-        <v>145</v>
+        <v>413</v>
       </c>
       <c r="D92">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>80</v>
+        <v>177</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B94" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>149</v>
+        <v>82</v>
       </c>
       <c r="B96" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C96">
-        <v>305</v>
+        <v>0</v>
       </c>
       <c r="D96">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>83</v>
+        <v>149</v>
       </c>
       <c r="B97" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C97">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D97">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E97">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>171</v>
+        <v>83</v>
       </c>
       <c r="B98" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C98">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D98">
+        <v>13</v>
+      </c>
+      <c r="E98">
+        <v>70</v>
+      </c>
+      <c r="F98">
         <v>2</v>
-      </c>
-      <c r="E98">
-        <v>14</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>84</v>
+        <v>171</v>
       </c>
       <c r="B99" t="s">
         <v>7</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3399,50 +3405,50 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>187</v>
+        <v>84</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C100">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>85</v>
+        <v>187</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -3459,10 +3465,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B103" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C103">
         <v>0</v>
@@ -3479,70 +3485,70 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B104" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C104">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E104">
         <v>0</v>
       </c>
       <c r="F104">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B105" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C105">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D105">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E105">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>2</v>
+        <v>37</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B106" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C107">
         <v>0</v>
@@ -3559,7 +3565,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
@@ -3579,10 +3585,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B109" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3599,10 +3605,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B110" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3619,7 +3625,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
@@ -3639,10 +3645,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B112" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -3659,116 +3665,116 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="C113">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D113">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E113">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B114" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C114">
-        <v>899</v>
+        <v>75</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E114">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="F114">
         <v>0</v>
-      </c>
-      <c r="G114" s="1">
-        <v>0.93</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B115" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F115">
-        <v>0</v>
-      </c>
-      <c r="G115" s="1">
-        <v>0.92</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B116" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D116">
         <v>0</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F116">
         <v>0</v>
+      </c>
+      <c r="G116" s="1">
+        <v>0.93</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C117">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F117">
         <v>0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>0.92</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C118">
         <v>0</v>
@@ -3785,19 +3791,19 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B119" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F119">
         <v>0</v>
@@ -3805,7 +3811,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B120" t="s">
         <v>9</v>
@@ -3825,10 +3831,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B121" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C121">
         <v>0</v>
@@ -3845,10 +3851,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="B122" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C122">
         <v>0</v>
@@ -3865,19 +3871,19 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="B123" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C123">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F123">
         <v>0</v>
@@ -3885,10 +3891,10 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B124" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3905,107 +3911,107 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
       </c>
       <c r="C125">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="D125">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E125">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F125">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
       <c r="C126">
-        <v>558</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="D127">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E127">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F127">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>558</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B129" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
@@ -4025,10 +4031,10 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B131" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C131">
         <v>0</v>
@@ -4045,7 +4051,7 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -4065,27 +4071,27 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B133" t="s">
         <v>6</v>
       </c>
       <c r="C133">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E133">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B134" t="s">
         <v>6</v>
@@ -4105,27 +4111,27 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B135" t="s">
         <v>6</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -4145,30 +4151,30 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B137" t="s">
         <v>6</v>
       </c>
       <c r="C137">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D137">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E137">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F137">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B138" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -4185,39 +4191,39 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="B139" t="s">
         <v>6</v>
       </c>
       <c r="C139">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="D139">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E139">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B140" t="s">
         <v>7</v>
       </c>
       <c r="C140">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E140">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F140">
         <v>0</v>
@@ -4225,19 +4231,19 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B141" t="s">
         <v>6</v>
       </c>
       <c r="C141">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E141">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -4245,19 +4251,19 @@
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
       </c>
       <c r="C142">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E142">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -4265,7 +4271,7 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B143" t="s">
         <v>6</v>
@@ -4285,19 +4291,19 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
       <c r="C144">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E144">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -4305,10 +4311,10 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B145" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C145">
         <v>0</v>
@@ -4325,19 +4331,19 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B146" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -4345,30 +4351,30 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C147">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D147">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E147">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F147">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B148" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C148">
         <v>0</v>
@@ -4385,110 +4391,110 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>330</v>
+      </c>
+      <c r="D149">
         <v>9</v>
       </c>
-      <c r="C149">
-        <v>0</v>
-      </c>
-      <c r="D149">
-        <v>0</v>
-      </c>
       <c r="E149">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F149">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="B150" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C150">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D150">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="B151" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C151">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="D151">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E151">
         <v>0</v>
       </c>
       <c r="F151">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="B152" t="s">
         <v>24</v>
       </c>
       <c r="C152">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D152">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F152">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="B153" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C153">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D153">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E153">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F153">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B154" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C154">
         <v>0</v>
@@ -4505,99 +4511,99 @@
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B155" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C155">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D155">
+        <v>3</v>
+      </c>
+      <c r="E155">
         <v>4</v>
       </c>
-      <c r="E155">
-        <v>22</v>
-      </c>
       <c r="F155">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="B156" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C156">
-        <v>289</v>
+        <v>0</v>
       </c>
       <c r="D156">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E156">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F156">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B157" t="s">
+        <v>6</v>
+      </c>
+      <c r="C157">
+        <v>104</v>
+      </c>
+      <c r="D157">
+        <v>4</v>
+      </c>
+      <c r="E157">
+        <v>22</v>
+      </c>
+      <c r="F157">
         <v>7</v>
-      </c>
-      <c r="C157">
-        <v>23</v>
-      </c>
-      <c r="D157">
-        <v>3</v>
-      </c>
-      <c r="E157">
-        <v>4</v>
-      </c>
-      <c r="F157">
-        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B158" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C158">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E158">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B159" t="s">
         <v>7</v>
       </c>
       <c r="C159">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D159">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E159">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -4605,39 +4611,39 @@
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B160" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C160">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D160">
         <v>2</v>
       </c>
       <c r="E160">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F160">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B161" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -4645,30 +4651,30 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C162">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D162">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E162">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F162">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B163" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C163">
         <v>0</v>
@@ -4685,10 +4691,10 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B164" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C164">
         <v>0</v>
@@ -4705,10 +4711,10 @@
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B165" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -4725,99 +4731,99 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="B166" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C166">
-        <v>371</v>
+        <v>0</v>
       </c>
       <c r="D166">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E166">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="F166">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B167" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C167">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D167">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E167">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F167">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="B168" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E168">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B169" t="s">
         <v>6</v>
       </c>
       <c r="C169">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D169">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B170" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C170">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D170">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E170">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -4825,10 +4831,10 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B171" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C171">
         <v>0</v>
@@ -4845,30 +4851,30 @@
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="B172" t="s">
         <v>6</v>
       </c>
       <c r="C172">
-        <v>307</v>
+        <v>68</v>
       </c>
       <c r="D172">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E172">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="F172">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B173" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C173">
         <v>0</v>
@@ -4885,59 +4891,59 @@
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
       </c>
       <c r="C174">
-        <v>151</v>
+        <v>307</v>
       </c>
       <c r="D174">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E174">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F174">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B175" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C175">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D175">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E175">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F175">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B176" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C176">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E176">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F176">
         <v>0</v>
@@ -4945,41 +4951,81 @@
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
+        <v>168</v>
+      </c>
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
         <v>150</v>
       </c>
-      <c r="B177" t="s">
-        <v>9</v>
-      </c>
-      <c r="C177">
-        <v>0</v>
-      </c>
       <c r="D177">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E177">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F177">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>144</v>
+      </c>
+      <c r="B178" t="s">
+        <v>9</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>150</v>
+      </c>
+      <c r="B179" t="s">
+        <v>9</v>
+      </c>
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>159</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B180" t="s">
         <v>24</v>
       </c>
-      <c r="C178">
+      <c r="C180">
         <v>59</v>
       </c>
-      <c r="D178">
+      <c r="D180">
         <v>10</v>
       </c>
-      <c r="E178">
+      <c r="E180">
         <v>4</v>
       </c>
-      <c r="F178">
+      <c r="F180">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Simplified expansion of staples.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -1402,8 +1402,8 @@
   <dimension ref="A1:G180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H115" sqref="H115"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Transfered a couple of recipes.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$180</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$182</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="192">
   <si>
     <t>IngredientName</t>
   </si>
@@ -592,6 +592,12 @@
   </si>
   <si>
     <t>new potatoes</t>
+  </si>
+  <si>
+    <t>halloumi cheese</t>
+  </si>
+  <si>
+    <t>green bananas</t>
   </si>
 </sst>
 </file>
@@ -1399,11 +1405,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G180"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3025,59 +3031,59 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>72</v>
+        <v>191</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="D81">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F81">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B82" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C83">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -3085,19 +3091,19 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>175</v>
+        <v>74</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F84">
         <v>0</v>
@@ -3105,7 +3111,7 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>175</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
@@ -3125,7 +3131,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>181</v>
+        <v>75</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
@@ -3145,7 +3151,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>76</v>
+        <v>181</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
@@ -3165,7 +3171,7 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
@@ -3185,7 +3191,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
@@ -3205,7 +3211,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
@@ -3225,7 +3231,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>154</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
@@ -3245,90 +3251,90 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>186</v>
+        <v>78</v>
       </c>
       <c r="B92" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C92">
-        <v>413</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E92">
         <v>0</v>
       </c>
       <c r="F92">
-        <v>32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B93" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C93">
-        <v>145</v>
+        <v>413</v>
       </c>
       <c r="D93">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E93">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>80</v>
+        <v>190</v>
       </c>
       <c r="B94" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>316</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>81</v>
+        <v>177</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C95">
-        <v>12</v>
+        <v>145</v>
       </c>
       <c r="D95">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F95">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B96" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C96">
         <v>0</v>
@@ -3345,107 +3351,107 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>149</v>
+        <v>81</v>
       </c>
       <c r="B97" t="s">
+        <v>6</v>
+      </c>
+      <c r="C97">
         <v>12</v>
       </c>
-      <c r="C97">
-        <v>305</v>
-      </c>
       <c r="D97">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F97">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B98" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C98">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C99">
-        <v>60</v>
+        <v>305</v>
       </c>
       <c r="D99">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E99">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B100" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C101">
-        <v>194</v>
+        <v>60</v>
       </c>
       <c r="D101">
         <v>2</v>
       </c>
       <c r="E101">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F101">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
@@ -3465,30 +3471,30 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>86</v>
+        <v>187</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>19</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C104">
         <v>0</v>
@@ -3505,90 +3511,90 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B105" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C105">
-        <v>410</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="E105">
         <v>0</v>
       </c>
       <c r="F105">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B106" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C106">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B107" t="s">
         <v>12</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>37</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B108" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C109">
         <v>0</v>
@@ -3605,10 +3611,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B110" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C110">
         <v>0</v>
@@ -3625,7 +3631,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
@@ -3645,10 +3651,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C112">
         <v>0</v>
@@ -3665,10 +3671,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -3685,19 +3691,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>189</v>
+        <v>95</v>
       </c>
       <c r="B114" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C114">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E114">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -3705,116 +3711,116 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
       </c>
       <c r="C115">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B116" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C116">
-        <v>899</v>
+        <v>75</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E116">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="F116">
         <v>0</v>
-      </c>
-      <c r="G116" s="1">
-        <v>0.93</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B117" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F117">
-        <v>0</v>
-      </c>
-      <c r="G117" s="1">
-        <v>0.92</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>899</v>
       </c>
       <c r="D118">
         <v>0</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="F118">
         <v>0</v>
+      </c>
+      <c r="G118" s="1">
+        <v>0.93</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C119">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F119">
         <v>0</v>
+      </c>
+      <c r="G119" s="1">
+        <v>0.92</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C120">
         <v>0</v>
@@ -3831,19 +3837,19 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -3851,7 +3857,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>148</v>
+        <v>102</v>
       </c>
       <c r="B122" t="s">
         <v>9</v>
@@ -3871,10 +3877,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B123" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C123">
         <v>0</v>
@@ -3891,10 +3897,10 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>105</v>
+        <v>148</v>
       </c>
       <c r="B124" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C124">
         <v>0</v>
@@ -3911,19 +3917,19 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>152</v>
+        <v>104</v>
       </c>
       <c r="B125" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C125">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E125">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F125">
         <v>0</v>
@@ -3931,10 +3937,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B126" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -3951,107 +3957,107 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>132</v>
+        <v>24</v>
       </c>
       <c r="D127">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E127">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="F127">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
       </c>
       <c r="C128">
-        <v>558</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="E128">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F128">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
       </c>
       <c r="C129">
-        <v>564</v>
+        <v>132</v>
       </c>
       <c r="D129">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="E129">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="F129">
-        <v>46</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="B130" t="s">
         <v>6</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>558</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B131" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>46</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B132" t="s">
         <v>6</v>
@@ -4071,10 +4077,10 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B133" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C133">
         <v>0</v>
@@ -4091,7 +4097,7 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B134" t="s">
         <v>6</v>
@@ -4111,27 +4117,27 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B135" t="s">
         <v>6</v>
       </c>
       <c r="C135">
-        <v>265</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="F135">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B136" t="s">
         <v>6</v>
@@ -4151,27 +4157,27 @@
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B137" t="s">
         <v>6</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E137">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B138" t="s">
         <v>6</v>
@@ -4191,30 +4197,30 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B139" t="s">
         <v>6</v>
       </c>
       <c r="C139">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E139">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F139">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B140" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C140">
         <v>0</v>
@@ -4231,39 +4237,39 @@
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>119</v>
+        <v>167</v>
       </c>
       <c r="B141" t="s">
         <v>6</v>
       </c>
       <c r="C141">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="D141">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E141">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="F141">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B142" t="s">
         <v>7</v>
       </c>
       <c r="C142">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E142">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F142">
         <v>0</v>
@@ -4271,19 +4277,19 @@
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B143" t="s">
         <v>6</v>
       </c>
       <c r="C143">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E143">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F143">
         <v>0</v>
@@ -4291,19 +4297,19 @@
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B144" t="s">
         <v>7</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -4311,7 +4317,7 @@
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B145" t="s">
         <v>6</v>
@@ -4331,19 +4337,19 @@
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
       </c>
       <c r="C146">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D146">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E146">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -4351,10 +4357,10 @@
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C147">
         <v>0</v>
@@ -4371,19 +4377,19 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F148">
         <v>0</v>
@@ -4391,30 +4397,30 @@
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C149">
-        <v>330</v>
+        <v>0</v>
       </c>
       <c r="D149">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E149">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F149">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B150" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C150">
         <v>0</v>
@@ -4431,110 +4437,110 @@
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>330</v>
+      </c>
+      <c r="D151">
         <v>9</v>
       </c>
-      <c r="C151">
-        <v>0</v>
-      </c>
-      <c r="D151">
-        <v>0</v>
-      </c>
       <c r="E151">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F151">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="B152" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C152">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="D152">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E152">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F152">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>182</v>
+        <v>127</v>
       </c>
       <c r="B153" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C153">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="D153">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="E153">
         <v>0</v>
       </c>
       <c r="F153">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>129</v>
+        <v>161</v>
       </c>
       <c r="B154" t="s">
         <v>24</v>
       </c>
       <c r="C154">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>130</v>
+        <v>182</v>
       </c>
       <c r="B155" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C155">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D155">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E155">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F155">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B156" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C156">
         <v>0</v>
@@ -4551,99 +4557,99 @@
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B157" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="C157">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="D157">
+        <v>3</v>
+      </c>
+      <c r="E157">
         <v>4</v>
       </c>
-      <c r="E157">
-        <v>22</v>
-      </c>
       <c r="F157">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>183</v>
+        <v>131</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C158">
-        <v>289</v>
+        <v>0</v>
       </c>
       <c r="D158">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E158">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F158">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B159" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159">
+        <v>104</v>
+      </c>
+      <c r="D159">
+        <v>4</v>
+      </c>
+      <c r="E159">
+        <v>22</v>
+      </c>
+      <c r="F159">
         <v>7</v>
-      </c>
-      <c r="C159">
-        <v>23</v>
-      </c>
-      <c r="D159">
-        <v>3</v>
-      </c>
-      <c r="E159">
-        <v>4</v>
-      </c>
-      <c r="F159">
-        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>172</v>
+        <v>183</v>
       </c>
       <c r="B160" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C160">
-        <v>20</v>
+        <v>289</v>
       </c>
       <c r="D160">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E160">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F160">
-        <v>0</v>
+        <v>24</v>
       </c>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="B161" t="s">
         <v>7</v>
       </c>
       <c r="C161">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D161">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E161">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F161">
         <v>0</v>
@@ -4651,39 +4657,39 @@
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="B162" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C162">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="D162">
         <v>2</v>
       </c>
       <c r="E162">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F162">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="B163" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C163">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D163">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E163">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -4691,30 +4697,30 @@
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="B164" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C164">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D164">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E164">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F164">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C165">
         <v>0</v>
@@ -4731,10 +4737,10 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B166" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C166">
         <v>0</v>
@@ -4751,10 +4757,10 @@
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B167" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C167">
         <v>0</v>
@@ -4771,99 +4777,99 @@
     </row>
     <row r="168" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C168">
-        <v>371</v>
+        <v>0</v>
       </c>
       <c r="D168">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E168">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="F168">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B169" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C169">
-        <v>595</v>
+        <v>0</v>
       </c>
       <c r="D169">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="E169">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F169">
-        <v>54</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>151</v>
+        <v>178</v>
       </c>
       <c r="B170" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C170">
-        <v>0</v>
+        <v>371</v>
       </c>
       <c r="D170">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E170">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="F170">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="B171" t="s">
         <v>6</v>
       </c>
       <c r="C171">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D171">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E171">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F171">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C172">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D172">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E172">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F172">
         <v>0</v>
@@ -4871,50 +4877,50 @@
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B173" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F173">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>180</v>
+        <v>139</v>
       </c>
       <c r="B174" t="s">
         <v>6</v>
       </c>
       <c r="C174">
-        <v>307</v>
+        <v>68</v>
       </c>
       <c r="D174">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E174">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="F174">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B175" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C175">
         <v>0</v>
@@ -4931,59 +4937,59 @@
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>143</v>
+        <v>180</v>
       </c>
       <c r="B176" t="s">
         <v>6</v>
       </c>
       <c r="C176">
-        <v>151</v>
+        <v>307</v>
       </c>
       <c r="D176">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E176">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="F176">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>168</v>
+        <v>142</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C177">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="D177">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E177">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F177">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B178" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="D178">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E178">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="F178">
         <v>0</v>
@@ -4991,41 +4997,81 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
+        <v>168</v>
+      </c>
+      <c r="B179" t="s">
+        <v>6</v>
+      </c>
+      <c r="C179">
         <v>150</v>
       </c>
-      <c r="B179" t="s">
-        <v>9</v>
-      </c>
-      <c r="C179">
-        <v>0</v>
-      </c>
       <c r="D179">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E179">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F179">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
+        <v>144</v>
+      </c>
+      <c r="B180" t="s">
+        <v>9</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+      <c r="D180">
+        <v>0</v>
+      </c>
+      <c r="E180">
+        <v>0</v>
+      </c>
+      <c r="F180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>150</v>
+      </c>
+      <c r="B181" t="s">
+        <v>9</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+      <c r="D181">
+        <v>0</v>
+      </c>
+      <c r="E181">
+        <v>0</v>
+      </c>
+      <c r="F181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
         <v>159</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B182" t="s">
         <v>24</v>
       </c>
-      <c r="C180">
+      <c r="C182">
         <v>59</v>
       </c>
-      <c r="D180">
+      <c r="D182">
         <v>10</v>
       </c>
-      <c r="E180">
+      <c r="E182">
         <v>4</v>
       </c>
-      <c r="F180">
+      <c r="F182">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Calorie calculation for volume measure.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$182</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$186</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="196">
   <si>
     <t>IngredientName</t>
   </si>
@@ -598,6 +598,18 @@
   </si>
   <si>
     <t>green bananas</t>
+  </si>
+  <si>
+    <t>hazel nuts</t>
+  </si>
+  <si>
+    <t>lettuce</t>
+  </si>
+  <si>
+    <t>lime</t>
+  </si>
+  <si>
+    <t>onion seeds</t>
   </si>
 </sst>
 </file>
@@ -1405,11 +1417,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G182"/>
+  <dimension ref="A1:G186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H142" sqref="H142"/>
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H127" sqref="H127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,6 +1477,9 @@
       <c r="F2">
         <v>10</v>
       </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1485,6 +1500,9 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1505,6 +1523,9 @@
       <c r="F4">
         <v>0</v>
       </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1525,6 +1546,9 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1545,6 +1569,9 @@
       <c r="F6">
         <v>42</v>
       </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1565,6 +1592,9 @@
       <c r="F7">
         <v>0</v>
       </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1585,6 +1615,9 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1605,6 +1638,9 @@
       <c r="F9">
         <v>0</v>
       </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1625,6 +1661,9 @@
       <c r="F10">
         <v>0</v>
       </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1645,6 +1684,9 @@
       <c r="F11">
         <v>1</v>
       </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1665,6 +1707,9 @@
       <c r="F12">
         <v>0</v>
       </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1685,6 +1730,9 @@
       <c r="F13">
         <v>29</v>
       </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1705,6 +1753,9 @@
       <c r="F14">
         <v>0</v>
       </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1725,6 +1776,9 @@
       <c r="F15">
         <v>0</v>
       </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1745,8 +1799,11 @@
       <c r="F16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>176</v>
       </c>
@@ -1765,8 +1822,11 @@
       <c r="F17">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1785,8 +1845,11 @@
       <c r="F18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>179</v>
       </c>
@@ -1805,8 +1868,11 @@
       <c r="F19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>188</v>
       </c>
@@ -1825,8 +1891,11 @@
       <c r="F20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1845,8 +1914,11 @@
       <c r="F21">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1865,8 +1937,11 @@
       <c r="F22">
         <v>81</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>185</v>
       </c>
@@ -1885,8 +1960,11 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1905,8 +1983,11 @@
       <c r="F24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1925,8 +2006,11 @@
       <c r="F25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1945,8 +2029,11 @@
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>163</v>
       </c>
@@ -1965,8 +2052,11 @@
       <c r="F27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -1985,8 +2075,11 @@
       <c r="F28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -2005,8 +2098,11 @@
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>157</v>
       </c>
@@ -2025,8 +2121,11 @@
       <c r="F30">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2045,8 +2144,11 @@
       <c r="F31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2065,8 +2167,11 @@
       <c r="F32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2085,8 +2190,11 @@
       <c r="F33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>158</v>
       </c>
@@ -2105,8 +2213,11 @@
       <c r="F34">
         <v>18</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2125,8 +2236,11 @@
       <c r="F35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>155</v>
       </c>
@@ -2145,8 +2259,11 @@
       <c r="F36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -2165,8 +2282,11 @@
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2185,8 +2305,11 @@
       <c r="F38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2205,8 +2328,11 @@
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2225,8 +2351,11 @@
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -2245,8 +2374,11 @@
       <c r="F41">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2265,8 +2397,11 @@
       <c r="F42">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2285,8 +2420,11 @@
       <c r="F43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2305,8 +2443,11 @@
       <c r="F44">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2325,8 +2466,11 @@
       <c r="F45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2345,8 +2489,11 @@
       <c r="F46">
         <v>34</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2365,8 +2512,11 @@
       <c r="F47">
         <v>7</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2385,8 +2535,11 @@
       <c r="F48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -2405,8 +2558,11 @@
       <c r="F49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2425,8 +2581,11 @@
       <c r="F50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2445,8 +2604,11 @@
       <c r="F51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2465,8 +2627,11 @@
       <c r="F52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2485,8 +2650,11 @@
       <c r="F53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2505,8 +2673,11 @@
       <c r="F54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2525,8 +2696,11 @@
       <c r="F55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2545,8 +2719,11 @@
       <c r="F56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>145</v>
       </c>
@@ -2565,8 +2742,11 @@
       <c r="F57">
         <v>20</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -2585,8 +2765,11 @@
       <c r="F58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -2605,8 +2788,11 @@
       <c r="F59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -2625,8 +2811,11 @@
       <c r="F60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -2645,8 +2834,11 @@
       <c r="F61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -2665,8 +2857,11 @@
       <c r="F62">
         <v>69</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>58</v>
       </c>
@@ -2685,8 +2880,11 @@
       <c r="F63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>184</v>
       </c>
@@ -2704,6 +2902,9 @@
       </c>
       <c r="F64">
         <v>16</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -2725,6 +2926,9 @@
       <c r="F65">
         <v>0</v>
       </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -2745,6 +2949,9 @@
       <c r="F66">
         <v>0</v>
       </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -2765,6 +2972,9 @@
       <c r="F67">
         <v>33</v>
       </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
@@ -2785,6 +2995,9 @@
       <c r="F68">
         <v>0</v>
       </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -2805,6 +3018,9 @@
       <c r="F69">
         <v>0</v>
       </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -2825,6 +3041,9 @@
       <c r="F70">
         <v>11</v>
       </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -2845,6 +3064,9 @@
       <c r="F71">
         <v>0</v>
       </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -2865,6 +3087,9 @@
       <c r="F72">
         <v>0</v>
       </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
@@ -2908,6 +3133,9 @@
       <c r="F74">
         <v>0</v>
       </c>
+      <c r="G74" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -2928,6 +3156,9 @@
       <c r="F75">
         <v>0</v>
       </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
@@ -2948,6 +3179,9 @@
       <c r="F76">
         <v>0</v>
       </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -2968,6 +3202,9 @@
       <c r="F77">
         <v>0</v>
       </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
@@ -2988,6 +3225,9 @@
       <c r="F78">
         <v>0</v>
       </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -3008,6 +3248,9 @@
       <c r="F79">
         <v>0</v>
       </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
@@ -3028,8 +3271,11 @@
       <c r="F80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>191</v>
       </c>
@@ -3048,8 +3294,11 @@
       <c r="F81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>72</v>
       </c>
@@ -3068,8 +3317,11 @@
       <c r="F82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>73</v>
       </c>
@@ -3088,8 +3340,11 @@
       <c r="F83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -3108,8 +3363,11 @@
       <c r="F84">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>175</v>
       </c>
@@ -3128,8 +3386,11 @@
       <c r="F85">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -3148,8 +3409,11 @@
       <c r="F86">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -3168,8 +3432,11 @@
       <c r="F87">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>76</v>
       </c>
@@ -3188,8 +3455,11 @@
       <c r="F88">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -3208,8 +3478,11 @@
       <c r="F89">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>79</v>
       </c>
@@ -3228,8 +3501,11 @@
       <c r="F90">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>154</v>
       </c>
@@ -3248,8 +3524,11 @@
       <c r="F91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>78</v>
       </c>
@@ -3268,8 +3547,11 @@
       <c r="F92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>186</v>
       </c>
@@ -3288,8 +3570,11 @@
       <c r="F93">
         <v>32</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>190</v>
       </c>
@@ -3308,8 +3593,11 @@
       <c r="F94">
         <v>25</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>177</v>
       </c>
@@ -3328,170 +3616,197 @@
       <c r="F95">
         <v>21</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
+        <v>192</v>
+      </c>
+      <c r="B96" t="s">
+        <v>6</v>
+      </c>
+      <c r="C96">
+        <v>628</v>
+      </c>
+      <c r="D96">
+        <v>15</v>
+      </c>
+      <c r="E96">
+        <v>17</v>
+      </c>
+      <c r="F96">
+        <v>61</v>
+      </c>
+      <c r="G96" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>80</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>9</v>
       </c>
-      <c r="C96">
-        <v>0</v>
-      </c>
-      <c r="D96">
-        <v>0</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="C97">
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
         <v>81</v>
       </c>
-      <c r="B97" t="s">
-        <v>6</v>
-      </c>
-      <c r="C97">
+      <c r="B98" t="s">
+        <v>6</v>
+      </c>
+      <c r="C98">
         <v>12</v>
       </c>
-      <c r="D97">
+      <c r="D98">
         <v>3</v>
       </c>
-      <c r="E97">
+      <c r="E98">
         <v>1</v>
       </c>
-      <c r="F97">
+      <c r="F98">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="G98" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
         <v>82</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>7</v>
       </c>
-      <c r="C98">
-        <v>0</v>
-      </c>
-      <c r="D98">
-        <v>0</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>149</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>12</v>
       </c>
-      <c r="C99">
+      <c r="C100">
         <v>305</v>
       </c>
-      <c r="D99">
+      <c r="D100">
         <v>26</v>
       </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="F99">
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
         <v>22</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="G100" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
         <v>83</v>
       </c>
-      <c r="B100" t="s">
-        <v>6</v>
-      </c>
-      <c r="C100">
+      <c r="B101" t="s">
+        <v>6</v>
+      </c>
+      <c r="C101">
         <v>348</v>
       </c>
-      <c r="D100">
+      <c r="D101">
         <v>13</v>
       </c>
-      <c r="E100">
+      <c r="E101">
         <v>70</v>
       </c>
-      <c r="F100">
+      <c r="F101">
         <v>2</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="G101" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
         <v>171</v>
-      </c>
-      <c r="B101" t="s">
-        <v>7</v>
-      </c>
-      <c r="C101">
-        <v>60</v>
-      </c>
-      <c r="D101">
-        <v>2</v>
-      </c>
-      <c r="E101">
-        <v>14</v>
-      </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>84</v>
       </c>
       <c r="B102" t="s">
         <v>7</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F102">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G102" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>187</v>
+        <v>84</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C103">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="G103" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
       <c r="B104" t="s">
         <v>7</v>
@@ -3508,170 +3823,197 @@
       <c r="F104">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>194</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>187</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106">
+        <v>194</v>
+      </c>
+      <c r="D106">
+        <v>2</v>
+      </c>
+      <c r="E106">
+        <v>3</v>
+      </c>
+      <c r="F106">
+        <v>19</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>85</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+      <c r="F107">
+        <v>0</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
         <v>86</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B108" t="s">
         <v>9</v>
       </c>
-      <c r="C105">
-        <v>0</v>
-      </c>
-      <c r="D105">
-        <v>0</v>
-      </c>
-      <c r="E105">
-        <v>0</v>
-      </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>0</v>
+      </c>
+      <c r="F108">
+        <v>0</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
         <v>87</v>
       </c>
-      <c r="B106" t="s">
-        <v>6</v>
-      </c>
-      <c r="C106">
-        <v>0</v>
-      </c>
-      <c r="D106">
-        <v>0</v>
-      </c>
-      <c r="E106">
-        <v>0</v>
-      </c>
-      <c r="F106">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="B109" t="s">
+        <v>6</v>
+      </c>
+      <c r="C109">
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109">
+        <v>0</v>
+      </c>
+      <c r="F109">
+        <v>0</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
         <v>88</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B110" t="s">
         <v>12</v>
       </c>
-      <c r="C107">
+      <c r="C110">
         <v>410</v>
       </c>
-      <c r="D107">
+      <c r="D110">
         <v>19</v>
       </c>
-      <c r="E107">
-        <v>0</v>
-      </c>
-      <c r="F107">
+      <c r="E110">
+        <v>0</v>
+      </c>
+      <c r="F110">
         <v>37</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="G110" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>89</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B111" t="s">
         <v>24</v>
       </c>
-      <c r="C108">
+      <c r="C111">
         <v>46</v>
       </c>
-      <c r="D108">
+      <c r="D111">
         <v>3</v>
       </c>
-      <c r="E108">
+      <c r="E111">
         <v>5</v>
       </c>
-      <c r="F108">
+      <c r="F111">
         <v>2</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="G111" s="1">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
         <v>90</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B112" t="s">
         <v>12</v>
       </c>
-      <c r="C109">
-        <v>0</v>
-      </c>
-      <c r="D109">
-        <v>0</v>
-      </c>
-      <c r="E109">
-        <v>0</v>
-      </c>
-      <c r="F109">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>91</v>
-      </c>
-      <c r="B110" t="s">
-        <v>9</v>
-      </c>
-      <c r="C110">
-        <v>0</v>
-      </c>
-      <c r="D110">
-        <v>0</v>
-      </c>
-      <c r="E110">
-        <v>0</v>
-      </c>
-      <c r="F110">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
-        <v>92</v>
-      </c>
-      <c r="B111" t="s">
-        <v>9</v>
-      </c>
-      <c r="C111">
-        <v>0</v>
-      </c>
-      <c r="D111">
-        <v>0</v>
-      </c>
-      <c r="E111">
-        <v>0</v>
-      </c>
-      <c r="F111">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>93</v>
-      </c>
-      <c r="B112" t="s">
-        <v>7</v>
-      </c>
       <c r="C112">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E112">
         <v>0</v>
       </c>
       <c r="F112">
+        <v>13</v>
+      </c>
+      <c r="G112" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B113" t="s">
         <v>9</v>
@@ -3688,10 +4030,13 @@
       <c r="F113">
         <v>0</v>
       </c>
+      <c r="G113" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
@@ -3708,13 +4053,16 @@
       <c r="F114">
         <v>0</v>
       </c>
+      <c r="G114" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B115" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -3726,144 +4074,159 @@
         <v>0</v>
       </c>
       <c r="F115">
+        <v>0</v>
+      </c>
+      <c r="G115" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>189</v>
+        <v>94</v>
       </c>
       <c r="B116" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C116">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F116">
+        <v>0</v>
+      </c>
+      <c r="G116" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C117">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>0.5</v>
+        <v>0</v>
+      </c>
+      <c r="G117" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B118" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <v>899</v>
+        <v>0</v>
       </c>
       <c r="D118">
         <v>0</v>
       </c>
       <c r="E118">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="F118">
         <v>0</v>
       </c>
       <c r="G118" s="1">
-        <v>0.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>99</v>
+        <v>189</v>
       </c>
       <c r="B119" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F119">
         <v>0</v>
       </c>
       <c r="G119" s="1">
-        <v>0.92</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F120">
+        <v>0.5</v>
+      </c>
+      <c r="G120" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C121">
-        <v>36</v>
+        <v>884</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="G121" s="1">
+        <v>0.93</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B122" t="s">
         <v>9</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>884</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -3872,55 +4235,64 @@
         <v>0</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>100</v>
+      </c>
+      <c r="G122" s="1">
+        <v>0.92</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F123">
+        <v>13</v>
+      </c>
+      <c r="G123" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>148</v>
+        <v>101</v>
       </c>
       <c r="B124" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F124">
+        <v>0</v>
+      </c>
+      <c r="G124" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>104</v>
+        <v>195</v>
       </c>
       <c r="B125" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="C125">
         <v>0</v>
@@ -3932,15 +4304,18 @@
         <v>0</v>
       </c>
       <c r="F125">
+        <v>0</v>
+      </c>
+      <c r="G125" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B126" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C126">
         <v>0</v>
@@ -3952,532 +4327,613 @@
         <v>0</v>
       </c>
       <c r="F126">
+        <v>0</v>
+      </c>
+      <c r="G126" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>152</v>
+        <v>103</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>24</v>
+        <v>202</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E127">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F127">
+        <v>6</v>
+      </c>
+      <c r="G127" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>148</v>
+      </c>
+      <c r="B128" t="s">
+        <v>9</v>
+      </c>
+      <c r="C128">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128">
+        <v>0</v>
+      </c>
+      <c r="F128">
+        <v>0</v>
+      </c>
+      <c r="G128" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>104</v>
+      </c>
+      <c r="B129" t="s">
+        <v>24</v>
+      </c>
+      <c r="C129">
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129">
+        <v>0</v>
+      </c>
+      <c r="F129">
+        <v>0</v>
+      </c>
+      <c r="G129" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>105</v>
+      </c>
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130">
+        <v>0</v>
+      </c>
+      <c r="F130">
+        <v>0</v>
+      </c>
+      <c r="G130" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>152</v>
+      </c>
+      <c r="B131" t="s">
+        <v>6</v>
+      </c>
+      <c r="C131">
+        <v>24</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131">
+        <v>3</v>
+      </c>
+      <c r="F131">
+        <v>0</v>
+      </c>
+      <c r="G131" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
         <v>106</v>
       </c>
-      <c r="B128" t="s">
-        <v>6</v>
-      </c>
-      <c r="C128">
-        <v>0</v>
-      </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
-      <c r="E128">
-        <v>0</v>
-      </c>
-      <c r="F128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="B132" t="s">
+        <v>6</v>
+      </c>
+      <c r="C132">
+        <v>127</v>
+      </c>
+      <c r="D132">
+        <v>2</v>
+      </c>
+      <c r="E132">
+        <v>11</v>
+      </c>
+      <c r="F132">
+        <v>8</v>
+      </c>
+      <c r="G132" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
         <v>107</v>
       </c>
-      <c r="B129" t="s">
-        <v>6</v>
-      </c>
-      <c r="C129">
+      <c r="B133" t="s">
+        <v>6</v>
+      </c>
+      <c r="C133">
         <v>132</v>
       </c>
-      <c r="D129">
+      <c r="D133">
         <v>5</v>
       </c>
-      <c r="E129">
+      <c r="E133">
         <v>24</v>
       </c>
-      <c r="F129">
+      <c r="F133">
         <v>2</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="G133" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
         <v>164</v>
       </c>
-      <c r="B130" t="s">
-        <v>6</v>
-      </c>
-      <c r="C130">
+      <c r="B134" t="s">
+        <v>6</v>
+      </c>
+      <c r="C134">
         <v>558</v>
       </c>
-      <c r="D130">
+      <c r="D134">
         <v>25</v>
       </c>
-      <c r="E130">
+      <c r="E134">
         <v>20</v>
       </c>
-      <c r="F130">
+      <c r="F134">
         <v>50</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="G134" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
         <v>108</v>
       </c>
-      <c r="B131" t="s">
-        <v>6</v>
-      </c>
-      <c r="C131">
+      <c r="B135" t="s">
+        <v>6</v>
+      </c>
+      <c r="C135">
         <v>564</v>
       </c>
-      <c r="D131">
+      <c r="D135">
         <v>26</v>
       </c>
-      <c r="E131">
+      <c r="E135">
         <v>13</v>
       </c>
-      <c r="F131">
+      <c r="F135">
         <v>46</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="G135" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>109</v>
       </c>
-      <c r="B132" t="s">
-        <v>6</v>
-      </c>
-      <c r="C132">
-        <v>0</v>
-      </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
-      <c r="E132">
-        <v>0</v>
-      </c>
-      <c r="F132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="B136" t="s">
+        <v>6</v>
+      </c>
+      <c r="C136">
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136">
+        <v>0</v>
+      </c>
+      <c r="F136">
+        <v>0</v>
+      </c>
+      <c r="G136" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
         <v>110</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B137" t="s">
         <v>9</v>
       </c>
-      <c r="C133">
-        <v>0</v>
-      </c>
-      <c r="D133">
-        <v>0</v>
-      </c>
-      <c r="E133">
-        <v>0</v>
-      </c>
-      <c r="F133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="C137">
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137">
+        <v>0</v>
+      </c>
+      <c r="F137">
+        <v>0</v>
+      </c>
+      <c r="G137" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
         <v>111</v>
       </c>
-      <c r="B134" t="s">
-        <v>6</v>
-      </c>
-      <c r="C134">
-        <v>0</v>
-      </c>
-      <c r="D134">
-        <v>0</v>
-      </c>
-      <c r="E134">
-        <v>0</v>
-      </c>
-      <c r="F134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="B138" t="s">
+        <v>6</v>
+      </c>
+      <c r="C138">
+        <v>534</v>
+      </c>
+      <c r="D138">
+        <v>18</v>
+      </c>
+      <c r="E138">
+        <v>5</v>
+      </c>
+      <c r="F138">
+        <v>50</v>
+      </c>
+      <c r="G138" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
         <v>113</v>
       </c>
-      <c r="B135" t="s">
-        <v>6</v>
-      </c>
-      <c r="C135">
-        <v>0</v>
-      </c>
-      <c r="D135">
-        <v>0</v>
-      </c>
-      <c r="E135">
-        <v>0</v>
-      </c>
-      <c r="F135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="B139" t="s">
+        <v>6</v>
+      </c>
+      <c r="C139">
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139">
+        <v>0</v>
+      </c>
+      <c r="G139" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
         <v>112</v>
       </c>
-      <c r="B136" t="s">
-        <v>6</v>
-      </c>
-      <c r="C136">
-        <v>0</v>
-      </c>
-      <c r="D136">
-        <v>0</v>
-      </c>
-      <c r="E136">
-        <v>0</v>
-      </c>
-      <c r="F136">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="B140" t="s">
+        <v>6</v>
+      </c>
+      <c r="C140">
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>0</v>
+      </c>
+      <c r="G140" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
         <v>114</v>
       </c>
-      <c r="B137" t="s">
-        <v>6</v>
-      </c>
-      <c r="C137">
+      <c r="B141" t="s">
+        <v>6</v>
+      </c>
+      <c r="C141">
         <v>265</v>
       </c>
-      <c r="D137">
+      <c r="D141">
         <v>9</v>
       </c>
-      <c r="E137">
+      <c r="E141">
         <v>58</v>
       </c>
-      <c r="F137">
+      <c r="F141">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="G141" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
         <v>115</v>
       </c>
-      <c r="B138" t="s">
-        <v>6</v>
-      </c>
-      <c r="C138">
-        <v>0</v>
-      </c>
-      <c r="D138">
-        <v>0</v>
-      </c>
-      <c r="E138">
-        <v>0</v>
-      </c>
-      <c r="F138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="B142" t="s">
+        <v>6</v>
+      </c>
+      <c r="C142">
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142">
+        <v>0</v>
+      </c>
+      <c r="F142">
+        <v>0</v>
+      </c>
+      <c r="G142" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
         <v>116</v>
       </c>
-      <c r="B139" t="s">
-        <v>6</v>
-      </c>
-      <c r="C139">
-        <v>0</v>
-      </c>
-      <c r="D139">
-        <v>0</v>
-      </c>
-      <c r="E139">
-        <v>0</v>
-      </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="B143" t="s">
+        <v>6</v>
+      </c>
+      <c r="C143">
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+      <c r="F143">
+        <v>0</v>
+      </c>
+      <c r="G143" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
         <v>117</v>
       </c>
-      <c r="B140" t="s">
-        <v>6</v>
-      </c>
-      <c r="C140">
-        <v>0</v>
-      </c>
-      <c r="D140">
-        <v>0</v>
-      </c>
-      <c r="E140">
-        <v>0</v>
-      </c>
-      <c r="F140">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="B144" t="s">
+        <v>6</v>
+      </c>
+      <c r="C144">
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144">
+        <v>0</v>
+      </c>
+      <c r="G144" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
         <v>167</v>
       </c>
-      <c r="B141" t="s">
-        <v>6</v>
-      </c>
-      <c r="C141">
+      <c r="B145" t="s">
+        <v>6</v>
+      </c>
+      <c r="C145">
         <v>364</v>
       </c>
-      <c r="D141">
+      <c r="D145">
         <v>12</v>
       </c>
-      <c r="E141">
+      <c r="E145">
         <v>86</v>
       </c>
-      <c r="F141">
+      <c r="F145">
         <v>2</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="G145" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
         <v>118</v>
-      </c>
-      <c r="B142" t="s">
-        <v>7</v>
-      </c>
-      <c r="C142">
-        <v>77</v>
-      </c>
-      <c r="D142">
-        <v>2</v>
-      </c>
-      <c r="E142">
-        <v>17</v>
-      </c>
-      <c r="F142">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>119</v>
-      </c>
-      <c r="B143" t="s">
-        <v>6</v>
-      </c>
-      <c r="C143">
-        <v>299</v>
-      </c>
-      <c r="D143">
-        <v>3</v>
-      </c>
-      <c r="E143">
-        <v>79</v>
-      </c>
-      <c r="F143">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>120</v>
-      </c>
-      <c r="B144" t="s">
-        <v>7</v>
-      </c>
-      <c r="C144">
-        <v>26</v>
-      </c>
-      <c r="D144">
-        <v>2</v>
-      </c>
-      <c r="E144">
-        <v>4</v>
-      </c>
-      <c r="F144">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>121</v>
-      </c>
-      <c r="B145" t="s">
-        <v>6</v>
-      </c>
-      <c r="C145">
-        <v>0</v>
-      </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="E145">
-        <v>0</v>
-      </c>
-      <c r="F145">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>122</v>
       </c>
       <c r="B146" t="s">
         <v>7</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F146">
         <v>0</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G146" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B147" t="s">
         <v>6</v>
       </c>
       <c r="C147">
-        <v>0</v>
+        <v>299</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="F147">
         <v>0</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G147" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>120</v>
       </c>
       <c r="B148" t="s">
         <v>7</v>
       </c>
       <c r="C148">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D148">
         <v>2</v>
       </c>
       <c r="E148">
+        <v>4</v>
+      </c>
+      <c r="F148">
+        <v>0</v>
+      </c>
+      <c r="G148" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>121</v>
+      </c>
+      <c r="B149" t="s">
+        <v>6</v>
+      </c>
+      <c r="C149">
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+      <c r="F149">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>122</v>
+      </c>
+      <c r="B150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+      <c r="F150">
+        <v>0</v>
+      </c>
+      <c r="G150" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>128</v>
+      </c>
+      <c r="B151" t="s">
+        <v>6</v>
+      </c>
+      <c r="C151">
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+      <c r="F151">
+        <v>0</v>
+      </c>
+      <c r="G151" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>147</v>
+      </c>
+      <c r="B152" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152">
+        <v>27</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152">
         <v>3</v>
       </c>
-      <c r="F148">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="F152">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
         <v>123</v>
-      </c>
-      <c r="B149" t="s">
-        <v>9</v>
-      </c>
-      <c r="C149">
-        <v>0</v>
-      </c>
-      <c r="D149">
-        <v>0</v>
-      </c>
-      <c r="E149">
-        <v>0</v>
-      </c>
-      <c r="F149">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>124</v>
-      </c>
-      <c r="B150" t="s">
-        <v>12</v>
-      </c>
-      <c r="C150">
-        <v>0</v>
-      </c>
-      <c r="D150">
-        <v>0</v>
-      </c>
-      <c r="E150">
-        <v>0</v>
-      </c>
-      <c r="F150">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>125</v>
-      </c>
-      <c r="B151" t="s">
-        <v>6</v>
-      </c>
-      <c r="C151">
-        <v>330</v>
-      </c>
-      <c r="D151">
-        <v>9</v>
-      </c>
-      <c r="E151">
-        <v>76</v>
-      </c>
-      <c r="F151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>126</v>
-      </c>
-      <c r="B152" t="s">
-        <v>9</v>
-      </c>
-      <c r="C152">
-        <v>0</v>
-      </c>
-      <c r="D152">
-        <v>0</v>
-      </c>
-      <c r="E152">
-        <v>0</v>
-      </c>
-      <c r="F152">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>127</v>
       </c>
       <c r="B153" t="s">
         <v>9</v>
@@ -4494,156 +4950,180 @@
       <c r="F153">
         <v>0</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G153" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
+        <v>124</v>
+      </c>
+      <c r="B154" t="s">
+        <v>12</v>
+      </c>
+      <c r="C154">
+        <v>0</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+      <c r="F154">
+        <v>0</v>
+      </c>
+      <c r="G154" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>125</v>
+      </c>
+      <c r="B155" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155">
+        <v>330</v>
+      </c>
+      <c r="D155">
+        <v>9</v>
+      </c>
+      <c r="E155">
+        <v>76</v>
+      </c>
+      <c r="F155">
+        <v>1</v>
+      </c>
+      <c r="G155" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>126</v>
+      </c>
+      <c r="B156" t="s">
+        <v>9</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+      <c r="F156">
+        <v>0</v>
+      </c>
+      <c r="G156" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>127</v>
+      </c>
+      <c r="B157" t="s">
+        <v>9</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>0</v>
+      </c>
+      <c r="G157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
         <v>161</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B158" t="s">
         <v>24</v>
       </c>
-      <c r="C154">
+      <c r="C158">
         <v>133</v>
       </c>
-      <c r="D154">
+      <c r="D158">
         <v>3</v>
       </c>
-      <c r="E154">
+      <c r="E158">
         <v>4</v>
       </c>
-      <c r="F154">
+      <c r="F158">
         <v>12</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="G158" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>182</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B159" t="s">
         <v>12</v>
       </c>
-      <c r="C155">
+      <c r="C159">
         <v>310</v>
       </c>
-      <c r="D155">
+      <c r="D159">
         <v>22</v>
       </c>
-      <c r="E155">
-        <v>0</v>
-      </c>
-      <c r="F155">
+      <c r="E159">
+        <v>0</v>
+      </c>
+      <c r="F159">
         <v>25</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="G159" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>129</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B160" t="s">
         <v>24</v>
       </c>
-      <c r="C156">
-        <v>0</v>
-      </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-      <c r="E156">
-        <v>0</v>
-      </c>
-      <c r="F156">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="C160">
+        <v>0</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+      <c r="F160">
+        <v>0</v>
+      </c>
+      <c r="G160" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
         <v>130</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B161" t="s">
         <v>24</v>
       </c>
-      <c r="C157">
+      <c r="C161">
         <v>205</v>
-      </c>
-      <c r="D157">
-        <v>3</v>
-      </c>
-      <c r="E157">
-        <v>4</v>
-      </c>
-      <c r="F157">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>131</v>
-      </c>
-      <c r="B158" t="s">
-        <v>9</v>
-      </c>
-      <c r="C158">
-        <v>0</v>
-      </c>
-      <c r="D158">
-        <v>0</v>
-      </c>
-      <c r="E158">
-        <v>0</v>
-      </c>
-      <c r="F158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>132</v>
-      </c>
-      <c r="B159" t="s">
-        <v>6</v>
-      </c>
-      <c r="C159">
-        <v>104</v>
-      </c>
-      <c r="D159">
-        <v>4</v>
-      </c>
-      <c r="E159">
-        <v>22</v>
-      </c>
-      <c r="F159">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>183</v>
-      </c>
-      <c r="B160" t="s">
-        <v>6</v>
-      </c>
-      <c r="C160">
-        <v>289</v>
-      </c>
-      <c r="D160">
-        <v>15</v>
-      </c>
-      <c r="E160">
-        <v>3</v>
-      </c>
-      <c r="F160">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>133</v>
-      </c>
-      <c r="B161" t="s">
-        <v>7</v>
-      </c>
-      <c r="C161">
-        <v>23</v>
       </c>
       <c r="D161">
         <v>3</v>
@@ -4652,392 +5132,452 @@
         <v>4</v>
       </c>
       <c r="F161">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="G161" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
+        <v>131</v>
+      </c>
+      <c r="B162" t="s">
+        <v>9</v>
+      </c>
+      <c r="C162">
+        <v>0</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+      <c r="F162">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>132</v>
+      </c>
+      <c r="B163" t="s">
+        <v>6</v>
+      </c>
+      <c r="C163">
+        <v>104</v>
+      </c>
+      <c r="D163">
+        <v>4</v>
+      </c>
+      <c r="E163">
+        <v>22</v>
+      </c>
+      <c r="F163">
+        <v>7</v>
+      </c>
+      <c r="G163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>183</v>
+      </c>
+      <c r="B164" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164">
+        <v>289</v>
+      </c>
+      <c r="D164">
+        <v>15</v>
+      </c>
+      <c r="E164">
+        <v>3</v>
+      </c>
+      <c r="F164">
+        <v>24</v>
+      </c>
+      <c r="G164" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>133</v>
+      </c>
+      <c r="B165" t="s">
+        <v>7</v>
+      </c>
+      <c r="C165">
+        <v>23</v>
+      </c>
+      <c r="D165">
+        <v>3</v>
+      </c>
+      <c r="E165">
+        <v>4</v>
+      </c>
+      <c r="F165">
+        <v>0</v>
+      </c>
+      <c r="G165" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
         <v>172</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B166" t="s">
         <v>7</v>
       </c>
-      <c r="C162">
+      <c r="C166">
         <v>20</v>
       </c>
-      <c r="D162">
+      <c r="D166">
         <v>2</v>
       </c>
-      <c r="E162">
+      <c r="E166">
         <v>2</v>
       </c>
-      <c r="F162">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="F166">
+        <v>0</v>
+      </c>
+      <c r="G166" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
         <v>146</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B167" t="s">
         <v>7</v>
       </c>
-      <c r="C163">
+      <c r="C167">
         <v>32</v>
       </c>
-      <c r="D163">
+      <c r="D167">
         <v>2</v>
       </c>
-      <c r="E163">
+      <c r="E167">
         <v>7</v>
       </c>
-      <c r="F163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="F167">
+        <v>0</v>
+      </c>
+      <c r="G167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
         <v>160</v>
       </c>
-      <c r="B164" t="s">
-        <v>6</v>
-      </c>
-      <c r="C164">
+      <c r="B168" t="s">
+        <v>6</v>
+      </c>
+      <c r="C168">
         <v>127</v>
       </c>
-      <c r="D164">
+      <c r="D168">
         <v>2</v>
       </c>
-      <c r="E164">
+      <c r="E168">
         <v>11</v>
       </c>
-      <c r="F164">
+      <c r="F168">
         <v>8</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="G168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
         <v>134</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B169" t="s">
         <v>9</v>
       </c>
-      <c r="C165">
-        <v>0</v>
-      </c>
-      <c r="D165">
-        <v>0</v>
-      </c>
-      <c r="E165">
-        <v>0</v>
-      </c>
-      <c r="F165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="C169">
+        <v>0</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169">
+        <v>0</v>
+      </c>
+      <c r="F169">
+        <v>0</v>
+      </c>
+      <c r="G169" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
         <v>135</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B170" t="s">
         <v>9</v>
       </c>
-      <c r="C166">
-        <v>0</v>
-      </c>
-      <c r="D166">
-        <v>0</v>
-      </c>
-      <c r="E166">
-        <v>0</v>
-      </c>
-      <c r="F166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="C170">
+        <v>0</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170">
+        <v>0</v>
+      </c>
+      <c r="F170">
+        <v>0</v>
+      </c>
+      <c r="G170" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
         <v>136</v>
       </c>
-      <c r="B167" t="s">
-        <v>6</v>
-      </c>
-      <c r="C167">
-        <v>0</v>
-      </c>
-      <c r="D167">
-        <v>0</v>
-      </c>
-      <c r="E167">
-        <v>0</v>
-      </c>
-      <c r="F167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="B171" t="s">
+        <v>6</v>
+      </c>
+      <c r="C171">
+        <v>0</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171">
+        <v>0</v>
+      </c>
+      <c r="G171" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>137</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B172" t="s">
         <v>7</v>
       </c>
-      <c r="C168">
-        <v>0</v>
-      </c>
-      <c r="D168">
-        <v>0</v>
-      </c>
-      <c r="E168">
-        <v>0</v>
-      </c>
-      <c r="F168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="C172">
+        <v>0</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172">
+        <v>0</v>
+      </c>
+      <c r="G172" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
         <v>138</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B173" t="s">
         <v>7</v>
       </c>
-      <c r="C169">
-        <v>0</v>
-      </c>
-      <c r="D169">
-        <v>0</v>
-      </c>
-      <c r="E169">
-        <v>0</v>
-      </c>
-      <c r="F169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173">
+        <v>0</v>
+      </c>
+      <c r="G173" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
         <v>178</v>
       </c>
-      <c r="B170" t="s">
-        <v>6</v>
-      </c>
-      <c r="C170">
+      <c r="B174" t="s">
+        <v>6</v>
+      </c>
+      <c r="C174">
         <v>371</v>
       </c>
-      <c r="D170">
+      <c r="D174">
         <v>11</v>
       </c>
-      <c r="E170">
+      <c r="E174">
         <v>55</v>
       </c>
-      <c r="F170">
+      <c r="F174">
         <v>2</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="G174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
         <v>153</v>
       </c>
-      <c r="B171" t="s">
-        <v>6</v>
-      </c>
-      <c r="C171">
+      <c r="B175" t="s">
+        <v>6</v>
+      </c>
+      <c r="C175">
         <v>595</v>
       </c>
-      <c r="D171">
+      <c r="D175">
         <v>17</v>
       </c>
-      <c r="E171">
+      <c r="E175">
         <v>21</v>
       </c>
-      <c r="F171">
+      <c r="F175">
         <v>54</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
+      <c r="G175" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
         <v>151</v>
       </c>
-      <c r="B172" t="s">
+      <c r="B176" t="s">
         <v>9</v>
       </c>
-      <c r="C172">
-        <v>0</v>
-      </c>
-      <c r="D172">
-        <v>0</v>
-      </c>
-      <c r="E172">
-        <v>0</v>
-      </c>
-      <c r="F172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
+      <c r="C176">
+        <v>0</v>
+      </c>
+      <c r="D176">
+        <v>0</v>
+      </c>
+      <c r="E176">
+        <v>0</v>
+      </c>
+      <c r="F176">
+        <v>0</v>
+      </c>
+      <c r="G176" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
         <v>141</v>
       </c>
-      <c r="B173" t="s">
-        <v>6</v>
-      </c>
-      <c r="C173">
+      <c r="B177" t="s">
+        <v>6</v>
+      </c>
+      <c r="C177">
         <v>110</v>
       </c>
-      <c r="D173">
+      <c r="D177">
         <v>16</v>
       </c>
-      <c r="E173">
+      <c r="E177">
         <v>2</v>
       </c>
-      <c r="F173">
+      <c r="F177">
         <v>5</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
+      <c r="G177" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
         <v>139</v>
       </c>
-      <c r="B174" t="s">
-        <v>6</v>
-      </c>
-      <c r="C174">
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178">
         <v>68</v>
       </c>
-      <c r="D174">
+      <c r="D178">
         <v>5</v>
       </c>
-      <c r="E174">
+      <c r="E178">
         <v>13</v>
       </c>
-      <c r="F174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>140</v>
       </c>
-      <c r="B175" t="s">
+      <c r="B179" t="s">
         <v>7</v>
       </c>
-      <c r="C175">
-        <v>0</v>
-      </c>
-      <c r="D175">
-        <v>0</v>
-      </c>
-      <c r="E175">
-        <v>0</v>
-      </c>
-      <c r="F175">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
+      <c r="C179">
+        <v>0</v>
+      </c>
+      <c r="D179">
+        <v>0</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
         <v>180</v>
       </c>
-      <c r="B176" t="s">
-        <v>6</v>
-      </c>
-      <c r="C176">
+      <c r="B180" t="s">
+        <v>6</v>
+      </c>
+      <c r="C180">
         <v>307</v>
       </c>
-      <c r="D176">
+      <c r="D180">
         <v>14</v>
       </c>
-      <c r="E176">
+      <c r="E180">
         <v>47</v>
       </c>
-      <c r="F176">
+      <c r="F180">
         <v>7</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
+      <c r="G180" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
         <v>142</v>
-      </c>
-      <c r="B177" t="s">
-        <v>9</v>
-      </c>
-      <c r="C177">
-        <v>0</v>
-      </c>
-      <c r="D177">
-        <v>0</v>
-      </c>
-      <c r="E177">
-        <v>0</v>
-      </c>
-      <c r="F177">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>143</v>
-      </c>
-      <c r="B178" t="s">
-        <v>6</v>
-      </c>
-      <c r="C178">
-        <v>151</v>
-      </c>
-      <c r="D178">
-        <v>3</v>
-      </c>
-      <c r="E178">
-        <v>34</v>
-      </c>
-      <c r="F178">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>168</v>
-      </c>
-      <c r="B179" t="s">
-        <v>6</v>
-      </c>
-      <c r="C179">
-        <v>150</v>
-      </c>
-      <c r="D179">
-        <v>8</v>
-      </c>
-      <c r="E179">
-        <v>8</v>
-      </c>
-      <c r="F179">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>144</v>
-      </c>
-      <c r="B180" t="s">
-        <v>9</v>
-      </c>
-      <c r="C180">
-        <v>0</v>
-      </c>
-      <c r="D180">
-        <v>0</v>
-      </c>
-      <c r="E180">
-        <v>0</v>
-      </c>
-      <c r="F180">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>150</v>
       </c>
       <c r="B181" t="s">
         <v>9</v>
@@ -5054,24 +5594,122 @@
       <c r="F181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G181" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>143</v>
+      </c>
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182">
+        <v>151</v>
+      </c>
+      <c r="D182">
+        <v>3</v>
+      </c>
+      <c r="E182">
+        <v>34</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>168</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183">
+        <v>150</v>
+      </c>
+      <c r="D183">
+        <v>8</v>
+      </c>
+      <c r="E183">
+        <v>8</v>
+      </c>
+      <c r="F183">
+        <v>8</v>
+      </c>
+      <c r="G183" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>144</v>
+      </c>
+      <c r="B184" t="s">
+        <v>9</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+      <c r="E184">
+        <v>0</v>
+      </c>
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>150</v>
+      </c>
+      <c r="B185" t="s">
+        <v>9</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+      <c r="D185">
+        <v>0</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185">
+        <v>0</v>
+      </c>
+      <c r="G185" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
         <v>159</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B186" t="s">
         <v>24</v>
       </c>
-      <c r="C182">
+      <c r="C186">
         <v>59</v>
       </c>
-      <c r="D182">
+      <c r="D186">
         <v>10</v>
       </c>
-      <c r="E182">
+      <c r="E186">
         <v>4</v>
       </c>
-      <c r="F182">
+      <c r="F186">
+        <v>0</v>
+      </c>
+      <c r="G186" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Keep section and recipes on same page in table of contents.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc_d4jqqip\Documents\Projects\jjc_food_file\ConsoleApp\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$178</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$179</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="191">
   <si>
     <t>IngredientName</t>
   </si>
@@ -592,6 +592,9 @@
   </si>
   <si>
     <t>SpecificGravity</t>
+  </si>
+  <si>
+    <t>fennel</t>
   </si>
 </sst>
 </file>
@@ -1399,11 +1402,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:G179"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F50" sqref="F50"/>
+      <selection pane="bottomLeft" activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,22 +2963,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="B68" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C68">
-        <v>249</v>
+        <v>14</v>
       </c>
       <c r="D68">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="F68">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -2983,22 +2986,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B69" t="s">
         <v>3</v>
       </c>
       <c r="C69">
-        <v>630</v>
+        <v>249</v>
       </c>
       <c r="D69">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E69">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F69">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -3006,22 +3009,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G70" s="1">
         <v>0</v>
@@ -3029,19 +3032,19 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C71">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F71">
         <v>0</v>
@@ -3052,19 +3055,19 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B72" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F72">
         <v>0</v>
@@ -3075,10 +3078,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C73">
         <v>0</v>
@@ -3098,22 +3101,22 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B74" t="s">
         <v>4</v>
       </c>
       <c r="C74">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="1">
         <v>0</v>
@@ -3121,22 +3124,22 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>159</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G75" s="1">
         <v>0</v>
@@ -3144,19 +3147,19 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>180</v>
+        <v>159</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F76">
         <v>0</v>
@@ -3167,22 +3170,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>66</v>
+        <v>180</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
       </c>
       <c r="C77">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="D77">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
@@ -3190,22 +3193,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
@@ -3213,19 +3216,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3236,19 +3239,19 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>164</v>
+        <v>68</v>
       </c>
       <c r="B80" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F80">
         <v>0</v>
@@ -3259,7 +3262,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
@@ -3282,7 +3285,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
@@ -3305,7 +3308,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
@@ -3328,7 +3331,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
@@ -3351,7 +3354,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
@@ -3374,7 +3377,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>145</v>
+        <v>73</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
@@ -3397,7 +3400,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
@@ -3420,22 +3423,22 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
       <c r="B88" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C88">
-        <v>413</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G88" s="1">
         <v>0</v>
@@ -3443,22 +3446,22 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B89" t="s">
         <v>21</v>
       </c>
       <c r="C89">
-        <v>316</v>
+        <v>413</v>
       </c>
       <c r="D89">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G89" s="1">
         <v>0</v>
@@ -3466,22 +3469,22 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C90">
-        <v>145</v>
+        <v>316</v>
       </c>
       <c r="D90">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E90">
         <v>2</v>
       </c>
       <c r="F90">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G90" s="1">
         <v>0</v>
@@ -3489,22 +3492,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="B91" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C91">
-        <v>628</v>
+        <v>145</v>
       </c>
       <c r="D91">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E91">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F91">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="G91" s="1">
         <v>0</v>
@@ -3512,68 +3515,68 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C92">
-        <v>304</v>
+        <v>628</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E92">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G92" s="1">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B93" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C93">
-        <v>12</v>
+        <v>304</v>
       </c>
       <c r="D93">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="F93">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G93" s="1">
-        <v>0</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E94">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
@@ -3581,22 +3584,22 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B95" t="s">
+        <v>4</v>
+      </c>
+      <c r="C95">
+        <v>49</v>
+      </c>
+      <c r="D95">
+        <v>4</v>
+      </c>
+      <c r="E95">
         <v>9</v>
       </c>
-      <c r="C95">
-        <v>305</v>
-      </c>
-      <c r="D95">
-        <v>26</v>
-      </c>
-      <c r="E95">
-        <v>0</v>
-      </c>
       <c r="F95">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G95" s="1">
         <v>0</v>
@@ -3604,22 +3607,22 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>77</v>
+        <v>140</v>
       </c>
       <c r="B96" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C96">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D96">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E96">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G96" s="1">
         <v>0</v>
@@ -3627,22 +3630,22 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C97">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D97">
+        <v>13</v>
+      </c>
+      <c r="E97">
+        <v>70</v>
+      </c>
+      <c r="F97">
         <v>2</v>
-      </c>
-      <c r="E97">
-        <v>14</v>
-      </c>
-      <c r="F97">
-        <v>0</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
@@ -3650,19 +3653,19 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>78</v>
+        <v>161</v>
       </c>
       <c r="B98" t="s">
         <v>4</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F98">
         <v>0</v>
@@ -3673,19 +3676,19 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>182</v>
+        <v>78</v>
       </c>
       <c r="B99" t="s">
         <v>4</v>
       </c>
       <c r="C99">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F99">
         <v>0</v>
@@ -3696,19 +3699,19 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B100" t="s">
         <v>4</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F100">
         <v>0</v>
@@ -3719,22 +3722,22 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B101" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C101">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F101">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G101" s="1">
         <v>0</v>
@@ -3742,22 +3745,22 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G102" s="1">
         <v>0</v>
@@ -3765,22 +3768,22 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B103" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C103">
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G103" s="1">
         <v>0</v>
@@ -3788,22 +3791,22 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C104">
-        <v>410</v>
+        <v>680</v>
       </c>
       <c r="D104">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F104">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G104" s="1">
         <v>0</v>
@@ -3811,68 +3814,68 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B105" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C105">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D105">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E105">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G105" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B106" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C106">
-        <v>217</v>
+        <v>46</v>
       </c>
       <c r="D106">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F106">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G106" s="1">
-        <v>0</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B107" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E107">
         <v>0</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
@@ -3880,7 +3883,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
@@ -3903,19 +3906,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C109">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F109">
         <v>0</v>
@@ -3926,19 +3929,19 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F110">
         <v>0</v>
@@ -3949,10 +3952,10 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B111" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C111">
         <v>0</v>
@@ -3972,19 +3975,19 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>178</v>
+        <v>88</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C112">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -3995,22 +3998,22 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>89</v>
+        <v>178</v>
       </c>
       <c r="B113" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D113">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="E113">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F113">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G113" s="1">
         <v>0</v>
@@ -4018,30 +4021,30 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C114">
-        <v>884</v>
+        <v>62</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F114">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="G114" s="1">
-        <v>0.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
@@ -4059,50 +4062,50 @@
         <v>100</v>
       </c>
       <c r="G115" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B116" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C116">
-        <v>150</v>
+        <v>884</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="G116" s="1">
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C117">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="D117">
         <v>1</v>
       </c>
       <c r="E117">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G117" s="1">
         <v>0</v>
@@ -4110,19 +4113,19 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>184</v>
+        <v>93</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F118">
         <v>0</v>
@@ -4133,7 +4136,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -4156,22 +4159,22 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C120">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G120" s="1">
         <v>0</v>
@@ -4179,22 +4182,22 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="B121" t="s">
+        <v>3</v>
+      </c>
+      <c r="C121">
+        <v>202</v>
+      </c>
+      <c r="D121">
+        <v>3</v>
+      </c>
+      <c r="E121">
+        <v>33</v>
+      </c>
+      <c r="F121">
         <v>6</v>
-      </c>
-      <c r="C121">
-        <v>0</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
-      <c r="E121">
-        <v>0</v>
-      </c>
-      <c r="F121">
-        <v>0</v>
       </c>
       <c r="G121" s="1">
         <v>0</v>
@@ -4202,22 +4205,22 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>96</v>
+        <v>139</v>
       </c>
       <c r="B122" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C122">
-        <v>431</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E122">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G122" s="1">
         <v>0</v>
@@ -4225,22 +4228,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B123" t="s">
+        <v>21</v>
+      </c>
+      <c r="C123">
+        <v>431</v>
+      </c>
+      <c r="D123">
+        <v>38</v>
+      </c>
+      <c r="E123">
         <v>4</v>
       </c>
-      <c r="C123">
-        <v>75</v>
-      </c>
-      <c r="D123">
-        <v>1</v>
-      </c>
-      <c r="E123">
-        <v>18</v>
-      </c>
       <c r="F123">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G123" s="1">
         <v>0</v>
@@ -4248,19 +4251,19 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
       <c r="B124" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C124">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D124">
         <v>1</v>
       </c>
       <c r="E124">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F124">
         <v>0</v>
@@ -4271,22 +4274,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>98</v>
+        <v>143</v>
       </c>
       <c r="B125" t="s">
         <v>3</v>
       </c>
       <c r="C125">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="D125">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E125">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F125">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
@@ -4294,22 +4297,22 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B126" t="s">
         <v>3</v>
       </c>
       <c r="C126">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D126">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E126">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F126">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G126" s="1">
         <v>0</v>
@@ -4317,22 +4320,22 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>154</v>
+        <v>99</v>
       </c>
       <c r="B127" t="s">
         <v>3</v>
       </c>
       <c r="C127">
-        <v>558</v>
+        <v>132</v>
       </c>
       <c r="D127">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="E127">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F127">
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G127" s="1">
         <v>0</v>
@@ -4340,22 +4343,22 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>100</v>
+        <v>154</v>
       </c>
       <c r="B128" t="s">
         <v>3</v>
       </c>
       <c r="C128">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D128">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E128">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F128">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G128" s="1">
         <v>0</v>
@@ -4363,22 +4366,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G129" s="1">
         <v>0</v>
@@ -4386,10 +4389,10 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B130" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C130">
         <v>0</v>
@@ -4409,22 +4412,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B131" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C131">
-        <v>534</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
@@ -4432,22 +4435,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
       </c>
       <c r="C132">
-        <v>673</v>
+        <v>534</v>
       </c>
       <c r="D132">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E132">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F132">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G132" s="1">
         <v>0</v>
@@ -4455,22 +4458,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B133" t="s">
         <v>3</v>
       </c>
       <c r="C133">
-        <v>60</v>
+        <v>673</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E133">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
@@ -4478,22 +4481,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B134" t="s">
         <v>3</v>
       </c>
       <c r="C134">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="D134">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E134">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="F134">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G134" s="1">
         <v>0</v>
@@ -4501,22 +4504,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B135" t="s">
         <v>3</v>
       </c>
       <c r="C135">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E135">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G135" s="1">
         <v>0</v>
@@ -4524,7 +4527,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B136" t="s">
         <v>3</v>
@@ -4547,7 +4550,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B137" t="s">
         <v>3</v>
@@ -4570,65 +4573,65 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="B138" t="s">
         <v>3</v>
       </c>
       <c r="C138">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E138">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F138">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G138" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>110</v>
+        <v>157</v>
       </c>
       <c r="B139" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C139">
-        <v>77</v>
+        <v>364</v>
       </c>
       <c r="D139">
+        <v>12</v>
+      </c>
+      <c r="E139">
+        <v>86</v>
+      </c>
+      <c r="F139">
         <v>2</v>
       </c>
-      <c r="E139">
-        <v>17</v>
-      </c>
-      <c r="F139">
-        <v>0</v>
-      </c>
       <c r="G139" s="1">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C140">
-        <v>299</v>
+        <v>77</v>
       </c>
       <c r="D140">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E140">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F140">
         <v>0</v>
@@ -4639,19 +4642,19 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B141" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C141">
-        <v>26</v>
+        <v>299</v>
       </c>
       <c r="D141">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E141">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="F141">
         <v>0</v>
@@ -4662,65 +4665,65 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B142" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C142">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="D142">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E142">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F142">
         <v>0</v>
       </c>
       <c r="G142" s="1">
-        <v>0.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C143">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D143">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E143">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F143">
         <v>0</v>
       </c>
       <c r="G143" s="1">
-        <v>0</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B144" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C144">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -4731,19 +4734,19 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C145">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E145">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F145">
         <v>0</v>
@@ -4754,19 +4757,19 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
       <c r="B146" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C146">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -4777,22 +4780,22 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B147" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C147">
-        <v>301</v>
+        <v>0</v>
       </c>
       <c r="D147">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E147">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F147">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G147" s="1">
         <v>0</v>
@@ -4800,114 +4803,114 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C148">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="D148">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E148">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="F148">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G148" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B149" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C149">
-        <v>884</v>
+        <v>330</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F149">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G149" s="1">
-        <v>0.92</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B150" t="s">
         <v>6</v>
       </c>
       <c r="C150">
-        <v>116</v>
+        <v>884</v>
       </c>
       <c r="D150">
         <v>0</v>
       </c>
       <c r="E150">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F150">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G150" s="1">
-        <v>1</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>151</v>
+        <v>119</v>
       </c>
       <c r="B151" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C151">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D151">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E151">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F151">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G151" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C152">
-        <v>310</v>
+        <v>133</v>
       </c>
       <c r="D152">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E152">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F152">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G152" s="1">
         <v>0</v>
@@ -4915,91 +4918,91 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="B153" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C153">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D153">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E153">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F153">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G153" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C154">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="D154">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E154">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G154" s="1">
-        <v>1.08</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B155" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C155">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="D155">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E155">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F155">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G155" s="1">
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>172</v>
+        <v>123</v>
       </c>
       <c r="B156" t="s">
         <v>3</v>
       </c>
       <c r="C156">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="D156">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E156">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F156">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G156" s="1">
         <v>0</v>
@@ -5007,22 +5010,22 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="B157" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C157">
-        <v>23</v>
+        <v>289</v>
       </c>
       <c r="D157">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E157">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F157">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
@@ -5030,19 +5033,19 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="B158" t="s">
         <v>4</v>
       </c>
       <c r="C158">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D158">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E158">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F158">
         <v>0</v>
@@ -5053,19 +5056,19 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>137</v>
+        <v>162</v>
       </c>
       <c r="B159" t="s">
         <v>4</v>
       </c>
       <c r="C159">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D159">
         <v>2</v>
       </c>
       <c r="E159">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F159">
         <v>0</v>
@@ -5076,22 +5079,22 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="B160" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C160">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D160">
         <v>2</v>
       </c>
       <c r="E160">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F160">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G160" s="1">
         <v>0</v>
@@ -5099,22 +5102,22 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="B161" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D161">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E161">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F161">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G161" s="1">
         <v>0</v>
@@ -5122,88 +5125,88 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B162" t="s">
         <v>6</v>
       </c>
       <c r="C162">
-        <v>387</v>
+        <v>0</v>
       </c>
       <c r="D162">
         <v>0</v>
       </c>
       <c r="E162">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F162">
         <v>0</v>
       </c>
       <c r="G162" s="1">
-        <v>1.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C163">
-        <v>584</v>
+        <v>387</v>
       </c>
       <c r="D163">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E163">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F163">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="G163" s="1">
-        <v>0.7</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B164" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C164">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="D164">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E164">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F164">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="G164" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B165" t="s">
         <v>4</v>
       </c>
       <c r="C165">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="D165">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E165">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F165">
         <v>0</v>
@@ -5214,22 +5217,22 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C166">
-        <v>371</v>
+        <v>86</v>
       </c>
       <c r="D166">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E166">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F166">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G166" s="1">
         <v>0</v>
@@ -5237,22 +5240,22 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B167" t="s">
         <v>3</v>
       </c>
       <c r="C167">
-        <v>595</v>
+        <v>371</v>
       </c>
       <c r="D167">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E167">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F167">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G167" s="1">
         <v>0</v>
@@ -5260,22 +5263,22 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C168">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D168">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E168">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G168" s="1">
         <v>0</v>
@@ -5283,22 +5286,22 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="B169" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C169">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="D169">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E169">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F169">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G169" s="1">
         <v>0</v>
@@ -5306,22 +5309,22 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B170" t="s">
         <v>3</v>
       </c>
       <c r="C170">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D170">
+        <v>16</v>
+      </c>
+      <c r="E170">
+        <v>2</v>
+      </c>
+      <c r="F170">
         <v>5</v>
-      </c>
-      <c r="E170">
-        <v>13</v>
-      </c>
-      <c r="F170">
-        <v>0</v>
       </c>
       <c r="G170" s="1">
         <v>0</v>
@@ -5329,19 +5332,19 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B171" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C171">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D171">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E171">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F171">
         <v>0</v>
@@ -5352,22 +5355,22 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="B172" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C172">
-        <v>307</v>
+        <v>18</v>
       </c>
       <c r="D172">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E172">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="F172">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G172" s="1">
         <v>0</v>
@@ -5375,22 +5378,22 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="B173" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F173">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G173" s="1">
         <v>0</v>
@@ -5398,19 +5401,19 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B174" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C174">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="D174">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E174">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F174">
         <v>0</v>
@@ -5421,22 +5424,22 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>158</v>
+        <v>134</v>
       </c>
       <c r="B175" t="s">
         <v>3</v>
       </c>
       <c r="C175">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D175">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E175">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F175">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G175" s="1">
         <v>0</v>
@@ -5444,36 +5447,36 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="B176" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C176">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="D176">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E176">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F176">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G176" s="1">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B177" t="s">
         <v>6</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -5485,29 +5488,52 @@
         <v>0</v>
       </c>
       <c r="G177" s="1">
-        <v>0</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
+        <v>141</v>
+      </c>
+      <c r="B178" t="s">
+        <v>6</v>
+      </c>
+      <c r="C178">
+        <v>0</v>
+      </c>
+      <c r="D178">
+        <v>0</v>
+      </c>
+      <c r="E178">
+        <v>0</v>
+      </c>
+      <c r="F178">
+        <v>0</v>
+      </c>
+      <c r="G178" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
         <v>149</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>21</v>
       </c>
-      <c r="C178">
+      <c r="C179">
         <v>59</v>
       </c>
-      <c r="D178">
+      <c r="D179">
         <v>10</v>
       </c>
-      <c r="E178">
+      <c r="E179">
         <v>4</v>
       </c>
-      <c r="F178">
-        <v>0</v>
-      </c>
-      <c r="G178" s="1">
+      <c r="F179">
+        <v>0</v>
+      </c>
+      <c r="G179" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Up to menu F.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -1411,8 +1411,8 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I132" sqref="I132"/>
+      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5226,7 +5226,7 @@
         <v>127</v>
       </c>
       <c r="B166" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C166">
         <v>584</v>

</xml_diff>

<commit_message>
Plain flour in check list.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -1411,8 +1411,8 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B166" sqref="B166"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2673,7 +2673,7 @@
         <v>136</v>
       </c>
       <c r="B55" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>395</v>
@@ -4651,7 +4651,7 @@
         <v>157</v>
       </c>
       <c r="B141" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C141">
         <v>364</v>

</xml_diff>

<commit_message>
Added 2 quick meals
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$182</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$183</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="195">
   <si>
     <t>IngredientName</t>
   </si>
@@ -604,6 +604,9 @@
   </si>
   <si>
     <t>lasagne</t>
+  </si>
+  <si>
+    <t>can corned beef</t>
   </si>
 </sst>
 </file>
@@ -1411,11 +1414,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G182"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,22 +2101,22 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
         <v>3</v>
       </c>
       <c r="C30">
-        <v>90</v>
+        <v>222</v>
       </c>
       <c r="D30">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F30">
-        <v>4</v>
+        <v>13.5</v>
       </c>
       <c r="G30" s="1">
         <v>0</v>
@@ -2121,22 +2124,22 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>146</v>
       </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
       <c r="C31">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="D31">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G31" s="1">
         <v>0</v>
@@ -2144,22 +2147,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
       <c r="C32">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="D32">
         <v>7</v>
       </c>
       <c r="E32">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G32" s="1">
         <v>0</v>
@@ -2167,22 +2170,22 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="D33">
         <v>7</v>
       </c>
       <c r="E33">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="1">
         <v>0</v>
@@ -2190,22 +2193,22 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>147</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34">
-        <v>245</v>
+        <v>57</v>
       </c>
       <c r="D34">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F34">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G34" s="1">
         <v>0</v>
@@ -2213,22 +2216,22 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
       <c r="C35">
-        <v>273</v>
+        <v>245</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <v>18</v>
-      </c>
-      <c r="F35">
-        <v>20</v>
       </c>
       <c r="G35" s="1">
         <v>0</v>
@@ -2236,22 +2239,22 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>145</v>
+        <v>30</v>
       </c>
       <c r="B36" t="s">
         <v>3</v>
       </c>
       <c r="C36">
-        <v>60</v>
+        <v>273</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G36" s="1">
         <v>0</v>
@@ -2259,22 +2262,22 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
       </c>
       <c r="C37">
-        <v>208</v>
+        <v>60</v>
       </c>
       <c r="D37">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="F37">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G37" s="1">
         <v>0</v>
@@ -2282,22 +2285,22 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B38" t="s">
         <v>3</v>
       </c>
       <c r="C38">
-        <v>111</v>
+        <v>208</v>
       </c>
       <c r="D38">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="E38">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G38" s="1">
         <v>0</v>
@@ -2305,22 +2308,22 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
         <v>3</v>
       </c>
       <c r="C39">
-        <v>16</v>
+        <v>111</v>
       </c>
       <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39">
+        <v>22</v>
+      </c>
+      <c r="F39">
         <v>1</v>
-      </c>
-      <c r="E39">
-        <v>3</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
       </c>
       <c r="G39" s="1">
         <v>0</v>
@@ -2328,22 +2331,22 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B40" t="s">
         <v>3</v>
       </c>
       <c r="C40">
-        <v>116</v>
+        <v>16</v>
       </c>
       <c r="D40">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G40" s="1">
         <v>0</v>
@@ -2351,19 +2354,19 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="D41">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="E41">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2374,22 +2377,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>35</v>
       </c>
       <c r="B42" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42" s="1">
         <v>0</v>
@@ -2397,19 +2400,19 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>36</v>
+        <v>192</v>
       </c>
       <c r="B43" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -2420,22 +2423,22 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44">
-        <v>553</v>
+        <v>35</v>
       </c>
       <c r="D44">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="F44">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="G44" s="1">
         <v>0</v>
@@ -2443,22 +2446,22 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C45">
-        <v>25</v>
+        <v>553</v>
       </c>
       <c r="D45">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E45">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="G45" s="1">
         <v>0</v>
@@ -2466,19 +2469,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B46" t="s">
         <v>4</v>
       </c>
       <c r="C46">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E46">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -2489,22 +2492,22 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C47">
-        <v>412</v>
+        <v>7</v>
       </c>
       <c r="D47">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -2512,22 +2515,22 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C48">
-        <v>183</v>
+        <v>412</v>
       </c>
       <c r="D48">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -2535,22 +2538,22 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -2558,10 +2561,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C50">
         <v>0</v>
@@ -2581,19 +2584,19 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B51" t="s">
         <v>4</v>
       </c>
       <c r="C51">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -2604,22 +2607,22 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C52">
-        <v>455</v>
+        <v>13</v>
       </c>
       <c r="D52">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E52">
         <v>2</v>
       </c>
       <c r="F52">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="G52" s="1">
         <v>0</v>
@@ -2627,22 +2630,22 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B53" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C53">
-        <v>43</v>
+        <v>455</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E53">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="G53" s="1">
         <v>0</v>
@@ -2650,19 +2653,19 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2673,10 +2676,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B55" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="C55">
         <v>0</v>
@@ -2696,22 +2699,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="C56">
-        <v>395</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G56" s="1">
         <v>0</v>
@@ -2719,22 +2722,22 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>49</v>
+        <v>135</v>
       </c>
       <c r="B57" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C57">
-        <v>98</v>
+        <v>395</v>
       </c>
       <c r="D57">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="E57">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="F57">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G57" s="1">
         <v>0</v>
@@ -2742,22 +2745,22 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58">
+        <v>98</v>
+      </c>
+      <c r="D58">
+        <v>11</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58">
         <v>4</v>
-      </c>
-      <c r="C58">
-        <v>17</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-      <c r="E58">
-        <v>3</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
       </c>
       <c r="G58" s="1">
         <v>0</v>
@@ -2765,19 +2768,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B59" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C59">
-        <v>176</v>
+        <v>17</v>
       </c>
       <c r="D59">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -2788,91 +2791,91 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C60">
-        <v>342</v>
+        <v>176</v>
       </c>
       <c r="D60">
         <v>6</v>
       </c>
       <c r="E60">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="F60">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="G60" s="1">
-        <v>0.98</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C61">
-        <v>669</v>
+        <v>342</v>
       </c>
       <c r="D61">
         <v>6</v>
       </c>
       <c r="E61">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F61">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="G61" s="1">
-        <v>1.01</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
       <c r="B62" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="C62">
-        <v>175</v>
+        <v>669</v>
       </c>
       <c r="D62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E62">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F62">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="G62" s="1">
-        <v>0</v>
+        <v>1.01</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>54</v>
+        <v>172</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>175</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="G63" s="1">
         <v>0</v>
@@ -2880,7 +2883,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -2903,22 +2906,22 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>154</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C65">
-        <v>354</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
@@ -2926,22 +2929,22 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
       <c r="B66" t="s">
         <v>3</v>
       </c>
       <c r="C66">
-        <v>241</v>
+        <v>354</v>
       </c>
       <c r="D66">
         <v>3</v>
       </c>
       <c r="E66">
-        <v>63</v>
+        <v>15</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="G66" s="1">
         <v>0</v>
@@ -2949,19 +2952,19 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>241</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="F67">
         <v>0</v>
@@ -2972,22 +2975,22 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>147</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -2995,22 +2998,22 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>189</v>
+        <v>58</v>
       </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C69">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E69">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G69" s="1">
         <v>0</v>
@@ -3018,22 +3021,22 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C70">
-        <v>264</v>
+        <v>14</v>
       </c>
       <c r="D70">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F70">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="G70" s="1">
         <v>0</v>
@@ -3041,22 +3044,22 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>59</v>
+        <v>190</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="C71">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="D71">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E71">
+        <v>4</v>
+      </c>
+      <c r="F71">
         <v>21</v>
-      </c>
-      <c r="F71">
-        <v>13</v>
       </c>
       <c r="G71" s="1">
         <v>0</v>
@@ -3064,22 +3067,22 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B72" t="s">
         <v>3</v>
       </c>
       <c r="C72">
-        <v>630</v>
+        <v>249</v>
       </c>
       <c r="D72">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E72">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="F72">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G72" s="1">
         <v>0</v>
@@ -3087,22 +3090,22 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>630</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="G73" s="1">
         <v>0</v>
@@ -3110,19 +3113,19 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C74">
-        <v>81</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F74">
         <v>0</v>
@@ -3133,19 +3136,19 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B75" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F75">
         <v>0</v>
@@ -3156,10 +3159,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C76">
         <v>0</v>
@@ -3179,22 +3182,22 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B77" t="s">
         <v>4</v>
       </c>
       <c r="C77">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G77" s="1">
         <v>0</v>
@@ -3202,22 +3205,22 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>158</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G78" s="1">
         <v>0</v>
@@ -3225,19 +3228,19 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>179</v>
+        <v>158</v>
       </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="F79">
         <v>0</v>
@@ -3248,22 +3251,22 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>179</v>
       </c>
       <c r="B80" t="s">
         <v>4</v>
       </c>
       <c r="C80">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="D80">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G80" s="1">
         <v>0</v>
@@ -3271,22 +3274,22 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G81" s="1">
         <v>0</v>
@@ -3294,19 +3297,19 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C82">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F82">
         <v>0</v>
@@ -3317,19 +3320,19 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>163</v>
+        <v>68</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F83">
         <v>0</v>
@@ -3340,7 +3343,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>163</v>
       </c>
       <c r="B84" t="s">
         <v>6</v>
@@ -3363,7 +3366,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>169</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
@@ -3386,7 +3389,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
@@ -3409,7 +3412,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
@@ -3432,7 +3435,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
@@ -3455,7 +3458,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
@@ -3478,7 +3481,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
@@ -3501,22 +3504,22 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>174</v>
+        <v>72</v>
       </c>
       <c r="B91" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C91">
-        <v>413</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="E91">
         <v>0</v>
       </c>
       <c r="F91">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="G91" s="1">
         <v>0</v>
@@ -3524,22 +3527,22 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B92" t="s">
         <v>21</v>
       </c>
       <c r="C92">
-        <v>316</v>
+        <v>413</v>
       </c>
       <c r="D92">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G92" s="1">
         <v>0</v>
@@ -3547,22 +3550,22 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="B93" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C93">
-        <v>145</v>
+        <v>316</v>
       </c>
       <c r="D93">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="E93">
         <v>2</v>
       </c>
       <c r="F93">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G93" s="1">
         <v>0</v>
@@ -3570,22 +3573,22 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="B94" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C94">
-        <v>628</v>
+        <v>145</v>
       </c>
       <c r="D94">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E94">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="F94">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="G94" s="1">
         <v>0</v>
@@ -3593,68 +3596,68 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>74</v>
+        <v>180</v>
       </c>
       <c r="B95" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C95">
-        <v>304</v>
+        <v>628</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E95">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="G95" s="1">
-        <v>1.42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B96" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C96">
-        <v>12</v>
+        <v>304</v>
       </c>
       <c r="D96">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="F96">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G96" s="1">
-        <v>0</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C97">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="D97">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E97">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F97">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G97" s="1">
         <v>0</v>
@@ -3662,22 +3665,22 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>76</v>
       </c>
       <c r="B98" t="s">
+        <v>4</v>
+      </c>
+      <c r="C98">
+        <v>49</v>
+      </c>
+      <c r="D98">
+        <v>4</v>
+      </c>
+      <c r="E98">
         <v>9</v>
       </c>
-      <c r="C98">
-        <v>305</v>
-      </c>
-      <c r="D98">
-        <v>26</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
       <c r="F98">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G98" s="1">
         <v>0</v>
@@ -3685,22 +3688,22 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>193</v>
+        <v>139</v>
       </c>
       <c r="B99" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C99">
-        <v>348</v>
+        <v>305</v>
       </c>
       <c r="D99">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="E99">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="G99" s="1">
         <v>0</v>
@@ -3708,22 +3711,22 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>193</v>
       </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100">
-        <v>60</v>
+        <v>348</v>
       </c>
       <c r="D100">
+        <v>13</v>
+      </c>
+      <c r="E100">
+        <v>70</v>
+      </c>
+      <c r="F100">
         <v>2</v>
-      </c>
-      <c r="E100">
-        <v>14</v>
-      </c>
-      <c r="F100">
-        <v>0</v>
       </c>
       <c r="G100" s="1">
         <v>0</v>
@@ -3731,19 +3734,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>77</v>
+        <v>160</v>
       </c>
       <c r="B101" t="s">
         <v>4</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F101">
         <v>0</v>
@@ -3754,19 +3757,19 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>181</v>
+        <v>77</v>
       </c>
       <c r="B102" t="s">
         <v>4</v>
       </c>
       <c r="C102">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F102">
         <v>0</v>
@@ -3777,19 +3780,19 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B103" t="s">
         <v>4</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F103">
         <v>0</v>
@@ -3800,22 +3803,22 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B104" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C104">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="G104" s="1">
         <v>0</v>
@@ -3823,22 +3826,22 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>194</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="G105" s="1">
         <v>0</v>
@@ -3846,22 +3849,22 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B106" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C106">
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G106" s="1">
         <v>0</v>
@@ -3869,22 +3872,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C107">
-        <v>410</v>
+        <v>680</v>
       </c>
       <c r="D107">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
@@ -3892,68 +3895,68 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B108" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C108">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D108">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E108">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G108" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C109">
-        <v>217</v>
+        <v>46</v>
       </c>
       <c r="D109">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F109">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G109" s="1">
-        <v>0</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E110">
         <v>0</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G110" s="1">
         <v>0</v>
@@ -3961,7 +3964,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
@@ -3984,19 +3987,19 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C112">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F112">
         <v>0</v>
@@ -4007,19 +4010,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -4030,10 +4033,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B114" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C114">
         <v>0</v>
@@ -4053,19 +4056,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C115">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F115">
         <v>0</v>
@@ -4076,22 +4079,22 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="B116" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C116">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D116">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="E116">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F116">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G116" s="1">
         <v>0</v>
@@ -4099,30 +4102,30 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B117" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C117">
-        <v>884</v>
+        <v>62</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F117">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="G117" s="1">
-        <v>0.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
@@ -4140,50 +4143,50 @@
         <v>100</v>
       </c>
       <c r="G118" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B119" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C119">
-        <v>150</v>
+        <v>884</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="G119" s="1">
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="D120">
         <v>1</v>
       </c>
       <c r="E120">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G120" s="1">
         <v>0</v>
@@ -4191,19 +4194,19 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="B121" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F121">
         <v>0</v>
@@ -4214,7 +4217,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
@@ -4237,22 +4240,22 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B123" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C123">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G123" s="1">
         <v>0</v>
@@ -4260,22 +4263,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="B124" t="s">
+        <v>3</v>
+      </c>
+      <c r="C124">
+        <v>202</v>
+      </c>
+      <c r="D124">
+        <v>3</v>
+      </c>
+      <c r="E124">
+        <v>33</v>
+      </c>
+      <c r="F124">
         <v>6</v>
-      </c>
-      <c r="C124">
-        <v>0</v>
-      </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
-      <c r="E124">
-        <v>0</v>
-      </c>
-      <c r="F124">
-        <v>0</v>
       </c>
       <c r="G124" s="1">
         <v>0</v>
@@ -4283,22 +4286,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="B125" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C125">
-        <v>431</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E125">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F125">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
@@ -4306,22 +4309,22 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B126" t="s">
+        <v>21</v>
+      </c>
+      <c r="C126">
+        <v>431</v>
+      </c>
+      <c r="D126">
+        <v>38</v>
+      </c>
+      <c r="E126">
         <v>4</v>
       </c>
-      <c r="C126">
-        <v>75</v>
-      </c>
-      <c r="D126">
-        <v>1</v>
-      </c>
-      <c r="E126">
-        <v>18</v>
-      </c>
       <c r="F126">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G126" s="1">
         <v>0</v>
@@ -4329,19 +4332,19 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="B127" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C127">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D127">
         <v>1</v>
       </c>
       <c r="E127">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F127">
         <v>0</v>
@@ -4352,22 +4355,22 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="B128" t="s">
         <v>3</v>
       </c>
       <c r="C128">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="D128">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F128">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G128" s="1">
         <v>0</v>
@@ -4375,22 +4378,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
       </c>
       <c r="C129">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D129">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E129">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F129">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G129" s="1">
         <v>0</v>
@@ -4398,22 +4401,22 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="B130" t="s">
         <v>3</v>
       </c>
       <c r="C130">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="D130">
+        <v>5</v>
+      </c>
+      <c r="E130">
+        <v>24</v>
+      </c>
+      <c r="F130">
         <v>2</v>
-      </c>
-      <c r="E130">
-        <v>13</v>
-      </c>
-      <c r="F130">
-        <v>11</v>
       </c>
       <c r="G130" s="1">
         <v>0</v>
@@ -4421,22 +4424,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B131" t="s">
         <v>3</v>
       </c>
       <c r="C131">
-        <v>558</v>
+        <v>158</v>
       </c>
       <c r="D131">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E131">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F131">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
@@ -4444,22 +4447,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
       </c>
       <c r="C132">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D132">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E132">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F132">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G132" s="1">
         <v>0</v>
@@ -4467,22 +4470,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B133" t="s">
         <v>3</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
@@ -4490,10 +4493,10 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B134" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C134">
         <v>0</v>
@@ -4513,22 +4516,22 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B135" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C135">
-        <v>534</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E135">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F135">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G135" s="1">
         <v>0</v>
@@ -4536,22 +4539,22 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B136" t="s">
         <v>3</v>
       </c>
       <c r="C136">
-        <v>673</v>
+        <v>534</v>
       </c>
       <c r="D136">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E136">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F136">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G136" s="1">
         <v>0</v>
@@ -4559,22 +4562,22 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B137" t="s">
         <v>3</v>
       </c>
       <c r="C137">
-        <v>60</v>
+        <v>673</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E137">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F137">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G137" s="1">
         <v>0</v>
@@ -4582,22 +4585,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B138" t="s">
         <v>3</v>
       </c>
       <c r="C138">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="D138">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E138">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="F138">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G138" s="1">
         <v>0</v>
@@ -4605,22 +4608,22 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B139" t="s">
         <v>3</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E139">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G139" s="1">
         <v>0</v>
@@ -4628,7 +4631,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B140" t="s">
         <v>3</v>
@@ -4651,7 +4654,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B141" t="s">
         <v>3</v>
@@ -4674,65 +4677,65 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="B142" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C142">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E142">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F142">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G142" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="B143" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C143">
-        <v>77</v>
+        <v>364</v>
       </c>
       <c r="D143">
+        <v>12</v>
+      </c>
+      <c r="E143">
+        <v>86</v>
+      </c>
+      <c r="F143">
         <v>2</v>
       </c>
-      <c r="E143">
-        <v>17</v>
-      </c>
-      <c r="F143">
-        <v>0</v>
-      </c>
       <c r="G143" s="1">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B144" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C144">
-        <v>299</v>
+        <v>77</v>
       </c>
       <c r="D144">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E144">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F144">
         <v>0</v>
@@ -4743,19 +4746,19 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B145" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C145">
-        <v>26</v>
+        <v>299</v>
       </c>
       <c r="D145">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E145">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="F145">
         <v>0</v>
@@ -4766,65 +4769,65 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C146">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="D146">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E146">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F146">
         <v>0</v>
       </c>
       <c r="G146" s="1">
-        <v>0.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B147" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C147">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D147">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E147">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F147">
         <v>0</v>
       </c>
       <c r="G147" s="1">
-        <v>0</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C148">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D148">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E148">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F148">
         <v>0</v>
@@ -4835,19 +4838,19 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B149" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C149">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D149">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E149">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F149">
         <v>0</v>
@@ -4858,19 +4861,19 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B150" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D150">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E150">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F150">
         <v>0</v>
@@ -4881,22 +4884,22 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B151" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C151">
-        <v>301</v>
+        <v>0</v>
       </c>
       <c r="D151">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E151">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F151">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G151" s="1">
         <v>0</v>
@@ -4904,114 +4907,114 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C152">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="D152">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E152">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="F152">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G152" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B153" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C153">
-        <v>884</v>
+        <v>330</v>
       </c>
       <c r="D153">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E153">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F153">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G153" s="1">
-        <v>0.92</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B154" t="s">
         <v>6</v>
       </c>
       <c r="C154">
-        <v>116</v>
+        <v>884</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="E154">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G154" s="1">
-        <v>1</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B155" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C155">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D155">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E155">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F155">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G155" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B156" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C156">
-        <v>310</v>
+        <v>133</v>
       </c>
       <c r="D156">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E156">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F156">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G156" s="1">
         <v>0</v>
@@ -5019,91 +5022,91 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="B157" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C157">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D157">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E157">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F157">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G157" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B158" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C158">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="D158">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E158">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G158" s="1">
-        <v>1.08</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B159" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C159">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="D159">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E159">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F159">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G159" s="1">
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="B160" t="s">
         <v>3</v>
       </c>
       <c r="C160">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="D160">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E160">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F160">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G160" s="1">
         <v>0</v>
@@ -5111,22 +5114,22 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="B161" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C161">
-        <v>23</v>
+        <v>289</v>
       </c>
       <c r="D161">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E161">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F161">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G161" s="1">
         <v>0</v>
@@ -5134,19 +5137,19 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B162" t="s">
         <v>4</v>
       </c>
       <c r="C162">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D162">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E162">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F162">
         <v>0</v>
@@ -5157,19 +5160,19 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B163" t="s">
         <v>4</v>
       </c>
       <c r="C163">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D163">
         <v>2</v>
       </c>
       <c r="E163">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -5180,22 +5183,22 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B164" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C164">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D164">
         <v>2</v>
       </c>
       <c r="E164">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F164">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G164" s="1">
         <v>0</v>
@@ -5203,22 +5206,22 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B165" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C165">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D165">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E165">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F165">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G165" s="1">
         <v>0</v>
@@ -5226,88 +5229,88 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B166" t="s">
         <v>6</v>
       </c>
       <c r="C166">
-        <v>387</v>
+        <v>0</v>
       </c>
       <c r="D166">
         <v>0</v>
       </c>
       <c r="E166">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F166">
         <v>0</v>
       </c>
       <c r="G166" s="1">
-        <v>1.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B167" t="s">
         <v>6</v>
       </c>
       <c r="C167">
-        <v>584</v>
+        <v>387</v>
       </c>
       <c r="D167">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E167">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F167">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="G167" s="1">
-        <v>0.7</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B168" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C168">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="D168">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E168">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="G168" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B169" t="s">
         <v>4</v>
       </c>
       <c r="C169">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="D169">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E169">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F169">
         <v>0</v>
@@ -5318,22 +5321,22 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="B170" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C170">
-        <v>371</v>
+        <v>86</v>
       </c>
       <c r="D170">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E170">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F170">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G170" s="1">
         <v>0</v>
@@ -5341,22 +5344,22 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="B171" t="s">
         <v>3</v>
       </c>
       <c r="C171">
-        <v>595</v>
+        <v>371</v>
       </c>
       <c r="D171">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E171">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F171">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G171" s="1">
         <v>0</v>
@@ -5364,22 +5367,22 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B172" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C172">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D172">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E172">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F172">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G172" s="1">
         <v>0</v>
@@ -5387,22 +5390,22 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B173" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C173">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="D173">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E173">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F173">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G173" s="1">
         <v>0</v>
@@ -5410,22 +5413,22 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B174" t="s">
         <v>3</v>
       </c>
       <c r="C174">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D174">
+        <v>16</v>
+      </c>
+      <c r="E174">
+        <v>2</v>
+      </c>
+      <c r="F174">
         <v>5</v>
-      </c>
-      <c r="E174">
-        <v>13</v>
-      </c>
-      <c r="F174">
-        <v>0</v>
       </c>
       <c r="G174" s="1">
         <v>0</v>
@@ -5433,19 +5436,19 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B175" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C175">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D175">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E175">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F175">
         <v>0</v>
@@ -5456,22 +5459,22 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="B176" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C176">
-        <v>307</v>
+        <v>18</v>
       </c>
       <c r="D176">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E176">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="F176">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G176" s="1">
         <v>0</v>
@@ -5479,22 +5482,22 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C177">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="D177">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E177">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F177">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G177" s="1">
         <v>0</v>
@@ -5502,19 +5505,19 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B178" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C178">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="D178">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E178">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F178">
         <v>0</v>
@@ -5525,22 +5528,22 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B179" t="s">
         <v>3</v>
       </c>
       <c r="C179">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D179">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E179">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F179">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G179" s="1">
         <v>0</v>
@@ -5548,36 +5551,36 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C180">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="D180">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E180">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F180">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G180" s="1">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B181" t="s">
         <v>6</v>
       </c>
       <c r="C181">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D181">
         <v>0</v>
@@ -5589,29 +5592,52 @@
         <v>0</v>
       </c>
       <c r="G181" s="1">
-        <v>0</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
+        <v>140</v>
+      </c>
+      <c r="B182" t="s">
+        <v>6</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>0</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182">
+        <v>0</v>
+      </c>
+      <c r="G182" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
         <v>148</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B183" t="s">
         <v>21</v>
       </c>
-      <c r="C182">
+      <c r="C183">
         <v>59</v>
       </c>
-      <c r="D182">
+      <c r="D183">
         <v>10</v>
       </c>
-      <c r="E182">
+      <c r="E183">
         <v>4</v>
       </c>
-      <c r="F182">
-        <v>0</v>
-      </c>
-      <c r="G182" s="1">
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Nut roast up date.
</commit_message>
<xml_diff>
--- a/ConsoleApp/Input/Ingredients.xlsx
+++ b/ConsoleApp/Input/Ingredients.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc\Documents\Projects\jjc-csharp-food-file-harmony-angel\ConsoleApp\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joejc\Documents\Projects\jjc-food-file-harmony-angel\ConsoleApp\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="Ingredients" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$183</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Ingredients!$A$2:$G$184</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="196">
   <si>
     <t>IngredientName</t>
   </si>
@@ -607,6 +607,9 @@
   </si>
   <si>
     <t>can corned beef</t>
+  </si>
+  <si>
+    <t>marmite</t>
   </si>
 </sst>
 </file>
@@ -1414,11 +1417,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G183"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C106" sqref="C106:G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3849,7 +3852,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>78</v>
+        <v>195</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
@@ -3872,22 +3875,22 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B107" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C107">
-        <v>680</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
@@ -3895,22 +3898,22 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B108" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C108">
-        <v>410</v>
+        <v>680</v>
       </c>
       <c r="D108">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="G108" s="1">
         <v>0</v>
@@ -3918,68 +3921,68 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B109" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C109">
-        <v>46</v>
+        <v>410</v>
       </c>
       <c r="D109">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E109">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="G109" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B110" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C110">
-        <v>217</v>
+        <v>46</v>
       </c>
       <c r="D110">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F110">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="G110" s="1">
-        <v>0</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>217</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="E111">
         <v>0</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G111" s="1">
         <v>0</v>
@@ -3987,7 +3990,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
@@ -4010,19 +4013,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C113">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D113">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F113">
         <v>0</v>
@@ -4033,19 +4036,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B114" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F114">
         <v>0</v>
@@ -4056,10 +4059,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B115" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C115">
         <v>0</v>
@@ -4079,19 +4082,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>177</v>
+        <v>87</v>
       </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F116">
         <v>0</v>
@@ -4102,22 +4105,22 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>88</v>
+        <v>177</v>
       </c>
       <c r="B117" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C117">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="D117">
-        <v>2.2000000000000002</v>
+        <v>2</v>
       </c>
       <c r="E117">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="F117">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G117" s="1">
         <v>0</v>
@@ -4125,30 +4128,30 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B118" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C118">
-        <v>884</v>
+        <v>62</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F118">
-        <v>100</v>
+        <v>0.5</v>
       </c>
       <c r="G118" s="1">
-        <v>0.93</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
@@ -4166,50 +4169,50 @@
         <v>100</v>
       </c>
       <c r="G119" s="1">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B120" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C120">
-        <v>150</v>
+        <v>884</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="G120" s="1">
-        <v>0</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C121">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="D121">
         <v>1</v>
       </c>
       <c r="E121">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G121" s="1">
         <v>0</v>
@@ -4217,19 +4220,19 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>183</v>
+        <v>92</v>
       </c>
       <c r="B122" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F122">
         <v>0</v>
@@ -4240,7 +4243,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
@@ -4263,22 +4266,22 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B124" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C124">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E124">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F124">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G124" s="1">
         <v>0</v>
@@ -4286,22 +4289,22 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="B125" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>202</v>
+      </c>
+      <c r="D125">
+        <v>3</v>
+      </c>
+      <c r="E125">
+        <v>33</v>
+      </c>
+      <c r="F125">
         <v>6</v>
-      </c>
-      <c r="C125">
-        <v>0</v>
-      </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
-      <c r="E125">
-        <v>0</v>
-      </c>
-      <c r="F125">
-        <v>0</v>
       </c>
       <c r="G125" s="1">
         <v>0</v>
@@ -4309,22 +4312,22 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>95</v>
+        <v>138</v>
       </c>
       <c r="B126" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C126">
-        <v>431</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="G126" s="1">
         <v>0</v>
@@ -4332,22 +4335,22 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B127" t="s">
+        <v>21</v>
+      </c>
+      <c r="C127">
+        <v>431</v>
+      </c>
+      <c r="D127">
+        <v>38</v>
+      </c>
+      <c r="E127">
         <v>4</v>
       </c>
-      <c r="C127">
-        <v>75</v>
-      </c>
-      <c r="D127">
-        <v>1</v>
-      </c>
-      <c r="E127">
-        <v>18</v>
-      </c>
       <c r="F127">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="G127" s="1">
         <v>0</v>
@@ -4355,19 +4358,19 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="B128" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C128">
-        <v>24</v>
+        <v>75</v>
       </c>
       <c r="D128">
         <v>1</v>
       </c>
       <c r="E128">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="F128">
         <v>0</v>
@@ -4378,22 +4381,22 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>97</v>
+        <v>142</v>
       </c>
       <c r="B129" t="s">
         <v>3</v>
       </c>
       <c r="C129">
-        <v>127</v>
+        <v>24</v>
       </c>
       <c r="D129">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E129">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="F129">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G129" s="1">
         <v>0</v>
@@ -4401,22 +4404,22 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B130" t="s">
         <v>3</v>
       </c>
       <c r="C130">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D130">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E130">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F130">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G130" s="1">
         <v>0</v>
@@ -4424,22 +4427,22 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>191</v>
+        <v>98</v>
       </c>
       <c r="B131" t="s">
         <v>3</v>
       </c>
       <c r="C131">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="D131">
+        <v>5</v>
+      </c>
+      <c r="E131">
+        <v>24</v>
+      </c>
+      <c r="F131">
         <v>2</v>
-      </c>
-      <c r="E131">
-        <v>13</v>
-      </c>
-      <c r="F131">
-        <v>11</v>
       </c>
       <c r="G131" s="1">
         <v>0</v>
@@ -4447,22 +4450,22 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B132" t="s">
         <v>3</v>
       </c>
       <c r="C132">
-        <v>558</v>
+        <v>158</v>
       </c>
       <c r="D132">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="E132">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F132">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="G132" s="1">
         <v>0</v>
@@ -4470,22 +4473,22 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>99</v>
+        <v>153</v>
       </c>
       <c r="B133" t="s">
         <v>3</v>
       </c>
       <c r="C133">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="D133">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E133">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F133">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G133" s="1">
         <v>0</v>
@@ -4493,22 +4496,22 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B134" t="s">
         <v>3</v>
       </c>
       <c r="C134">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="E134">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="F134">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="G134" s="1">
         <v>0</v>
@@ -4516,10 +4519,10 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B135" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C135">
         <v>0</v>
@@ -4539,22 +4542,22 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B136" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C136">
-        <v>534</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E136">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F136">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="G136" s="1">
         <v>0</v>
@@ -4562,22 +4565,22 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B137" t="s">
         <v>3</v>
       </c>
       <c r="C137">
-        <v>673</v>
+        <v>534</v>
       </c>
       <c r="D137">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E137">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F137">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="G137" s="1">
         <v>0</v>
@@ -4585,22 +4588,22 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B138" t="s">
         <v>3</v>
       </c>
       <c r="C138">
-        <v>60</v>
+        <v>673</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E138">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="G138" s="1">
         <v>0</v>
@@ -4608,22 +4611,22 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B139" t="s">
         <v>3</v>
       </c>
       <c r="C139">
-        <v>265</v>
+        <v>60</v>
       </c>
       <c r="D139">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E139">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="F139">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G139" s="1">
         <v>0</v>
@@ -4631,22 +4634,22 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B140" t="s">
         <v>3</v>
       </c>
       <c r="C140">
-        <v>0</v>
+        <v>265</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E140">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="F140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G140" s="1">
         <v>0</v>
@@ -4654,7 +4657,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B141" t="s">
         <v>3</v>
@@ -4677,7 +4680,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B142" t="s">
         <v>3</v>
@@ -4700,65 +4703,65 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>156</v>
+        <v>108</v>
       </c>
       <c r="B143" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C143">
-        <v>364</v>
+        <v>0</v>
       </c>
       <c r="D143">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E143">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F143">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G143" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="B144" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C144">
-        <v>77</v>
+        <v>364</v>
       </c>
       <c r="D144">
+        <v>12</v>
+      </c>
+      <c r="E144">
+        <v>86</v>
+      </c>
+      <c r="F144">
         <v>2</v>
       </c>
-      <c r="E144">
-        <v>17</v>
-      </c>
-      <c r="F144">
-        <v>0</v>
-      </c>
       <c r="G144" s="1">
-        <v>0</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B145" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C145">
-        <v>299</v>
+        <v>77</v>
       </c>
       <c r="D145">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E145">
-        <v>79</v>
+        <v>17</v>
       </c>
       <c r="F145">
         <v>0</v>
@@ -4769,19 +4772,19 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B146" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C146">
-        <v>26</v>
+        <v>299</v>
       </c>
       <c r="D146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E146">
-        <v>4</v>
+        <v>79</v>
       </c>
       <c r="F146">
         <v>0</v>
@@ -4792,65 +4795,65 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C147">
-        <v>111</v>
+        <v>26</v>
       </c>
       <c r="D147">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E147">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="F147">
         <v>0</v>
       </c>
       <c r="G147" s="1">
-        <v>0.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B148" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C148">
-        <v>40</v>
+        <v>111</v>
       </c>
       <c r="D148">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E148">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="F148">
         <v>0</v>
       </c>
       <c r="G148" s="1">
-        <v>0</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C149">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E149">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F149">
         <v>0</v>
@@ -4861,19 +4864,19 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="B150" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C150">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="D150">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E150">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F150">
         <v>0</v>
@@ -4884,19 +4887,19 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>114</v>
+        <v>137</v>
       </c>
       <c r="B151" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C151">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E151">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F151">
         <v>0</v>
@@ -4907,22 +4910,22 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B152" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C152">
-        <v>301</v>
+        <v>0</v>
       </c>
       <c r="D152">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E152">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F152">
-        <v>27</v>
+        <v>0</v>
       </c>
       <c r="G152" s="1">
         <v>0</v>
@@ -4930,114 +4933,114 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B153" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C153">
-        <v>330</v>
+        <v>301</v>
       </c>
       <c r="D153">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E153">
-        <v>76</v>
+        <v>2</v>
       </c>
       <c r="F153">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="G153" s="1">
-        <v>0.55000000000000004</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B154" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C154">
-        <v>884</v>
+        <v>330</v>
       </c>
       <c r="D154">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E154">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="F154">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="G154" s="1">
-        <v>0.92</v>
+        <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B155" t="s">
         <v>6</v>
       </c>
       <c r="C155">
-        <v>116</v>
+        <v>884</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F155">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G155" s="1">
-        <v>1</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>150</v>
+        <v>118</v>
       </c>
       <c r="B156" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="C156">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D156">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E156">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F156">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G156" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="B157" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C157">
-        <v>310</v>
+        <v>133</v>
       </c>
       <c r="D157">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="E157">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F157">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="G157" s="1">
         <v>0</v>
@@ -5045,91 +5048,91 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>120</v>
+        <v>170</v>
       </c>
       <c r="B158" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="C158">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="D158">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E158">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F158">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G158" s="1">
-        <v>1.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B159" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C159">
-        <v>53</v>
+        <v>205</v>
       </c>
       <c r="D159">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E159">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F159">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G159" s="1">
-        <v>1.08</v>
+        <v>1.03</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B160" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C160">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="D160">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E160">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="F160">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G160" s="1">
-        <v>0</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>171</v>
+        <v>122</v>
       </c>
       <c r="B161" t="s">
         <v>3</v>
       </c>
       <c r="C161">
-        <v>289</v>
+        <v>104</v>
       </c>
       <c r="D161">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E161">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="F161">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G161" s="1">
         <v>0</v>
@@ -5137,22 +5140,22 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>123</v>
+        <v>171</v>
       </c>
       <c r="B162" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C162">
-        <v>23</v>
+        <v>289</v>
       </c>
       <c r="D162">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E162">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F162">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="G162" s="1">
         <v>0</v>
@@ -5160,19 +5163,19 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B163" t="s">
         <v>4</v>
       </c>
       <c r="C163">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D163">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E163">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F163">
         <v>0</v>
@@ -5183,19 +5186,19 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="B164" t="s">
         <v>4</v>
       </c>
       <c r="C164">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="D164">
         <v>2</v>
       </c>
       <c r="E164">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F164">
         <v>0</v>
@@ -5206,22 +5209,22 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="B165" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C165">
-        <v>127</v>
+        <v>32</v>
       </c>
       <c r="D165">
         <v>2</v>
       </c>
       <c r="E165">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F165">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G165" s="1">
         <v>0</v>
@@ -5229,22 +5232,22 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>124</v>
+        <v>149</v>
       </c>
       <c r="B166" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C166">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="D166">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E166">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F166">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G166" s="1">
         <v>0</v>
@@ -5252,88 +5255,88 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B167" t="s">
         <v>6</v>
       </c>
       <c r="C167">
-        <v>387</v>
+        <v>0</v>
       </c>
       <c r="D167">
         <v>0</v>
       </c>
       <c r="E167">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F167">
         <v>0</v>
       </c>
       <c r="G167" s="1">
-        <v>1.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B168" t="s">
         <v>6</v>
       </c>
       <c r="C168">
-        <v>584</v>
+        <v>387</v>
       </c>
       <c r="D168">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="E168">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="F168">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="G168" s="1">
-        <v>0.7</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B169" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C169">
-        <v>38</v>
+        <v>584</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="E169">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="F169">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="G169" s="1">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B170" t="s">
         <v>4</v>
       </c>
       <c r="C170">
-        <v>86</v>
+        <v>38</v>
       </c>
       <c r="D170">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E170">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F170">
         <v>0</v>
@@ -5344,22 +5347,22 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="B171" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C171">
-        <v>371</v>
+        <v>86</v>
       </c>
       <c r="D171">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="E171">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="F171">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G171" s="1">
         <v>0</v>
@@ -5367,22 +5370,22 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="B172" t="s">
         <v>3</v>
       </c>
       <c r="C172">
-        <v>595</v>
+        <v>371</v>
       </c>
       <c r="D172">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="E172">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F172">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="G172" s="1">
         <v>0</v>
@@ -5390,22 +5393,22 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B173" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C173">
-        <v>0</v>
+        <v>595</v>
       </c>
       <c r="D173">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="E173">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F173">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G173" s="1">
         <v>0</v>
@@ -5413,22 +5416,22 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="B174" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C174">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="D174">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E174">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F174">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G174" s="1">
         <v>0</v>
@@ -5436,22 +5439,22 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B175" t="s">
         <v>3</v>
       </c>
       <c r="C175">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="D175">
+        <v>16</v>
+      </c>
+      <c r="E175">
+        <v>2</v>
+      </c>
+      <c r="F175">
         <v>5</v>
-      </c>
-      <c r="E175">
-        <v>13</v>
-      </c>
-      <c r="F175">
-        <v>0</v>
       </c>
       <c r="G175" s="1">
         <v>0</v>
@@ -5459,19 +5462,19 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B176" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C176">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="D176">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E176">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="F176">
         <v>0</v>
@@ -5482,22 +5485,22 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="B177" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C177">
-        <v>307</v>
+        <v>18</v>
       </c>
       <c r="D177">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E177">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="F177">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G177" s="1">
         <v>0</v>
@@ -5505,22 +5508,22 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>132</v>
+        <v>168</v>
       </c>
       <c r="B178" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C178">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="D178">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="E178">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="F178">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G178" s="1">
         <v>0</v>
@@ -5528,19 +5531,19 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B179" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C179">
-        <v>151</v>
+        <v>0</v>
       </c>
       <c r="D179">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E179">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="F179">
         <v>0</v>
@@ -5551,22 +5554,22 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>157</v>
+        <v>133</v>
       </c>
       <c r="B180" t="s">
         <v>3</v>
       </c>
       <c r="C180">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D180">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E180">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="F180">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G180" s="1">
         <v>0</v>
@@ -5574,36 +5577,36 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="B181" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C181">
-        <v>18</v>
+        <v>150</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E181">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F181">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G181" s="1">
-        <v>1.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B182" t="s">
         <v>6</v>
       </c>
       <c r="C182">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -5615,29 +5618,52 @@
         <v>0</v>
       </c>
       <c r="G182" s="1">
-        <v>0</v>
+        <v>1.05</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
+        <v>140</v>
+      </c>
+      <c r="B183" t="s">
+        <v>6</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+      <c r="D183">
+        <v>0</v>
+      </c>
+      <c r="E183">
+        <v>0</v>
+      </c>
+      <c r="F183">
+        <v>0</v>
+      </c>
+      <c r="G183" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
         <v>148</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>21</v>
       </c>
-      <c r="C183">
+      <c r="C184">
         <v>59</v>
       </c>
-      <c r="D183">
+      <c r="D184">
         <v>10</v>
       </c>
-      <c r="E183">
+      <c r="E184">
         <v>4</v>
       </c>
-      <c r="F183">
-        <v>0</v>
-      </c>
-      <c r="G183" s="1">
+      <c r="F184">
+        <v>0</v>
+      </c>
+      <c r="G184" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>